<commit_message>
changes in clan capital
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Documents\GitHub\clashMacacos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39F3FEBA-3DB8-4DB0-96DC-D6E2224365A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F289E908-83D3-4296-AE08-B7CB434EB9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CWL 1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="200">
   <si>
     <t>nome</t>
   </si>
@@ -618,6 +618,27 @@
   </si>
   <si>
     <t>HikariNoRob</t>
+  </si>
+  <si>
+    <t>Robby</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Giosan</t>
+  </si>
+  <si>
+    <t>Omar</t>
+  </si>
+  <si>
+    <t>Staenta</t>
+  </si>
+  <si>
+    <t>Dado</t>
+  </si>
+  <si>
+    <t>Xblade</t>
   </si>
 </sst>
 </file>
@@ -884,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1159,6 +1180,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1621,8 +1645,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella2" displayName="Tabella2" ref="A1:CI51" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87">
   <autoFilter ref="A1:CI51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CI51">
-    <sortCondition descending="1" ref="D1:D51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CI50">
+    <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="87">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NAME" dataDxfId="86"/>
@@ -4050,8 +4074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="Z32" sqref="Z32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28:V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -7025,31 +7049,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>15</v>
       </c>
@@ -7062,8 +7092,11 @@
       <c r="J3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -7079,8 +7112,11 @@
       <c r="J4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -7096,8 +7132,11 @@
       <c r="J5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13</v>
       </c>
@@ -7113,8 +7152,11 @@
       <c r="J6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>13</v>
       </c>
@@ -7127,16 +7169,22 @@
       <c r="J7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13</v>
       </c>
@@ -7149,16 +7197,22 @@
       <c r="J9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13</v>
       </c>
@@ -7171,8 +7225,11 @@
       <c r="J11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -7185,8 +7242,11 @@
       <c r="J12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -7199,8 +7259,11 @@
       <c r="J13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -7213,8 +7276,11 @@
       <c r="J14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -7227,16 +7293,22 @@
       <c r="J15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -7249,8 +7321,11 @@
       <c r="J17" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -7263,8 +7338,11 @@
       <c r="J18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -7277,16 +7355,22 @@
       <c r="J19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -7294,7 +7378,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -7302,7 +7386,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>12</v>
       </c>
@@ -7310,7 +7394,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -7318,7 +7402,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12</v>
       </c>
@@ -7326,7 +7410,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
@@ -7334,7 +7418,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12</v>
       </c>
@@ -7342,7 +7426,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>12</v>
       </c>
@@ -7350,7 +7434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12</v>
       </c>
@@ -7367,8 +7451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CI50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7665,144 +7749,116 @@
     </row>
     <row r="2" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
-        <v>159</v>
+        <v>60</v>
       </c>
       <c r="B2" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="68">
-        <f t="shared" ref="E2:E11" si="0">SUM(G2:L2)</f>
-        <v>12</v>
+        <f>SUM(G2:M2)</f>
+        <v>3</v>
       </c>
       <c r="F2" s="84">
-        <f t="shared" ref="F2:F18" si="1">ROUND(AVERAGE(G2:L2),1)</f>
-        <v>3</v>
-      </c>
-      <c r="G2" s="83" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" s="84" t="s">
-        <v>158</v>
+        <f>ROUND(AVERAGE(G2:L2),1)</f>
+        <v>1.5</v>
       </c>
       <c r="I2" s="83">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" s="84">
-        <v>3</v>
-      </c>
-      <c r="K2" s="83">
-        <v>3</v>
-      </c>
-      <c r="L2" s="84">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B3" s="83">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" s="84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="83">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="68">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F3" s="84">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G3" s="83">
-        <v>1</v>
-      </c>
-      <c r="H3" s="84" t="s">
-        <v>158</v>
-      </c>
-      <c r="I3" s="83">
-        <v>1</v>
-      </c>
-      <c r="J3" s="84" t="s">
-        <v>158</v>
-      </c>
-      <c r="K3" s="68" t="s">
-        <v>158</v>
-      </c>
-      <c r="L3" s="68" t="s">
-        <v>158</v>
-      </c>
+        <f>SUM(G3:M3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="84" t="e">
+        <f>ROUND(AVERAGE(G3:L3),1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
     </row>
     <row r="4" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B4" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="83">
         <v>3</v>
       </c>
       <c r="E4" s="68">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUM(G4:L4)</f>
+        <v>6</v>
       </c>
       <c r="F4" s="84">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <f>ROUND(AVERAGE(G4:L4),1)</f>
+        <v>1</v>
       </c>
       <c r="G4" s="83">
         <v>2</v>
       </c>
       <c r="H4" s="84">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4" s="84">
-        <v>3</v>
-      </c>
-      <c r="K4" s="83" t="s">
-        <v>158</v>
-      </c>
-      <c r="L4" s="84" t="s">
-        <v>158</v>
+        <v>0</v>
+      </c>
+      <c r="K4" s="83">
+        <v>2</v>
+      </c>
+      <c r="L4" s="84">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="83">
+        <v>0</v>
+      </c>
+      <c r="C5" s="84">
+        <v>0</v>
+      </c>
+      <c r="D5" s="83">
+        <v>1</v>
+      </c>
+      <c r="E5" s="68">
+        <f>SUM(G6:M6)</f>
         <v>6</v>
       </c>
-      <c r="B5" s="83">
-        <v>0</v>
-      </c>
-      <c r="C5" s="84">
-        <v>0</v>
-      </c>
-      <c r="D5" s="83">
-        <v>3</v>
-      </c>
-      <c r="E5" s="68">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
       <c r="F5" s="84">
-        <f t="shared" si="1"/>
-        <v>2.7</v>
+        <f>ROUND(AVERAGE(G5:L5),1)</f>
+        <v>3</v>
       </c>
       <c r="G5" s="83">
         <v>3</v>
@@ -7810,22 +7866,12 @@
       <c r="H5" s="84">
         <v>3</v>
       </c>
-      <c r="I5" s="83">
-        <v>3</v>
-      </c>
-      <c r="J5" s="84">
-        <v>2</v>
-      </c>
-      <c r="K5" s="68">
-        <v>2</v>
-      </c>
-      <c r="L5" s="68">
-        <v>3</v>
-      </c>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
     </row>
     <row r="6" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="B6" s="83">
         <v>0</v>
@@ -7834,26 +7880,14 @@
         <v>0</v>
       </c>
       <c r="D6" s="83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="68">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>SUM(G6:L6)</f>
+        <v>6</v>
       </c>
       <c r="F6" s="84">
-        <f t="shared" si="1"/>
-        <v>2.8</v>
-      </c>
-      <c r="G6" s="83">
-        <v>3</v>
-      </c>
-      <c r="H6" s="84">
-        <v>3</v>
-      </c>
-      <c r="I6" s="83">
-        <v>2</v>
-      </c>
-      <c r="J6" s="84">
+        <f>ROUND(AVERAGE(G6:L6),1)</f>
         <v>3</v>
       </c>
       <c r="K6" s="83">
@@ -7865,7 +7899,7 @@
     </row>
     <row r="7" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="B7" s="83">
         <v>0</v>
@@ -7874,38 +7908,20 @@
         <v>0</v>
       </c>
       <c r="D7" s="83">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E7" s="68">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F7" s="84">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G7" s="83">
-        <v>2</v>
-      </c>
-      <c r="H7" s="84">
-        <v>3</v>
-      </c>
-      <c r="I7" s="83">
-        <v>1</v>
-      </c>
-      <c r="J7" s="84">
-        <v>1</v>
-      </c>
-      <c r="K7" s="83">
-        <v>3</v>
-      </c>
-      <c r="L7" s="84">
-        <v>2</v>
+        <f>SUM(G7:M7)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="84" t="e">
+        <f>ROUND(AVERAGE(G7:L7),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="B8" s="83">
         <v>0</v>
@@ -7914,38 +7930,22 @@
         <v>0</v>
       </c>
       <c r="D8" s="83">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8" s="68">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="F8" s="84">
-        <f t="shared" si="1"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G8" s="83">
-        <v>1</v>
-      </c>
-      <c r="H8" s="84">
-        <v>3</v>
-      </c>
-      <c r="I8" s="83">
-        <v>3</v>
-      </c>
-      <c r="J8" s="84">
-        <v>3</v>
-      </c>
-      <c r="K8" s="68">
-        <v>1</v>
-      </c>
-      <c r="L8" s="68">
-        <v>3</v>
-      </c>
+        <f>SUM(G8:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="84" t="e">
+        <f>ROUND(AVERAGE(G8:L8),1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
     </row>
     <row r="9" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="B9" s="83">
         <v>0</v>
@@ -7954,72 +7954,42 @@
         <v>0</v>
       </c>
       <c r="D9" s="83">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E9" s="68">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F9" s="84">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G9" s="83">
-        <v>2</v>
-      </c>
-      <c r="H9" s="84">
-        <v>1</v>
-      </c>
-      <c r="I9" s="83">
-        <v>0</v>
-      </c>
-      <c r="J9" s="84">
-        <v>0</v>
-      </c>
-      <c r="K9" s="83">
-        <v>2</v>
-      </c>
-      <c r="L9" s="84">
-        <v>1</v>
+        <f>SUM(G9:M9)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="84" t="e">
+        <f>ROUND(AVERAGE(G9:L9),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B10" s="83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="68">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F10" s="84">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I10" s="83" t="s">
-        <v>158</v>
-      </c>
-      <c r="J10" s="84" t="s">
-        <v>158</v>
-      </c>
-      <c r="K10" s="83">
-        <v>3</v>
-      </c>
-      <c r="L10" s="84">
-        <v>3</v>
+        <f>SUM(G10:M10)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="84" t="e">
+        <f>ROUND(AVERAGE(G10:L10),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
-        <v>174</v>
+        <v>6</v>
       </c>
       <c r="B11" s="83">
         <v>0</v>
@@ -8028,24 +7998,30 @@
         <v>0</v>
       </c>
       <c r="D11" s="83">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="68">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUM(G11:L11)</f>
+        <v>16</v>
       </c>
       <c r="F11" s="84">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <f>ROUND(AVERAGE(G11:L11),1)</f>
+        <v>2.7</v>
+      </c>
+      <c r="G11" s="83">
+        <v>3</v>
+      </c>
+      <c r="H11" s="84">
+        <v>3</v>
       </c>
       <c r="I11" s="83">
         <v>3</v>
       </c>
       <c r="J11" s="84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" s="68">
         <v>3</v>
@@ -8053,7 +8029,7 @@
     </row>
     <row r="12" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="B12" s="83">
         <v>0</v>
@@ -8062,32 +8038,26 @@
         <v>0</v>
       </c>
       <c r="D12" s="83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="68">
-        <f>SUM(G13:M13)</f>
-        <v>10</v>
+        <f>SUM(G12:M12)</f>
+        <v>4</v>
       </c>
       <c r="F12" s="84">
-        <f t="shared" si="1"/>
-        <v>2.8</v>
-      </c>
-      <c r="G12" s="83">
-        <v>3</v>
-      </c>
-      <c r="H12" s="84">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G12:L12),1)</f>
+        <v>2</v>
       </c>
       <c r="I12" s="83">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J12" s="84">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
-        <v>58</v>
+        <v>171</v>
       </c>
       <c r="B13" s="83">
         <v>0</v>
@@ -8096,66 +8066,48 @@
         <v>0</v>
       </c>
       <c r="D13" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E13" s="68">
-        <f>SUM(G14:M14)</f>
-        <v>7</v>
-      </c>
-      <c r="F13" s="84">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="G13" s="83">
-        <v>3</v>
-      </c>
-      <c r="H13" s="84">
-        <v>1</v>
-      </c>
-      <c r="I13" s="83">
-        <v>3</v>
-      </c>
-      <c r="J13" s="84">
-        <v>3</v>
+        <f>SUM(G13:M13)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="84" t="e">
+        <f>ROUND(AVERAGE(G13:L13),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
-        <v>59</v>
+        <v>161</v>
       </c>
       <c r="B14" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="84">
         <v>0</v>
       </c>
       <c r="D14" s="83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="68">
-        <f>SUM(G15:M15)</f>
-        <v>9</v>
+        <f>SUM(G14:M14)</f>
+        <v>2</v>
       </c>
       <c r="F14" s="84">
-        <f t="shared" si="1"/>
-        <v>1.8</v>
-      </c>
-      <c r="G14" s="83">
-        <v>1</v>
-      </c>
-      <c r="H14" s="84">
+        <f>ROUND(AVERAGE(G14:L14),1)</f>
         <v>2</v>
       </c>
       <c r="I14" s="83">
-        <v>1</v>
-      </c>
-      <c r="J14" s="84">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="J14" s="84" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="B15" s="83">
         <v>0</v>
@@ -8164,32 +8116,20 @@
         <v>0</v>
       </c>
       <c r="D15" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E15" s="68">
-        <f>SUM(G16:M16)</f>
-        <v>10</v>
-      </c>
-      <c r="F15" s="84">
-        <f t="shared" si="1"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G15" s="83">
-        <v>1</v>
-      </c>
-      <c r="H15" s="84">
-        <v>2</v>
-      </c>
-      <c r="I15" s="83">
-        <v>3</v>
-      </c>
-      <c r="J15" s="84">
-        <v>3</v>
+        <f>SUM(G15:M15)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="84" t="e">
+        <f>ROUND(AVERAGE(G15:L15),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A16" s="79" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="B16" s="83">
         <v>0</v>
@@ -8198,202 +8138,202 @@
         <v>0</v>
       </c>
       <c r="D16" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16" s="68">
-        <f>SUM(G16:L16)</f>
-        <v>10</v>
-      </c>
-      <c r="F16" s="84">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="G16" s="83">
-        <v>3</v>
-      </c>
-      <c r="H16" s="84">
-        <v>3</v>
-      </c>
-      <c r="K16" s="83">
-        <v>2</v>
-      </c>
-      <c r="L16" s="84">
-        <v>2</v>
+        <f>SUM(G16:M16)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="84" t="e">
+        <f>ROUND(AVERAGE(G16:L16),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="79" t="s">
-        <v>179</v>
+        <v>59</v>
       </c>
       <c r="B17" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17" s="84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="68">
-        <f>SUM(G17:L17)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="84" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="83" t="s">
-        <v>158</v>
-      </c>
-      <c r="L17" s="84" t="s">
-        <v>158</v>
+        <f>SUM(G18:M18)</f>
+        <v>10</v>
+      </c>
+      <c r="F17" s="84">
+        <f>ROUND(AVERAGE(G17:L17),1)</f>
+        <v>1.8</v>
+      </c>
+      <c r="G17" s="83">
+        <v>1</v>
+      </c>
+      <c r="H17" s="84">
+        <v>2</v>
+      </c>
+      <c r="I17" s="83">
+        <v>1</v>
+      </c>
+      <c r="J17" s="84">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="79" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B18" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18" s="84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="68">
         <f>SUM(G18:L18)</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="84" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="83" t="s">
-        <v>158</v>
-      </c>
-      <c r="L18" s="84" t="s">
-        <v>158</v>
+        <v>10</v>
+      </c>
+      <c r="F18" s="84">
+        <f>ROUND(AVERAGE(G18:L18),1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I18" s="83">
+        <v>3</v>
+      </c>
+      <c r="J18" s="84">
+        <v>1</v>
+      </c>
+      <c r="K18" s="83">
+        <v>3</v>
+      </c>
+      <c r="L18" s="84">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="79" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="B19" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19" s="84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="68">
-        <f>SUM(G19:M19)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="84" t="e">
-        <f>AVERAGE(G19:M19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="83" t="s">
-        <v>158</v>
-      </c>
-      <c r="J19" s="84" t="s">
-        <v>158</v>
+        <f>SUM(G19:L19)</f>
+        <v>10</v>
+      </c>
+      <c r="F19" s="84">
+        <f>ROUND(AVERAGE(G19:L19),1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G19" s="83">
+        <v>3</v>
+      </c>
+      <c r="H19" s="84">
+        <v>3</v>
+      </c>
+      <c r="K19" s="83">
+        <v>2</v>
+      </c>
+      <c r="L19" s="84">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="79" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B20" s="83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C20" s="84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="68">
         <f>SUM(G20:M20)</f>
         <v>0</v>
       </c>
       <c r="F20" s="84" t="e">
-        <f t="shared" ref="F20:F50" si="2">ROUND(AVERAGE(G20:L20),1)</f>
+        <f>ROUND(AVERAGE(G20:L20),1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="83" t="s">
-        <v>158</v>
-      </c>
-      <c r="H20" s="84" t="s">
-        <v>158</v>
-      </c>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="94"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="79" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="B21" s="83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="84">
         <v>0</v>
       </c>
       <c r="D21" s="83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="68">
-        <f>SUM(G21:M21)</f>
-        <v>2</v>
+        <f>SUM(G22:M22)</f>
+        <v>0</v>
       </c>
       <c r="F21" s="84">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G21:L21),1)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G21" s="83">
+        <v>1</v>
+      </c>
+      <c r="H21" s="84">
         <v>2</v>
       </c>
       <c r="I21" s="83">
-        <v>2</v>
-      </c>
-      <c r="J21" s="84" t="s">
-        <v>158</v>
+        <v>3</v>
+      </c>
+      <c r="J21" s="84">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="79" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B22" s="83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="84">
         <v>0</v>
       </c>
       <c r="D22" s="83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="68">
         <f>SUM(G22:M22)</f>
-        <v>2</v>
-      </c>
-      <c r="F22" s="84">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I22" s="83">
-        <v>2</v>
-      </c>
-      <c r="J22" s="84" t="s">
-        <v>158</v>
+        <v>0</v>
+      </c>
+      <c r="F22" s="84" t="e">
+        <f>ROUND(AVERAGE(G22:L22),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="79" t="s">
-        <v>60</v>
+        <v>176</v>
       </c>
       <c r="B23" s="83">
         <v>0</v>
@@ -8402,26 +8342,20 @@
         <v>0</v>
       </c>
       <c r="D23" s="83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="68">
         <f>SUM(G23:M23)</f>
-        <v>3</v>
-      </c>
-      <c r="F23" s="84">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
-      </c>
-      <c r="I23" s="83">
-        <v>2</v>
-      </c>
-      <c r="J23" s="84">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F23" s="84" t="e">
+        <f>ROUND(AVERAGE(G23:L23),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="79" t="s">
-        <v>165</v>
+        <v>13</v>
       </c>
       <c r="B24" s="83">
         <v>0</v>
@@ -8430,57 +8364,51 @@
         <v>0</v>
       </c>
       <c r="D24" s="83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="68">
-        <f>SUM(G24:L24)</f>
-        <v>6</v>
-      </c>
-      <c r="F24" s="84">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="K24" s="83">
-        <v>3</v>
-      </c>
-      <c r="L24" s="84">
-        <v>3</v>
+        <f>SUM(G24:M24)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="84" t="e">
+        <f>ROUND(AVERAGE(G24:L24),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="79" t="s">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="B25" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C25" s="84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="83">
         <v>1</v>
       </c>
       <c r="E25" s="68">
         <f>SUM(G25:M25)</f>
-        <v>4</v>
-      </c>
-      <c r="F25" s="84">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I25" s="83">
-        <v>3</v>
-      </c>
-      <c r="J25" s="84">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F25" s="84" t="e">
+        <f>AVERAGE(G25:M25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="J25" s="84" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="79" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="B26" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="84">
         <v>0</v>
@@ -8490,22 +8418,22 @@
       </c>
       <c r="E26" s="68">
         <f>SUM(G26:M26)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F26" s="84">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f>ROUND(AVERAGE(G26:L26),1)</f>
+        <v>2</v>
       </c>
       <c r="I26" s="83">
-        <v>3</v>
-      </c>
-      <c r="J26" s="84">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="J26" s="84" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="79" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="B27" s="83">
         <v>0</v>
@@ -8514,54 +8442,60 @@
         <v>0</v>
       </c>
       <c r="D27" s="83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="68">
-        <f>SUM(G27:L27)</f>
-        <v>2</v>
-      </c>
-      <c r="F27" s="84">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K27" s="83">
-        <v>1</v>
-      </c>
-      <c r="L27" s="84">
-        <v>1</v>
+        <f>SUM(G27:M27)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="84" t="e">
+        <f>ROUND(AVERAGE(G27:L27),1)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="79" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="B28" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C28" s="84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="83">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E28" s="68">
-        <f>SUM(G29:M29)</f>
-        <v>0</v>
+        <f>SUM(G28:L28)</f>
+        <v>12</v>
       </c>
       <c r="F28" s="84">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="G28" s="83">
-        <v>3</v>
-      </c>
-      <c r="H28" s="84">
+        <f>ROUND(AVERAGE(G28:L28),1)</f>
+        <v>3</v>
+      </c>
+      <c r="G28" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="H28" s="84" t="s">
+        <v>158</v>
+      </c>
+      <c r="I28" s="83">
+        <v>3</v>
+      </c>
+      <c r="J28" s="84">
+        <v>3</v>
+      </c>
+      <c r="K28" s="83">
+        <v>3</v>
+      </c>
+      <c r="L28" s="84">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="79" t="s">
-        <v>164</v>
+        <v>58</v>
       </c>
       <c r="B29" s="83">
         <v>0</v>
@@ -8570,20 +8504,32 @@
         <v>0</v>
       </c>
       <c r="D29" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E29" s="68">
-        <f t="shared" ref="E29:E50" si="3">SUM(G29:M29)</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f>SUM(G30:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="84">
+        <f>ROUND(AVERAGE(G29:L29),1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G29" s="83">
+        <v>3</v>
+      </c>
+      <c r="H29" s="84">
+        <v>1</v>
+      </c>
+      <c r="I29" s="83">
+        <v>3</v>
+      </c>
+      <c r="J29" s="84">
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="79" t="s">
-        <v>166</v>
+        <v>41</v>
       </c>
       <c r="B30" s="83">
         <v>0</v>
@@ -8595,11 +8541,11 @@
         <v>0</v>
       </c>
       <c r="E30" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G30:M30)</f>
         <v>0</v>
       </c>
       <c r="F30" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G30:L30),1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K30" s="68"/>
@@ -8607,7 +8553,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="79" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B31" s="83">
         <v>0</v>
@@ -8619,17 +8565,17 @@
         <v>0</v>
       </c>
       <c r="E31" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G31:M31)</f>
         <v>0</v>
       </c>
       <c r="F31" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G31:L31),1)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="79" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="B32" s="83">
         <v>0</v>
@@ -8641,17 +8587,17 @@
         <v>0</v>
       </c>
       <c r="E32" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G32:M32)</f>
         <v>0</v>
       </c>
       <c r="F32" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G32:L32),1)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="79" t="s">
-        <v>169</v>
+        <v>10</v>
       </c>
       <c r="B33" s="83">
         <v>0</v>
@@ -8660,20 +8606,38 @@
         <v>0</v>
       </c>
       <c r="D33" s="83">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E33" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f>SUM(G33:L33)</f>
+        <v>17</v>
+      </c>
+      <c r="F33" s="84">
+        <f>ROUND(AVERAGE(G33:L33),1)</f>
+        <v>2.8</v>
+      </c>
+      <c r="G33" s="83">
+        <v>3</v>
+      </c>
+      <c r="H33" s="84">
+        <v>3</v>
+      </c>
+      <c r="I33" s="83">
+        <v>2</v>
+      </c>
+      <c r="J33" s="84">
+        <v>3</v>
+      </c>
+      <c r="K33" s="83">
+        <v>3</v>
+      </c>
+      <c r="L33" s="84">
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="79" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="B34" s="83">
         <v>0</v>
@@ -8682,66 +8646,90 @@
         <v>0</v>
       </c>
       <c r="D34" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K34" s="68"/>
-      <c r="L34" s="68"/>
+        <f>SUM(G34:M34)</f>
+        <v>6</v>
+      </c>
+      <c r="F34" s="84">
+        <f>ROUND(AVERAGE(G34:L34),1)</f>
+        <v>3</v>
+      </c>
+      <c r="I34" s="83">
+        <v>3</v>
+      </c>
+      <c r="J34" s="84">
+        <v>3</v>
+      </c>
+      <c r="K34" s="94"/>
+      <c r="L34" s="94"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="79" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B35" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C35" s="84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G35:L35)</f>
         <v>0</v>
       </c>
       <c r="F35" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G35:L35),1)</f>
         <v>#DIV/0!</v>
+      </c>
+      <c r="K35" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="L35" s="84" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="79" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B36" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E36" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f>SUM(G36:L36)</f>
+        <v>6</v>
+      </c>
+      <c r="F36" s="84">
+        <f>ROUND(AVERAGE(G36:L36),1)</f>
+        <v>3</v>
+      </c>
+      <c r="I36" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="J36" s="84" t="s">
+        <v>158</v>
+      </c>
+      <c r="K36" s="83">
+        <v>3</v>
+      </c>
+      <c r="L36" s="84">
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="79" t="s">
-        <v>16</v>
+        <v>180</v>
       </c>
       <c r="B37" s="83">
         <v>0</v>
@@ -8753,17 +8741,17 @@
         <v>0</v>
       </c>
       <c r="E37" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G37:M37)</f>
         <v>0</v>
       </c>
       <c r="F37" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G37:L37),1)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="79" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B38" s="83">
         <v>0</v>
@@ -8775,19 +8763,19 @@
         <v>0</v>
       </c>
       <c r="E38" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G38:M38)</f>
         <v>0</v>
       </c>
       <c r="F38" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G38:L38),1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
+      <c r="K38" s="94"/>
+      <c r="L38" s="94"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="79" t="s">
-        <v>176</v>
+        <v>22</v>
       </c>
       <c r="B39" s="83">
         <v>0</v>
@@ -8796,20 +8784,38 @@
         <v>0</v>
       </c>
       <c r="D39" s="83">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E39" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F39" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f>SUM(G39:L39)</f>
+        <v>14</v>
+      </c>
+      <c r="F39" s="84">
+        <f>ROUND(AVERAGE(G39:L39),1)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G39" s="83">
+        <v>1</v>
+      </c>
+      <c r="H39" s="84">
+        <v>3</v>
+      </c>
+      <c r="I39" s="83">
+        <v>3</v>
+      </c>
+      <c r="J39" s="84">
+        <v>3</v>
+      </c>
+      <c r="K39" s="83">
+        <v>1</v>
+      </c>
+      <c r="L39" s="84">
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="79" t="s">
-        <v>13</v>
+        <v>182</v>
       </c>
       <c r="B40" s="83">
         <v>0</v>
@@ -8821,11 +8827,11 @@
         <v>0</v>
       </c>
       <c r="E40" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G40:M40)</f>
         <v>0</v>
       </c>
       <c r="F40" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G40:L40),1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K40" s="68"/>
@@ -8833,31 +8839,47 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="79" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="B41" s="83">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C41" s="84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="83">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E41" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F41" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K41" s="68"/>
-      <c r="L41" s="68"/>
+        <f>SUM(G41:L41)</f>
+        <v>2</v>
+      </c>
+      <c r="F41" s="84">
+        <f>ROUND(AVERAGE(G41:L41),1)</f>
+        <v>1</v>
+      </c>
+      <c r="G41" s="83">
+        <v>1</v>
+      </c>
+      <c r="H41" s="84" t="s">
+        <v>158</v>
+      </c>
+      <c r="I41" s="83">
+        <v>1</v>
+      </c>
+      <c r="J41" s="84" t="s">
+        <v>158</v>
+      </c>
+      <c r="K41" s="68" t="s">
+        <v>158</v>
+      </c>
+      <c r="L41" s="68" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="79" t="s">
-        <v>41</v>
+        <v>188</v>
       </c>
       <c r="B42" s="83">
         <v>0</v>
@@ -8866,22 +8888,34 @@
         <v>0</v>
       </c>
       <c r="D42" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E42" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F42" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K42" s="68"/>
-      <c r="L42" s="68"/>
+        <f>SUM(G43:M43)</f>
+        <v>2</v>
+      </c>
+      <c r="F42" s="84">
+        <f>ROUND(AVERAGE(G42:L42),1)</f>
+        <v>2.8</v>
+      </c>
+      <c r="G42" s="83">
+        <v>3</v>
+      </c>
+      <c r="H42" s="84">
+        <v>3</v>
+      </c>
+      <c r="I42" s="83">
+        <v>2</v>
+      </c>
+      <c r="J42" s="84">
+        <v>3</v>
+      </c>
+      <c r="K42" s="94"/>
+      <c r="L42" s="94"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="79" t="s">
-        <v>177</v>
+        <v>47</v>
       </c>
       <c r="B43" s="83">
         <v>0</v>
@@ -8890,20 +8924,26 @@
         <v>0</v>
       </c>
       <c r="D43" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f>SUM(G43:L43)</f>
+        <v>2</v>
+      </c>
+      <c r="F43" s="84">
+        <f>ROUND(AVERAGE(G43:L43),1)</f>
+        <v>1</v>
+      </c>
+      <c r="K43" s="83">
+        <v>1</v>
+      </c>
+      <c r="L43" s="84">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="79" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B44" s="83">
         <v>0</v>
@@ -8912,22 +8952,38 @@
         <v>0</v>
       </c>
       <c r="D44" s="83">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E44" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F44" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K44" s="68"/>
-      <c r="L44" s="68"/>
+        <f>SUM(G44:L44)</f>
+        <v>12</v>
+      </c>
+      <c r="F44" s="84">
+        <f>ROUND(AVERAGE(G44:L44),1)</f>
+        <v>2</v>
+      </c>
+      <c r="G44" s="83">
+        <v>2</v>
+      </c>
+      <c r="H44" s="84">
+        <v>3</v>
+      </c>
+      <c r="I44" s="83">
+        <v>1</v>
+      </c>
+      <c r="J44" s="84">
+        <v>1</v>
+      </c>
+      <c r="K44" s="94">
+        <v>3</v>
+      </c>
+      <c r="L44" s="94">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="79" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B45" s="83">
         <v>0</v>
@@ -8939,11 +8995,11 @@
         <v>0</v>
       </c>
       <c r="E45" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G45:M45)</f>
         <v>0</v>
       </c>
       <c r="F45" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G45:L45),1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K45" s="68"/>
@@ -8951,7 +9007,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="79" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B46" s="83">
         <v>0</v>
@@ -8963,17 +9019,17 @@
         <v>0</v>
       </c>
       <c r="E46" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G46:M46)</f>
         <v>0</v>
       </c>
       <c r="F46" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G46:L46),1)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="79" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B47" s="83">
         <v>0</v>
@@ -8985,82 +9041,110 @@
         <v>0</v>
       </c>
       <c r="E47" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G47:M47)</f>
         <v>0</v>
       </c>
       <c r="F47" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G47:L47),1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K47" s="68"/>
-      <c r="L47" s="68"/>
+      <c r="K47" s="94"/>
+      <c r="L47" s="94"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="79" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B48" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C48" s="84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="68">
-        <f t="shared" si="3"/>
+        <f>SUM(G48:L48)</f>
         <v>0</v>
       </c>
       <c r="F48" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>ROUND(AVERAGE(G48:L48),1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K48" s="68"/>
-      <c r="L48" s="68"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K48" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="L48" s="94" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="79" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B49" s="83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C49" s="84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="83">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E49" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="84" t="e">
-        <f t="shared" si="2"/>
+        <f>SUM(G49:L49)</f>
+        <v>10</v>
+      </c>
+      <c r="F49" s="84">
+        <f>ROUND(AVERAGE(G49:L49),1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G49" s="83">
+        <v>2</v>
+      </c>
+      <c r="H49" s="84">
+        <v>3</v>
+      </c>
+      <c r="I49" s="83">
+        <v>2</v>
+      </c>
+      <c r="J49" s="84">
+        <v>3</v>
+      </c>
+      <c r="K49" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="L49" s="84" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="83">
+        <v>2</v>
+      </c>
+      <c r="C50" s="84">
+        <v>1</v>
+      </c>
+      <c r="D50" s="83">
+        <v>1</v>
+      </c>
+      <c r="E50" s="68">
+        <f>SUM(G50:M50)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="84" t="e">
+        <f>ROUND(AVERAGE(G50:L50),1)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="79" t="s">
-        <v>185</v>
-      </c>
-      <c r="B50" s="83">
-        <v>0</v>
-      </c>
-      <c r="C50" s="84">
-        <v>0</v>
-      </c>
-      <c r="D50" s="83">
-        <v>0</v>
-      </c>
-      <c r="E50" s="68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F50" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G50" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="H50" s="84" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update WAR data - 2026-01-19
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -9768,7 +9768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI48"/>
+  <dimension ref="A1:CI49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A57" sqref="A57"/>
@@ -9932,12 +9932,12 @@
       </c>
       <c r="Y1" s="107" t="inlineStr">
         <is>
-          <t>Colonna25</t>
+          <t>WAR-10 (1)</t>
         </is>
       </c>
       <c r="Z1" s="108" t="inlineStr">
         <is>
-          <t>Colonna26</t>
+          <t>WAR-10 (2)</t>
         </is>
       </c>
       <c r="AA1" s="107" t="inlineStr">
@@ -10262,11 +10262,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="122">
-        <f>SUM(G2:X2)</f>
+        <f>SUM(G2:Z2)</f>
         <v/>
       </c>
       <c r="F2" s="122">
-        <f>ROUND(AVERAGE(G2:X2),1)</f>
+        <f>ROUND(AVERAGE(G2:Z2),1)</f>
         <v/>
       </c>
       <c r="G2" s="121" t="n"/>
@@ -10382,14 +10382,14 @@
         <v>0</v>
       </c>
       <c r="D3" s="123" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="124">
-        <f>SUM(G3:X3)</f>
+        <f>SUM(G3:Z3)</f>
         <v/>
       </c>
       <c r="F3" s="124">
-        <f>ROUND(AVERAGE(G3:X3),1)</f>
+        <f>ROUND(AVERAGE(G3:Z3),1)</f>
         <v/>
       </c>
       <c r="G3" s="125" t="n"/>
@@ -10420,8 +10420,12 @@
       </c>
       <c r="W3" s="125" t="n"/>
       <c r="X3" s="124" t="n"/>
-      <c r="Y3" s="125" t="n"/>
-      <c r="Z3" s="124" t="n"/>
+      <c r="Y3" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="124" t="n">
+        <v>0</v>
+      </c>
       <c r="AA3" s="125" t="n"/>
       <c r="AB3" s="124" t="n"/>
       <c r="AC3" s="123" t="n"/>
@@ -10497,14 +10501,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="128" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="129">
-        <f>SUM(G4:X4)</f>
+        <f>SUM(G4:Z4)</f>
         <v/>
       </c>
       <c r="F4" s="129">
-        <f>ROUND(AVERAGE(G4:X4),1)</f>
+        <f>ROUND(AVERAGE(G4:Z4),1)</f>
         <v/>
       </c>
       <c r="G4" s="128" t="n">
@@ -10557,8 +10561,12 @@
       <c r="X4" s="129" t="n">
         <v>3</v>
       </c>
-      <c r="Y4" s="128" t="n"/>
-      <c r="Z4" s="129" t="n"/>
+      <c r="Y4" s="128" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="129" t="n">
+        <v>1</v>
+      </c>
       <c r="AA4" s="128" t="n"/>
       <c r="AB4" s="129" t="n"/>
       <c r="AC4" s="128" t="n"/>
@@ -10634,14 +10642,14 @@
         <v>0</v>
       </c>
       <c r="D5" s="123" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="124">
-        <f>SUM(G5:X5)</f>
+        <f>SUM(G5:Z5)</f>
         <v/>
       </c>
       <c r="F5" s="124">
-        <f>ROUND(AVERAGE(G5:X5),1)</f>
+        <f>ROUND(AVERAGE(G5:Z5),1)</f>
         <v/>
       </c>
       <c r="G5" s="125" t="n"/>
@@ -10670,8 +10678,12 @@
       <c r="X5" s="124" t="n">
         <v>2</v>
       </c>
-      <c r="Y5" s="125" t="n"/>
-      <c r="Z5" s="124" t="n"/>
+      <c r="Y5" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="124" t="n">
+        <v>3</v>
+      </c>
       <c r="AA5" s="125" t="n"/>
       <c r="AB5" s="124" t="n"/>
       <c r="AC5" s="123" t="n"/>
@@ -10750,11 +10762,11 @@
         <v>5</v>
       </c>
       <c r="E6" s="129">
-        <f>SUM(G6:X6)</f>
+        <f>SUM(G6:Z6)</f>
         <v/>
       </c>
       <c r="F6" s="129">
-        <f>ROUND(AVERAGE(G6:X6),1)</f>
+        <f>ROUND(AVERAGE(G6:Z6),1)</f>
         <v/>
       </c>
       <c r="G6" s="128" t="n">
@@ -10876,14 +10888,14 @@
         <v>1</v>
       </c>
       <c r="D7" s="123" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="124">
-        <f>SUM(G7:X7)</f>
+        <f>SUM(G7:Z7)</f>
         <v/>
       </c>
       <c r="F7" s="124">
-        <f>ROUND(AVERAGE(G7:X7),1)</f>
+        <f>ROUND(AVERAGE(G7:Z7),1)</f>
         <v/>
       </c>
       <c r="G7" s="123" t="n">
@@ -10936,8 +10948,12 @@
       <c r="X7" s="124" t="n">
         <v>3</v>
       </c>
-      <c r="Y7" s="125" t="n"/>
-      <c r="Z7" s="124" t="n"/>
+      <c r="Y7" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="124" t="n">
+        <v>3</v>
+      </c>
       <c r="AA7" s="125" t="n"/>
       <c r="AB7" s="124" t="n"/>
       <c r="AC7" s="123" t="n"/>
@@ -11016,11 +11032,11 @@
         <v>8</v>
       </c>
       <c r="E8" s="129">
-        <f>SUM(G8:X8)</f>
+        <f>SUM(G8:Z8)</f>
         <v/>
       </c>
       <c r="F8" s="129">
-        <f>ROUND(AVERAGE(G8:X8),1)</f>
+        <f>ROUND(AVERAGE(G8:Z8),1)</f>
         <v/>
       </c>
       <c r="G8" s="128" t="n">
@@ -11150,14 +11166,14 @@
         <v>1</v>
       </c>
       <c r="D9" s="123" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="124">
-        <f>SUM(G9:X9)</f>
+        <f>SUM(G9:Z9)</f>
         <v/>
       </c>
       <c r="F9" s="124">
-        <f>ROUND(AVERAGE(G9:X9),1)</f>
+        <f>ROUND(AVERAGE(G9:Z9),1)</f>
         <v/>
       </c>
       <c r="G9" s="125" t="n"/>
@@ -11194,8 +11210,12 @@
       <c r="X9" s="124" t="n">
         <v>3</v>
       </c>
-      <c r="Y9" s="125" t="n"/>
-      <c r="Z9" s="124" t="n"/>
+      <c r="Y9" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z9" s="124" t="n">
+        <v>3</v>
+      </c>
       <c r="AA9" s="125" t="n"/>
       <c r="AB9" s="124" t="n"/>
       <c r="AC9" s="123" t="n"/>
@@ -11271,14 +11291,14 @@
         <v>0</v>
       </c>
       <c r="D10" s="128" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" s="129">
-        <f>SUM(G10:X10)</f>
+        <f>SUM(G10:Z10)</f>
         <v/>
       </c>
       <c r="F10" s="129">
-        <f>ROUND(AVERAGE(G10:X10),1)</f>
+        <f>ROUND(AVERAGE(G10:Z10),1)</f>
         <v/>
       </c>
       <c r="G10" s="128" t="n">
@@ -11335,8 +11355,12 @@
       <c r="X10" s="129" t="n">
         <v>3</v>
       </c>
-      <c r="Y10" s="128" t="n"/>
-      <c r="Z10" s="129" t="n"/>
+      <c r="Y10" s="128" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="129" t="n">
+        <v>1</v>
+      </c>
       <c r="AA10" s="128" t="n"/>
       <c r="AB10" s="129" t="n"/>
       <c r="AC10" s="128" t="n"/>
@@ -11415,11 +11439,11 @@
         <v>2</v>
       </c>
       <c r="E11" s="124">
-        <f>SUM(G11:X11)</f>
+        <f>SUM(G11:Z11)</f>
         <v/>
       </c>
       <c r="F11" s="124">
-        <f>ROUND(AVERAGE(G11:X11),1)</f>
+        <f>ROUND(AVERAGE(G11:Z11),1)</f>
         <v/>
       </c>
       <c r="G11" s="125" t="n"/>
@@ -11528,11 +11552,11 @@
         <v>0</v>
       </c>
       <c r="E12" s="129">
-        <f>SUM(G12:X12)</f>
+        <f>SUM(G12:Z12)</f>
         <v/>
       </c>
       <c r="F12" s="129">
-        <f>ROUND(AVERAGE(G12:X12),1)</f>
+        <f>ROUND(AVERAGE(G12:Z12),1)</f>
         <v/>
       </c>
       <c r="G12" s="128" t="n"/>
@@ -11630,14 +11654,14 @@
         <v>2</v>
       </c>
       <c r="D13" s="123" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="124">
-        <f>SUM(G13:X13)</f>
+        <f>SUM(G13:Z13)</f>
         <v/>
       </c>
       <c r="F13" s="124">
-        <f>ROUND(AVERAGE(G13:X13),1)</f>
+        <f>ROUND(AVERAGE(G13:Z13),1)</f>
         <v/>
       </c>
       <c r="G13" s="123" t="n">
@@ -11694,8 +11718,12 @@
           <t>SKIP</t>
         </is>
       </c>
-      <c r="Y13" s="125" t="n"/>
-      <c r="Z13" s="124" t="n"/>
+      <c r="Y13" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="124" t="n">
+        <v>3</v>
+      </c>
       <c r="AA13" s="125" t="n"/>
       <c r="AB13" s="124" t="n"/>
       <c r="AC13" s="123" t="n"/>
@@ -11774,11 +11802,11 @@
         <v>1</v>
       </c>
       <c r="E14" s="129">
-        <f>SUM(G14:X14)</f>
+        <f>SUM(G14:Z14)</f>
         <v/>
       </c>
       <c r="F14" s="129">
-        <f>ROUND(AVERAGE(G14:X14),1)</f>
+        <f>ROUND(AVERAGE(G14:Z14),1)</f>
         <v/>
       </c>
       <c r="G14" s="128" t="n">
@@ -11883,11 +11911,11 @@
         <v>3</v>
       </c>
       <c r="E15" s="124">
-        <f>SUM(G15:X15)</f>
+        <f>SUM(G15:Z15)</f>
         <v/>
       </c>
       <c r="F15" s="124">
-        <f>ROUND(AVERAGE(G15:X15),1)</f>
+        <f>ROUND(AVERAGE(G15:Z15),1)</f>
         <v/>
       </c>
       <c r="G15" s="125" t="n"/>
@@ -12000,11 +12028,11 @@
         <v>0</v>
       </c>
       <c r="E16" s="129">
-        <f>SUM(G16:X16)</f>
+        <f>SUM(G16:Z16)</f>
         <v/>
       </c>
       <c r="F16" s="129">
-        <f>ROUND(AVERAGE(G16:X16),1)</f>
+        <f>ROUND(AVERAGE(G16:Z16),1)</f>
         <v/>
       </c>
       <c r="G16" s="128" t="n"/>
@@ -12105,11 +12133,11 @@
         <v>0</v>
       </c>
       <c r="E17" s="124">
-        <f>SUM(G17:X17)</f>
+        <f>SUM(G17:Z17)</f>
         <v/>
       </c>
       <c r="F17" s="124">
-        <f>ROUND(AVERAGE(G17:X17),1)</f>
+        <f>ROUND(AVERAGE(G17:Z17),1)</f>
         <v/>
       </c>
       <c r="G17" s="125" t="n"/>
@@ -12207,14 +12235,14 @@
         <v>0</v>
       </c>
       <c r="D18" s="128" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="129">
-        <f>SUM(G18:X18)</f>
+        <f>SUM(G18:Z18)</f>
         <v/>
       </c>
       <c r="F18" s="129">
-        <f>ROUND(AVERAGE(G18:X18),1)</f>
+        <f>ROUND(AVERAGE(G18:Z18),1)</f>
         <v/>
       </c>
       <c r="G18" s="128" t="n"/>
@@ -12243,8 +12271,12 @@
       </c>
       <c r="W18" s="128" t="n"/>
       <c r="X18" s="129" t="n"/>
-      <c r="Y18" s="128" t="n"/>
-      <c r="Z18" s="129" t="n"/>
+      <c r="Y18" s="128" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="129" t="n">
+        <v>2</v>
+      </c>
       <c r="AA18" s="128" t="n"/>
       <c r="AB18" s="129" t="n"/>
       <c r="AC18" s="128" t="n"/>
@@ -12320,14 +12352,14 @@
         <v>0</v>
       </c>
       <c r="D19" s="123" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E19" s="124">
-        <f>SUM(G19:X19)</f>
+        <f>SUM(G19:Z19)</f>
         <v/>
       </c>
       <c r="F19" s="124">
-        <f>ROUND(AVERAGE(G19:X19),1)</f>
+        <f>ROUND(AVERAGE(G19:Z19),1)</f>
         <v/>
       </c>
       <c r="G19" s="123" t="n">
@@ -12372,8 +12404,12 @@
       <c r="X19" s="124" t="n">
         <v>2</v>
       </c>
-      <c r="Y19" s="125" t="n"/>
-      <c r="Z19" s="124" t="n"/>
+      <c r="Y19" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z19" s="124" t="n">
+        <v>0</v>
+      </c>
       <c r="AA19" s="125" t="n"/>
       <c r="AB19" s="124" t="n"/>
       <c r="AC19" s="123" t="n"/>
@@ -12452,11 +12488,11 @@
         <v>0</v>
       </c>
       <c r="E20" s="129">
-        <f>SUM(G20:X20)</f>
+        <f>SUM(G20:Z20)</f>
         <v/>
       </c>
       <c r="F20" s="129">
-        <f>ROUND(AVERAGE(G20:X20),1)</f>
+        <f>ROUND(AVERAGE(G20:Z20),1)</f>
         <v/>
       </c>
       <c r="G20" s="128" t="n"/>
@@ -12557,11 +12593,11 @@
         <v>5</v>
       </c>
       <c r="E21" s="124">
-        <f>SUM(G21:X21)</f>
+        <f>SUM(G21:Z21)</f>
         <v/>
       </c>
       <c r="F21" s="124">
-        <f>ROUND(AVERAGE(G21:X21),1)</f>
+        <f>ROUND(AVERAGE(G21:Z21),1)</f>
         <v/>
       </c>
       <c r="G21" s="125" t="n"/>
@@ -12682,11 +12718,11 @@
         <v>4</v>
       </c>
       <c r="E22" s="129">
-        <f>SUM(G22:X22)</f>
+        <f>SUM(G22:Z22)</f>
         <v/>
       </c>
       <c r="F22" s="129">
-        <f>ROUND(AVERAGE(G22:X22),1)</f>
+        <f>ROUND(AVERAGE(G22:Z22),1)</f>
         <v/>
       </c>
       <c r="G22" s="128" t="n">
@@ -12800,14 +12836,14 @@
         <v>0</v>
       </c>
       <c r="D23" s="123" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" s="124">
-        <f>SUM(G23:X23)</f>
+        <f>SUM(G23:Z23)</f>
         <v/>
       </c>
       <c r="F23" s="124">
-        <f>ROUND(AVERAGE(G23:X23),1)</f>
+        <f>ROUND(AVERAGE(G23:Z23),1)</f>
         <v/>
       </c>
       <c r="G23" s="123" t="n">
@@ -12836,8 +12872,12 @@
       <c r="V23" s="124" t="n"/>
       <c r="W23" s="125" t="n"/>
       <c r="X23" s="124" t="n"/>
-      <c r="Y23" s="125" t="n"/>
-      <c r="Z23" s="124" t="n"/>
+      <c r="Y23" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z23" s="124" t="n">
+        <v>3</v>
+      </c>
       <c r="AA23" s="125" t="n"/>
       <c r="AB23" s="124" t="n"/>
       <c r="AC23" s="123" t="n"/>
@@ -12916,11 +12956,11 @@
         <v>0</v>
       </c>
       <c r="E24" s="129">
-        <f>SUM(G24:X24)</f>
+        <f>SUM(G24:Z24)</f>
         <v/>
       </c>
       <c r="F24" s="129">
-        <f>ROUND(AVERAGE(G24:X24),1)</f>
+        <f>ROUND(AVERAGE(G24:Z24),1)</f>
         <v/>
       </c>
       <c r="G24" s="128" t="n"/>
@@ -13021,11 +13061,11 @@
         <v>5</v>
       </c>
       <c r="E25" s="124">
-        <f>SUM(G25:X25)</f>
+        <f>SUM(G25:Z25)</f>
         <v/>
       </c>
       <c r="F25" s="124">
-        <f>ROUND(AVERAGE(G25:X25),1)</f>
+        <f>ROUND(AVERAGE(G25:Z25),1)</f>
         <v/>
       </c>
       <c r="G25" s="125" t="n"/>
@@ -13147,14 +13187,14 @@
         <v>1</v>
       </c>
       <c r="D26" s="128" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E26" s="129">
-        <f>SUM(G26:X26)</f>
+        <f>SUM(G26:Z26)</f>
         <v/>
       </c>
       <c r="F26" s="129">
-        <f>ROUND(AVERAGE(G26:X26),1)</f>
+        <f>ROUND(AVERAGE(G26:Z26),1)</f>
         <v/>
       </c>
       <c r="G26" s="128" t="inlineStr">
@@ -13201,8 +13241,12 @@
           <t>SKIP</t>
         </is>
       </c>
-      <c r="Y26" s="128" t="n"/>
-      <c r="Z26" s="129" t="n"/>
+      <c r="Y26" s="128" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z26" s="129" t="n">
+        <v>3</v>
+      </c>
       <c r="AA26" s="128" t="n"/>
       <c r="AB26" s="129" t="n"/>
       <c r="AC26" s="128" t="n"/>
@@ -13281,11 +13325,11 @@
         <v>0</v>
       </c>
       <c r="E27" s="124">
-        <f>SUM(G27:X27)</f>
+        <f>SUM(G27:Z27)</f>
         <v/>
       </c>
       <c r="F27" s="124">
-        <f>ROUND(AVERAGE(G27:X27),1)</f>
+        <f>ROUND(AVERAGE(G27:Z27),1)</f>
         <v/>
       </c>
       <c r="G27" s="125" t="n"/>
@@ -13383,14 +13427,14 @@
         <v>0</v>
       </c>
       <c r="D28" s="128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="129">
-        <f>SUM(G28:X28)</f>
+        <f>SUM(G28:Z28)</f>
         <v/>
       </c>
       <c r="F28" s="129">
-        <f>ROUND(AVERAGE(G28:X28),1)</f>
+        <f>ROUND(AVERAGE(G28:Z28),1)</f>
         <v/>
       </c>
       <c r="G28" s="128" t="n"/>
@@ -13415,8 +13459,12 @@
       </c>
       <c r="W28" s="128" t="n"/>
       <c r="X28" s="129" t="n"/>
-      <c r="Y28" s="128" t="n"/>
-      <c r="Z28" s="129" t="n"/>
+      <c r="Y28" s="128" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z28" s="129" t="n">
+        <v>3</v>
+      </c>
       <c r="AA28" s="128" t="n"/>
       <c r="AB28" s="129" t="n"/>
       <c r="AC28" s="128" t="n"/>
@@ -13492,14 +13540,14 @@
         <v>0</v>
       </c>
       <c r="D29" s="123" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E29" s="124">
-        <f>SUM(G29:X29)</f>
+        <f>SUM(G29:Z29)</f>
         <v/>
       </c>
       <c r="F29" s="124">
-        <f>ROUND(AVERAGE(G29:X29),1)</f>
+        <f>ROUND(AVERAGE(G29:Z29),1)</f>
         <v/>
       </c>
       <c r="G29" s="125" t="n"/>
@@ -13540,8 +13588,12 @@
       <c r="X29" s="124" t="n">
         <v>3</v>
       </c>
-      <c r="Y29" s="125" t="n"/>
-      <c r="Z29" s="124" t="n"/>
+      <c r="Y29" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z29" s="124" t="n">
+        <v>3</v>
+      </c>
       <c r="AA29" s="125" t="n"/>
       <c r="AB29" s="124" t="n"/>
       <c r="AC29" s="123" t="n"/>
@@ -13617,14 +13669,14 @@
         <v>1</v>
       </c>
       <c r="D30" s="128" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E30" s="129">
-        <f>SUM(G30:X30)</f>
+        <f>SUM(G30:Z30)</f>
         <v/>
       </c>
       <c r="F30" s="129">
-        <f>ROUND(AVERAGE(G30:X30),1)</f>
+        <f>ROUND(AVERAGE(G30:Z30),1)</f>
         <v/>
       </c>
       <c r="G30" s="128" t="n"/>
@@ -13677,8 +13729,12 @@
       <c r="X30" s="129" t="n">
         <v>3</v>
       </c>
-      <c r="Y30" s="128" t="n"/>
-      <c r="Z30" s="129" t="n"/>
+      <c r="Y30" s="128" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z30" s="129" t="n">
+        <v>2</v>
+      </c>
       <c r="AA30" s="128" t="n"/>
       <c r="AB30" s="129" t="n"/>
       <c r="AC30" s="128" t="n"/>
@@ -13757,11 +13813,11 @@
         <v>0</v>
       </c>
       <c r="E31" s="124">
-        <f>SUM(G31:X31)</f>
+        <f>SUM(G31:Z31)</f>
         <v/>
       </c>
       <c r="F31" s="124">
-        <f>ROUND(AVERAGE(G31:X31),1)</f>
+        <f>ROUND(AVERAGE(G31:Z31),1)</f>
         <v/>
       </c>
       <c r="G31" s="125" t="n"/>
@@ -13862,11 +13918,11 @@
         <v>4</v>
       </c>
       <c r="E32" s="129">
-        <f>SUM(G32:X32)</f>
+        <f>SUM(G32:Z32)</f>
         <v/>
       </c>
       <c r="F32" s="129">
-        <f>ROUND(AVERAGE(G32:X32),1)</f>
+        <f>ROUND(AVERAGE(G32:Z32),1)</f>
         <v/>
       </c>
       <c r="G32" s="128" t="n">
@@ -13991,11 +14047,11 @@
         <v>4</v>
       </c>
       <c r="E33" s="124">
-        <f>SUM(G33:X33)</f>
+        <f>SUM(G33:Z33)</f>
         <v/>
       </c>
       <c r="F33" s="124">
-        <f>ROUND(AVERAGE(G33:X33),1)</f>
+        <f>ROUND(AVERAGE(G33:Z33),1)</f>
         <v/>
       </c>
       <c r="G33" s="123" t="n">
@@ -14109,14 +14165,14 @@
         <v>0</v>
       </c>
       <c r="D34" s="128" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E34" s="129">
-        <f>SUM(G34:X34)</f>
+        <f>SUM(G34:Z34)</f>
         <v/>
       </c>
       <c r="F34" s="129">
-        <f>ROUND(AVERAGE(G34:X34),1)</f>
+        <f>ROUND(AVERAGE(G34:Z34),1)</f>
         <v/>
       </c>
       <c r="G34" s="128" t="n">
@@ -14165,8 +14221,12 @@
       </c>
       <c r="W34" s="128" t="n"/>
       <c r="X34" s="129" t="n"/>
-      <c r="Y34" s="128" t="n"/>
-      <c r="Z34" s="129" t="n"/>
+      <c r="Y34" s="128" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z34" s="129" t="n">
+        <v>2</v>
+      </c>
       <c r="AA34" s="128" t="n"/>
       <c r="AB34" s="129" t="n"/>
       <c r="AC34" s="128" t="n"/>
@@ -14245,11 +14305,11 @@
         <v>0</v>
       </c>
       <c r="E35" s="124">
-        <f>SUM(G35:X35)</f>
+        <f>SUM(G35:Z35)</f>
         <v/>
       </c>
       <c r="F35" s="124">
-        <f>ROUND(AVERAGE(G35:X35),1)</f>
+        <f>ROUND(AVERAGE(G35:Z35),1)</f>
         <v/>
       </c>
       <c r="G35" s="125" t="n"/>
@@ -14350,11 +14410,11 @@
         <v>3</v>
       </c>
       <c r="E36" s="129">
-        <f>SUM(G36:X36)</f>
+        <f>SUM(G36:Z36)</f>
         <v/>
       </c>
       <c r="F36" s="129">
-        <f>ROUND(AVERAGE(G36:X36),1)</f>
+        <f>ROUND(AVERAGE(G36:Z36),1)</f>
         <v/>
       </c>
       <c r="G36" s="128" t="n"/>
@@ -14467,11 +14527,11 @@
         <v>2</v>
       </c>
       <c r="E37" s="124">
-        <f>SUM(G37:X37)</f>
+        <f>SUM(G37:Z37)</f>
         <v/>
       </c>
       <c r="F37" s="124">
-        <f>ROUND(AVERAGE(G37:X37),1)</f>
+        <f>ROUND(AVERAGE(G37:Z37),1)</f>
         <v/>
       </c>
       <c r="G37" s="125" t="n"/>
@@ -14584,11 +14644,11 @@
         <v>2</v>
       </c>
       <c r="E38" s="129">
-        <f>SUM(G38:X38)</f>
+        <f>SUM(G38:Z38)</f>
         <v/>
       </c>
       <c r="F38" s="129">
-        <f>ROUND(AVERAGE(G38:X38),1)</f>
+        <f>ROUND(AVERAGE(G38:Z38),1)</f>
         <v/>
       </c>
       <c r="G38" s="128" t="inlineStr">
@@ -14700,14 +14760,14 @@
         <v>0</v>
       </c>
       <c r="D39" s="123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="124">
-        <f>SUM(G39:X39)</f>
+        <f>SUM(G39:Z39)</f>
         <v/>
       </c>
       <c r="F39" s="124">
-        <f>ROUND(AVERAGE(G39:X39),1)</f>
+        <f>ROUND(AVERAGE(G39:Z39),1)</f>
         <v/>
       </c>
       <c r="G39" s="125" t="n"/>
@@ -14732,8 +14792,12 @@
       </c>
       <c r="W39" s="125" t="n"/>
       <c r="X39" s="124" t="n"/>
-      <c r="Y39" s="125" t="n"/>
-      <c r="Z39" s="124" t="n"/>
+      <c r="Y39" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z39" s="124" t="n">
+        <v>2</v>
+      </c>
       <c r="AA39" s="125" t="n"/>
       <c r="AB39" s="124" t="n"/>
       <c r="AC39" s="123" t="n"/>
@@ -14809,14 +14873,14 @@
         <v>0</v>
       </c>
       <c r="D40" s="128" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E40" s="129">
-        <f>SUM(G40:X40)</f>
+        <f>SUM(G40:Z40)</f>
         <v/>
       </c>
       <c r="F40" s="129">
-        <f>ROUND(AVERAGE(G40:X40),1)</f>
+        <f>ROUND(AVERAGE(G40:Z40),1)</f>
         <v/>
       </c>
       <c r="G40" s="128" t="n"/>
@@ -14847,8 +14911,12 @@
           <t>SKIP</t>
         </is>
       </c>
-      <c r="Y40" s="128" t="n"/>
-      <c r="Z40" s="129" t="n"/>
+      <c r="Y40" s="128" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z40" s="129" t="n">
+        <v>2</v>
+      </c>
       <c r="AA40" s="128" t="n"/>
       <c r="AB40" s="129" t="n"/>
       <c r="AC40" s="128" t="n"/>
@@ -14927,11 +14995,11 @@
         <v>0</v>
       </c>
       <c r="E41" s="124">
-        <f>SUM(G41:X41)</f>
+        <f>SUM(G41:Z41)</f>
         <v/>
       </c>
       <c r="F41" s="124">
-        <f>ROUND(AVERAGE(G41:X41),1)</f>
+        <f>ROUND(AVERAGE(G41:Z41),1)</f>
         <v/>
       </c>
       <c r="G41" s="125" t="n"/>
@@ -15019,7 +15087,7 @@
     <row r="42">
       <c r="A42" s="128" t="inlineStr">
         <is>
-          <t>★deimon★</t>
+          <t>tazio</t>
         </is>
       </c>
       <c r="B42" s="128" t="n">
@@ -15032,11 +15100,11 @@
         <v>0</v>
       </c>
       <c r="E42" s="129">
-        <f>SUM(G42:X42)</f>
+        <f>SUM(G42:Z42)</f>
         <v/>
       </c>
       <c r="F42" s="129">
-        <f>ROUND(AVERAGE(G42:X42),1)</f>
+        <f>ROUND(AVERAGE(G42:Z42),1)</f>
         <v/>
       </c>
       <c r="G42" s="128" t="n"/>
@@ -15124,7 +15192,7 @@
     <row r="43">
       <c r="A43" s="123" t="inlineStr">
         <is>
-          <t>tazio</t>
+          <t>alhfmfh</t>
         </is>
       </c>
       <c r="B43" s="123" t="n">
@@ -15137,99 +15205,99 @@
         <v>0</v>
       </c>
       <c r="E43" s="124">
-        <f>SUM(G43:X43)</f>
+        <f>SUM(G43:Z43)</f>
         <v/>
       </c>
       <c r="F43" s="124">
-        <f>ROUND(AVERAGE(G43:X43),1)</f>
-        <v/>
-      </c>
-      <c r="G43" s="123" t="n"/>
+        <f>ROUND(AVERAGE(G43:Z43),1)</f>
+        <v/>
+      </c>
+      <c r="G43" s="125" t="n"/>
       <c r="H43" s="124" t="n"/>
-      <c r="I43" s="123" t="n"/>
+      <c r="I43" s="125" t="n"/>
       <c r="J43" s="124" t="n"/>
-      <c r="K43" s="123" t="n"/>
+      <c r="K43" s="125" t="n"/>
       <c r="L43" s="124" t="n"/>
-      <c r="M43" s="123" t="n"/>
+      <c r="M43" s="125" t="n"/>
       <c r="N43" s="124" t="n"/>
-      <c r="O43" s="123" t="n"/>
+      <c r="O43" s="125" t="n"/>
       <c r="P43" s="124" t="n"/>
-      <c r="Q43" s="123" t="n"/>
+      <c r="Q43" s="125" t="n"/>
       <c r="R43" s="124" t="n"/>
-      <c r="S43" s="123" t="n"/>
+      <c r="S43" s="125" t="n"/>
       <c r="T43" s="124" t="n"/>
-      <c r="U43" s="123" t="n"/>
+      <c r="U43" s="125" t="n"/>
       <c r="V43" s="124" t="n"/>
-      <c r="W43" s="123" t="n"/>
+      <c r="W43" s="125" t="n"/>
       <c r="X43" s="124" t="n"/>
-      <c r="Y43" s="123" t="n"/>
+      <c r="Y43" s="125" t="n"/>
       <c r="Z43" s="124" t="n"/>
-      <c r="AA43" s="123" t="n"/>
+      <c r="AA43" s="125" t="n"/>
       <c r="AB43" s="124" t="n"/>
       <c r="AC43" s="123" t="n"/>
-      <c r="AD43" s="124" t="n"/>
-      <c r="AE43" s="124" t="n"/>
-      <c r="AF43" s="124" t="n"/>
-      <c r="AG43" s="124" t="n"/>
-      <c r="AH43" s="124" t="n"/>
-      <c r="AI43" s="124" t="n"/>
-      <c r="AJ43" s="124" t="n"/>
-      <c r="AK43" s="124" t="n"/>
-      <c r="AL43" s="124" t="n"/>
-      <c r="AM43" s="124" t="n"/>
-      <c r="AN43" s="124" t="n"/>
-      <c r="AO43" s="124" t="n"/>
-      <c r="AP43" s="124" t="n"/>
-      <c r="AQ43" s="124" t="n"/>
-      <c r="AR43" s="124" t="n"/>
-      <c r="AS43" s="124" t="n"/>
-      <c r="AT43" s="124" t="n"/>
-      <c r="AU43" s="124" t="n"/>
-      <c r="AV43" s="124" t="n"/>
-      <c r="AW43" s="124" t="n"/>
-      <c r="AX43" s="124" t="n"/>
-      <c r="AY43" s="124" t="n"/>
-      <c r="AZ43" s="124" t="n"/>
-      <c r="BA43" s="124" t="n"/>
-      <c r="BB43" s="124" t="n"/>
-      <c r="BC43" s="124" t="n"/>
-      <c r="BD43" s="124" t="n"/>
-      <c r="BE43" s="124" t="n"/>
-      <c r="BF43" s="124" t="n"/>
-      <c r="BG43" s="124" t="n"/>
-      <c r="BH43" s="124" t="n"/>
-      <c r="BI43" s="124" t="n"/>
-      <c r="BJ43" s="124" t="n"/>
-      <c r="BK43" s="124" t="n"/>
-      <c r="BL43" s="124" t="n"/>
-      <c r="BM43" s="124" t="n"/>
-      <c r="BN43" s="124" t="n"/>
-      <c r="BO43" s="124" t="n"/>
-      <c r="BP43" s="124" t="n"/>
-      <c r="BQ43" s="124" t="n"/>
-      <c r="BR43" s="124" t="n"/>
-      <c r="BS43" s="124" t="n"/>
-      <c r="BT43" s="124" t="n"/>
-      <c r="BU43" s="124" t="n"/>
-      <c r="BV43" s="124" t="n"/>
-      <c r="BW43" s="124" t="n"/>
-      <c r="BX43" s="124" t="n"/>
-      <c r="BY43" s="124" t="n"/>
-      <c r="BZ43" s="124" t="n"/>
-      <c r="CA43" s="124" t="n"/>
-      <c r="CB43" s="124" t="n"/>
-      <c r="CC43" s="124" t="n"/>
-      <c r="CD43" s="124" t="n"/>
-      <c r="CE43" s="124" t="n"/>
-      <c r="CF43" s="124" t="n"/>
-      <c r="CG43" s="124" t="n"/>
-      <c r="CH43" s="124" t="n"/>
-      <c r="CI43" s="124" t="n"/>
+      <c r="AD43" s="125" t="n"/>
+      <c r="AE43" s="125" t="n"/>
+      <c r="AF43" s="125" t="n"/>
+      <c r="AG43" s="125" t="n"/>
+      <c r="AH43" s="125" t="n"/>
+      <c r="AI43" s="125" t="n"/>
+      <c r="AJ43" s="125" t="n"/>
+      <c r="AK43" s="125" t="n"/>
+      <c r="AL43" s="125" t="n"/>
+      <c r="AM43" s="125" t="n"/>
+      <c r="AN43" s="125" t="n"/>
+      <c r="AO43" s="125" t="n"/>
+      <c r="AP43" s="125" t="n"/>
+      <c r="AQ43" s="125" t="n"/>
+      <c r="AR43" s="125" t="n"/>
+      <c r="AS43" s="125" t="n"/>
+      <c r="AT43" s="125" t="n"/>
+      <c r="AU43" s="125" t="n"/>
+      <c r="AV43" s="125" t="n"/>
+      <c r="AW43" s="125" t="n"/>
+      <c r="AX43" s="125" t="n"/>
+      <c r="AY43" s="125" t="n"/>
+      <c r="AZ43" s="125" t="n"/>
+      <c r="BA43" s="125" t="n"/>
+      <c r="BB43" s="125" t="n"/>
+      <c r="BC43" s="125" t="n"/>
+      <c r="BD43" s="125" t="n"/>
+      <c r="BE43" s="125" t="n"/>
+      <c r="BF43" s="125" t="n"/>
+      <c r="BG43" s="125" t="n"/>
+      <c r="BH43" s="125" t="n"/>
+      <c r="BI43" s="125" t="n"/>
+      <c r="BJ43" s="125" t="n"/>
+      <c r="BK43" s="125" t="n"/>
+      <c r="BL43" s="125" t="n"/>
+      <c r="BM43" s="125" t="n"/>
+      <c r="BN43" s="125" t="n"/>
+      <c r="BO43" s="125" t="n"/>
+      <c r="BP43" s="125" t="n"/>
+      <c r="BQ43" s="125" t="n"/>
+      <c r="BR43" s="125" t="n"/>
+      <c r="BS43" s="125" t="n"/>
+      <c r="BT43" s="125" t="n"/>
+      <c r="BU43" s="125" t="n"/>
+      <c r="BV43" s="125" t="n"/>
+      <c r="BW43" s="125" t="n"/>
+      <c r="BX43" s="125" t="n"/>
+      <c r="BY43" s="125" t="n"/>
+      <c r="BZ43" s="125" t="n"/>
+      <c r="CA43" s="125" t="n"/>
+      <c r="CB43" s="125" t="n"/>
+      <c r="CC43" s="125" t="n"/>
+      <c r="CD43" s="125" t="n"/>
+      <c r="CE43" s="125" t="n"/>
+      <c r="CF43" s="125" t="n"/>
+      <c r="CG43" s="125" t="n"/>
+      <c r="CH43" s="125" t="n"/>
+      <c r="CI43" s="125" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="128" t="inlineStr">
         <is>
-          <t>alhfmfh</t>
+          <t>GioStyle</t>
         </is>
       </c>
       <c r="B44" s="128" t="n">
@@ -15242,11 +15310,11 @@
         <v>0</v>
       </c>
       <c r="E44" s="129">
-        <f>SUM(G44:X44)</f>
+        <f>SUM(G44:Z44)</f>
         <v/>
       </c>
       <c r="F44" s="129">
-        <f>ROUND(AVERAGE(G44:X44),1)</f>
+        <f>ROUND(AVERAGE(G44:Z44),1)</f>
         <v/>
       </c>
       <c r="G44" s="132" t="n"/>
@@ -15334,24 +15402,24 @@
     <row r="45">
       <c r="A45" s="123" t="inlineStr">
         <is>
-          <t>GioStyle</t>
+          <t>francesco</t>
         </is>
       </c>
       <c r="B45" s="123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="124" t="n">
         <v>0</v>
       </c>
       <c r="D45" s="123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="124">
-        <f>SUM(G45:X45)</f>
+        <f>SUM(G45:Z45)</f>
         <v/>
       </c>
       <c r="F45" s="124">
-        <f>ROUND(AVERAGE(G45:X45),1)</f>
+        <f>ROUND(AVERAGE(G45:Z45),1)</f>
         <v/>
       </c>
       <c r="G45" s="125" t="n"/>
@@ -15372,8 +15440,14 @@
       <c r="V45" s="124" t="n"/>
       <c r="W45" s="125" t="n"/>
       <c r="X45" s="124" t="n"/>
-      <c r="Y45" s="125" t="n"/>
-      <c r="Z45" s="124" t="n"/>
+      <c r="Y45" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="124" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
       <c r="AA45" s="125" t="n"/>
       <c r="AB45" s="124" t="n"/>
       <c r="AC45" s="123" t="n"/>
@@ -15439,24 +15513,24 @@
     <row r="46">
       <c r="A46" s="128" t="inlineStr">
         <is>
-          <t>francesco</t>
+          <t>PIPPII</t>
         </is>
       </c>
       <c r="B46" s="128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="129" t="n">
         <v>0</v>
       </c>
       <c r="D46" s="128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="129">
-        <f>SUM(G46:X46)</f>
+        <f>SUM(G46:Z46)</f>
         <v/>
       </c>
       <c r="F46" s="129">
-        <f>ROUND(AVERAGE(G46:X46),1)</f>
+        <f>ROUND(AVERAGE(G46:Z46),1)</f>
         <v/>
       </c>
       <c r="G46" s="132" t="n"/>
@@ -15477,8 +15551,14 @@
       <c r="V46" s="129" t="n"/>
       <c r="W46" s="132" t="n"/>
       <c r="X46" s="129" t="n"/>
-      <c r="Y46" s="132" t="n"/>
-      <c r="Z46" s="129" t="n"/>
+      <c r="Y46" s="132" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z46" s="129" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
       <c r="AA46" s="132" t="n"/>
       <c r="AB46" s="129" t="n"/>
       <c r="AC46" s="128" t="n"/>
@@ -15544,7 +15624,7 @@
     <row r="47">
       <c r="A47" s="123" t="inlineStr">
         <is>
-          <t>PIPPII</t>
+          <t>Fryck</t>
         </is>
       </c>
       <c r="B47" s="123" t="n">
@@ -15554,14 +15634,14 @@
         <v>0</v>
       </c>
       <c r="D47" s="123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="124">
-        <f>SUM(G47:X47)</f>
+        <f>SUM(G47:Z47)</f>
         <v/>
       </c>
       <c r="F47" s="124">
-        <f>ROUND(AVERAGE(G47:X47),1)</f>
+        <f>ROUND(AVERAGE(G47:Z47),1)</f>
         <v/>
       </c>
       <c r="G47" s="125" t="n"/>
@@ -15582,8 +15662,12 @@
       <c r="V47" s="124" t="n"/>
       <c r="W47" s="125" t="n"/>
       <c r="X47" s="124" t="n"/>
-      <c r="Y47" s="125" t="n"/>
-      <c r="Z47" s="124" t="n"/>
+      <c r="Y47" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z47" s="124" t="n">
+        <v>3</v>
+      </c>
       <c r="AA47" s="125" t="n"/>
       <c r="AB47" s="124" t="n"/>
       <c r="AC47" s="123" t="n"/>
@@ -15649,7 +15733,7 @@
     <row r="48">
       <c r="A48" s="128" t="inlineStr">
         <is>
-          <t>Fryck</t>
+          <t>alesofi</t>
         </is>
       </c>
       <c r="B48" s="128" t="n">
@@ -15662,11 +15746,11 @@
         <v>0</v>
       </c>
       <c r="E48" s="129">
-        <f>SUM(G48:X48)</f>
+        <f>SUM(G48:Z48)</f>
         <v/>
       </c>
       <c r="F48" s="129">
-        <f>ROUND(AVERAGE(G48:X48),1)</f>
+        <f>ROUND(AVERAGE(G48:Z48),1)</f>
         <v/>
       </c>
       <c r="G48" s="132" t="n"/>
@@ -15751,6 +15835,111 @@
       <c r="CH48" s="132" t="n"/>
       <c r="CI48" s="132" t="n"/>
     </row>
+    <row r="49">
+      <c r="A49" s="123" t="inlineStr">
+        <is>
+          <t>fabiovesco</t>
+        </is>
+      </c>
+      <c r="B49" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="124" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="124">
+        <f>SUM(G49:Z49)</f>
+        <v/>
+      </c>
+      <c r="F49" s="124">
+        <f>ROUND(AVERAGE(G49:Z49),1)</f>
+        <v/>
+      </c>
+      <c r="G49" s="125" t="n"/>
+      <c r="H49" s="124" t="n"/>
+      <c r="I49" s="125" t="n"/>
+      <c r="J49" s="124" t="n"/>
+      <c r="K49" s="125" t="n"/>
+      <c r="L49" s="124" t="n"/>
+      <c r="M49" s="125" t="n"/>
+      <c r="N49" s="124" t="n"/>
+      <c r="O49" s="125" t="n"/>
+      <c r="P49" s="124" t="n"/>
+      <c r="Q49" s="125" t="n"/>
+      <c r="R49" s="124" t="n"/>
+      <c r="S49" s="125" t="n"/>
+      <c r="T49" s="124" t="n"/>
+      <c r="U49" s="125" t="n"/>
+      <c r="V49" s="124" t="n"/>
+      <c r="W49" s="125" t="n"/>
+      <c r="X49" s="124" t="n"/>
+      <c r="Y49" s="125" t="n"/>
+      <c r="Z49" s="124" t="n"/>
+      <c r="AA49" s="125" t="n"/>
+      <c r="AB49" s="124" t="n"/>
+      <c r="AC49" s="123" t="n"/>
+      <c r="AD49" s="125" t="n"/>
+      <c r="AE49" s="125" t="n"/>
+      <c r="AF49" s="125" t="n"/>
+      <c r="AG49" s="125" t="n"/>
+      <c r="AH49" s="125" t="n"/>
+      <c r="AI49" s="125" t="n"/>
+      <c r="AJ49" s="125" t="n"/>
+      <c r="AK49" s="125" t="n"/>
+      <c r="AL49" s="125" t="n"/>
+      <c r="AM49" s="125" t="n"/>
+      <c r="AN49" s="125" t="n"/>
+      <c r="AO49" s="125" t="n"/>
+      <c r="AP49" s="125" t="n"/>
+      <c r="AQ49" s="125" t="n"/>
+      <c r="AR49" s="125" t="n"/>
+      <c r="AS49" s="125" t="n"/>
+      <c r="AT49" s="125" t="n"/>
+      <c r="AU49" s="125" t="n"/>
+      <c r="AV49" s="125" t="n"/>
+      <c r="AW49" s="125" t="n"/>
+      <c r="AX49" s="125" t="n"/>
+      <c r="AY49" s="125" t="n"/>
+      <c r="AZ49" s="125" t="n"/>
+      <c r="BA49" s="125" t="n"/>
+      <c r="BB49" s="125" t="n"/>
+      <c r="BC49" s="125" t="n"/>
+      <c r="BD49" s="125" t="n"/>
+      <c r="BE49" s="125" t="n"/>
+      <c r="BF49" s="125" t="n"/>
+      <c r="BG49" s="125" t="n"/>
+      <c r="BH49" s="125" t="n"/>
+      <c r="BI49" s="125" t="n"/>
+      <c r="BJ49" s="125" t="n"/>
+      <c r="BK49" s="125" t="n"/>
+      <c r="BL49" s="125" t="n"/>
+      <c r="BM49" s="125" t="n"/>
+      <c r="BN49" s="125" t="n"/>
+      <c r="BO49" s="125" t="n"/>
+      <c r="BP49" s="125" t="n"/>
+      <c r="BQ49" s="125" t="n"/>
+      <c r="BR49" s="125" t="n"/>
+      <c r="BS49" s="125" t="n"/>
+      <c r="BT49" s="125" t="n"/>
+      <c r="BU49" s="125" t="n"/>
+      <c r="BV49" s="125" t="n"/>
+      <c r="BW49" s="125" t="n"/>
+      <c r="BX49" s="125" t="n"/>
+      <c r="BY49" s="125" t="n"/>
+      <c r="BZ49" s="125" t="n"/>
+      <c r="CA49" s="125" t="n"/>
+      <c r="CB49" s="125" t="n"/>
+      <c r="CC49" s="125" t="n"/>
+      <c r="CD49" s="125" t="n"/>
+      <c r="CE49" s="125" t="n"/>
+      <c r="CF49" s="125" t="n"/>
+      <c r="CG49" s="125" t="n"/>
+      <c r="CH49" s="125" t="n"/>
+      <c r="CI49" s="125" t="n"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:CL1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update WAR data - 2026-01-30
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -11632,7 +11632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI50"/>
+  <dimension ref="A1:CI48"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -11869,12 +11869,12 @@
       </c>
       <c r="AI1" s="107" t="inlineStr">
         <is>
-          <t>Colonna35</t>
+          <t>WAR-15 (1)</t>
         </is>
       </c>
       <c r="AJ1" s="112" t="inlineStr">
         <is>
-          <t>Colonna36</t>
+          <t>WAR-15 (2)</t>
         </is>
       </c>
       <c r="AK1" s="107" t="inlineStr">
@@ -12149,11 +12149,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="111">
-        <f>SUM(G2:AH2)</f>
+        <f>SUM(G2:AJ2)</f>
         <v/>
       </c>
       <c r="F2" s="68">
-        <f>ROUND(AVERAGE(G2:AH2),1)</f>
+        <f>ROUND(AVERAGE(G2:AJ2),1)</f>
         <v/>
       </c>
       <c r="G2" s="110" t="n"/>
@@ -12268,11 +12268,11 @@
         <v>0</v>
       </c>
       <c r="E3" s="68">
-        <f>SUM(G3:AH3)</f>
+        <f>SUM(G3:AJ3)</f>
         <v/>
       </c>
       <c r="F3" s="68">
-        <f>ROUND(AVERAGE(G3:AH3),1)</f>
+        <f>ROUND(AVERAGE(G3:AJ3),1)</f>
         <v/>
       </c>
     </row>
@@ -12283,20 +12283,20 @@
         </is>
       </c>
       <c r="B4" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="68">
-        <f>SUM(G4:AH4)</f>
+        <f>SUM(G4:AJ4)</f>
         <v/>
       </c>
       <c r="F4" s="68">
-        <f>ROUND(AVERAGE(G4:AH4),1)</f>
+        <f>ROUND(AVERAGE(G4:AJ4),1)</f>
         <v/>
       </c>
       <c r="I4" s="79" t="n">
@@ -12310,6 +12310,16 @@
       </c>
       <c r="X4" s="80" t="n">
         <v>1</v>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -12328,11 +12338,11 @@
         <v>0</v>
       </c>
       <c r="E5" s="68">
-        <f>SUM(G5:AH5)</f>
+        <f>SUM(G5:AJ5)</f>
         <v/>
       </c>
       <c r="F5" s="68">
-        <f>ROUND(AVERAGE(G5:AH5),1)</f>
+        <f>ROUND(AVERAGE(G5:AJ5),1)</f>
         <v/>
       </c>
     </row>
@@ -12352,11 +12362,11 @@
         <v>0</v>
       </c>
       <c r="E6" s="68">
-        <f>SUM(G6:AH6)</f>
+        <f>SUM(G6:AJ6)</f>
         <v/>
       </c>
       <c r="F6" s="68">
-        <f>ROUND(AVERAGE(G6:AH6),1)</f>
+        <f>ROUND(AVERAGE(G6:AJ6),1)</f>
         <v/>
       </c>
     </row>
@@ -12376,11 +12386,11 @@
         <v>3</v>
       </c>
       <c r="E7" s="68">
-        <f>SUM(G7:AH7)</f>
+        <f>SUM(G7:AJ7)</f>
         <v/>
       </c>
       <c r="F7" s="68">
-        <f>ROUND(AVERAGE(G7:AH7),1)</f>
+        <f>ROUND(AVERAGE(G7:AJ7),1)</f>
         <v/>
       </c>
       <c r="U7" s="79" t="n">
@@ -12409,20 +12419,20 @@
         </is>
       </c>
       <c r="B8" s="79" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" s="68" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="79" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="68">
-        <f>SUM(G8:AH8)</f>
+        <f>SUM(G8:AJ8)</f>
         <v/>
       </c>
       <c r="F8" s="68">
-        <f>ROUND(AVERAGE(G8:AH8),1)</f>
+        <f>ROUND(AVERAGE(G8:AJ8),1)</f>
         <v/>
       </c>
       <c r="G8" s="79" t="n">
@@ -12493,6 +12503,16 @@
         </is>
       </c>
       <c r="AD8" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
@@ -12514,11 +12534,11 @@
         <v>4</v>
       </c>
       <c r="E9" s="68">
-        <f>SUM(G9:AH9)</f>
+        <f>SUM(G9:AJ9)</f>
         <v/>
       </c>
       <c r="F9" s="68">
-        <f>ROUND(AVERAGE(G9:AH9),1)</f>
+        <f>ROUND(AVERAGE(G9:AJ9),1)</f>
         <v/>
       </c>
       <c r="K9" s="79" t="n">
@@ -12562,11 +12582,11 @@
         <v>0</v>
       </c>
       <c r="E10" s="68">
-        <f>SUM(G10:AH10)</f>
+        <f>SUM(G10:AJ10)</f>
         <v/>
       </c>
       <c r="F10" s="68">
-        <f>ROUND(AVERAGE(G10:AH10),1)</f>
+        <f>ROUND(AVERAGE(G10:AJ10),1)</f>
         <v/>
       </c>
     </row>
@@ -12586,11 +12606,11 @@
         <v>11</v>
       </c>
       <c r="E11" s="68">
-        <f>SUM(G11:AH11)</f>
+        <f>SUM(G11:AJ11)</f>
         <v/>
       </c>
       <c r="F11" s="68">
-        <f>ROUND(AVERAGE(G11:AH11),1)</f>
+        <f>ROUND(AVERAGE(G11:AJ11),1)</f>
         <v/>
       </c>
       <c r="G11" s="79" t="n">
@@ -12676,11 +12696,11 @@
         <v>0</v>
       </c>
       <c r="E12" s="68">
-        <f>SUM(G12:AH12)</f>
+        <f>SUM(G12:AJ12)</f>
         <v/>
       </c>
       <c r="F12" s="68">
-        <f>ROUND(AVERAGE(G12:AH12),1)</f>
+        <f>ROUND(AVERAGE(G12:AJ12),1)</f>
         <v/>
       </c>
     </row>
@@ -12691,20 +12711,20 @@
         </is>
       </c>
       <c r="B13" s="79" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="79" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" s="68">
-        <f>SUM(G13:AH13)</f>
+        <f>SUM(G13:AJ13)</f>
         <v/>
       </c>
       <c r="F13" s="68">
-        <f>ROUND(AVERAGE(G13:AH13),1)</f>
+        <f>ROUND(AVERAGE(G13:AJ13),1)</f>
         <v/>
       </c>
       <c r="I13" s="79" t="n">
@@ -12730,36 +12750,78 @@
       </c>
       <c r="T13" s="80" t="n">
         <v>1</v>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="79" t="inlineStr">
         <is>
-          <t>fabiovesco</t>
+          <t>Floky23</t>
         </is>
       </c>
       <c r="B14" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D14" s="79" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E14" s="68">
-        <f>SUM(G14:AH14)</f>
+        <f>SUM(G14:AJ14)</f>
         <v/>
       </c>
       <c r="F14" s="68">
-        <f>ROUND(AVERAGE(G14:AH14),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G14:AJ14),1)</f>
+        <v/>
+      </c>
+      <c r="Q14" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R14" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="U14" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V14" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z14" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AE14" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF14" s="80" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="79" t="inlineStr">
         <is>
-          <t>Floky23</t>
+          <t>francesco</t>
         </is>
       </c>
       <c r="B15" s="79" t="n">
@@ -12769,85 +12831,77 @@
         <v>0</v>
       </c>
       <c r="D15" s="79" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="68">
-        <f>SUM(G15:AH15)</f>
+        <f>SUM(G15:AJ15)</f>
         <v/>
       </c>
       <c r="F15" s="68">
-        <f>ROUND(AVERAGE(G15:AH15),1)</f>
-        <v/>
-      </c>
-      <c r="Q15" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R15" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="U15" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V15" s="80" t="n">
-        <v>1</v>
+        <f>ROUND(AVERAGE(G15:AJ15),1)</f>
+        <v/>
       </c>
       <c r="Y15" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z15" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA15" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB15" s="80" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
-      </c>
-      <c r="AE15" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF15" s="80" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="79" t="inlineStr">
         <is>
-          <t>francesco</t>
+          <t>Fryck</t>
         </is>
       </c>
       <c r="B16" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="79" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E16" s="68">
-        <f>SUM(G16:AH16)</f>
+        <f>SUM(G16:AJ16)</f>
         <v/>
       </c>
       <c r="F16" s="68">
-        <f>ROUND(AVERAGE(G16:AH16),1)</f>
+        <f>ROUND(AVERAGE(G16:AJ16),1)</f>
         <v/>
       </c>
       <c r="Y16" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z16" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="Z16" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF16" s="80" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="79" t="inlineStr">
         <is>
-          <t>Fryck</t>
+          <t>gionny</t>
         </is>
       </c>
       <c r="B17" s="79" t="n">
@@ -12857,45 +12911,69 @@
         <v>0</v>
       </c>
       <c r="D17" s="79" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E17" s="68">
-        <f>SUM(G17:AH17)</f>
+        <f>SUM(G17:AJ17)</f>
         <v/>
       </c>
       <c r="F17" s="68">
-        <f>ROUND(AVERAGE(G17:AH17),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G17:AJ17),1)</f>
+        <v/>
+      </c>
+      <c r="G17" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="M17" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="O17" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P17" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U17" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V17" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="W17" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="X17" s="80" t="n">
+        <v>2</v>
       </c>
       <c r="Y17" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z17" s="80" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB17" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD17" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE17" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF17" s="80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="79" t="inlineStr">
         <is>
-          <t>gionny</t>
+          <t>Giorgio</t>
         </is>
       </c>
       <c r="B18" s="79" t="n">
@@ -12905,197 +12983,199 @@
         <v>0</v>
       </c>
       <c r="D18" s="79" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E18" s="68">
-        <f>SUM(G18:AH18)</f>
+        <f>SUM(G18:AJ18)</f>
         <v/>
       </c>
       <c r="F18" s="68">
-        <f>ROUND(AVERAGE(G18:AH18),1)</f>
-        <v/>
-      </c>
-      <c r="G18" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="I18" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M18" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="O18" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P18" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U18" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V18" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W18" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="X18" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y18" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z18" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB18" s="80" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G18:AJ18),1)</f>
+        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="79" t="inlineStr">
         <is>
-          <t>Giorgio</t>
+          <t>GiornoBrando</t>
         </is>
       </c>
       <c r="B19" s="79" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="79" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E19" s="68">
-        <f>SUM(G19:AH19)</f>
+        <f>SUM(G19:AJ19)</f>
         <v/>
       </c>
       <c r="F19" s="68">
-        <f>ROUND(AVERAGE(G19:AH19),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G19:AJ19),1)</f>
+        <v/>
+      </c>
+      <c r="I19" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="J19" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L19" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="O19" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P19" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R19" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U19" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V19" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB19" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC19" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD19" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE19" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF19" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AI19" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ19" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="79" t="inlineStr">
         <is>
-          <t>GiornoBrando</t>
+          <t>GioStyle</t>
         </is>
       </c>
       <c r="B20" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="79" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E20" s="68">
-        <f>SUM(G20:AH20)</f>
+        <f>SUM(G20:AJ20)</f>
         <v/>
       </c>
       <c r="F20" s="68">
-        <f>ROUND(AVERAGE(G20:AH20),1)</f>
-        <v/>
-      </c>
-      <c r="I20" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="J20" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L20" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="O20" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P20" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R20" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U20" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V20" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA20" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB20" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC20" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD20" s="80" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G20:AJ20),1)</f>
+        <v/>
       </c>
       <c r="AE20" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="AF20" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+      <c r="AF20" s="80" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="79" t="inlineStr">
         <is>
-          <t>GioStyle</t>
+          <t>haha</t>
         </is>
       </c>
       <c r="B21" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C21" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="79" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E21" s="68">
-        <f>SUM(G21:AH21)</f>
+        <f>SUM(G21:AJ21)</f>
         <v/>
       </c>
       <c r="F21" s="68">
-        <f>ROUND(AVERAGE(G21:AH21),1)</f>
-        <v/>
-      </c>
-      <c r="AE21" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF21" s="80" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G21:AJ21),1)</f>
+        <v/>
+      </c>
+      <c r="S21" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="T21" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="W21" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X21" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y21" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA21" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB21" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC21" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD21" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI21" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ21" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="79" t="inlineStr">
         <is>
-          <t>haha</t>
+          <t>HikariNoRob</t>
         </is>
       </c>
       <c r="B22" s="79" t="n">
@@ -13105,51 +13185,39 @@
         <v>0</v>
       </c>
       <c r="D22" s="79" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E22" s="68">
-        <f>SUM(G22:AH22)</f>
+        <f>SUM(G22:AJ22)</f>
         <v/>
       </c>
       <c r="F22" s="68">
-        <f>ROUND(AVERAGE(G22:AH22),1)</f>
-        <v/>
-      </c>
-      <c r="S22" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="T22" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W22" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X22" s="80" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G22:AJ22),1)</f>
+        <v/>
+      </c>
+      <c r="G22" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="J22" s="80" t="n">
+        <v>3</v>
       </c>
       <c r="Y22" s="79" t="n">
         <v>3</v>
       </c>
       <c r="Z22" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA22" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB22" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC22" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD22" s="80" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="79" t="inlineStr">
         <is>
-          <t>HikariNoRob</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B23" s="79" t="n">
@@ -13159,130 +13227,160 @@
         <v>0</v>
       </c>
       <c r="D23" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E23" s="68">
-        <f>SUM(G23:AH23)</f>
+        <f>SUM(G23:AJ23)</f>
         <v/>
       </c>
       <c r="F23" s="68">
-        <f>ROUND(AVERAGE(G23:AH23),1)</f>
-        <v/>
-      </c>
-      <c r="G23" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H23" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="I23" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="J23" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y23" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z23" s="80" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G23:AJ23),1)</f>
+        <v/>
+      </c>
+      <c r="AE23" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF23" s="80" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="79" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>Luigi</t>
         </is>
       </c>
       <c r="B24" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C24" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D24" s="79" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E24" s="68">
-        <f>SUM(G24:AH24)</f>
+        <f>SUM(G24:AJ24)</f>
         <v/>
       </c>
       <c r="F24" s="68">
-        <f>ROUND(AVERAGE(G24:AH24),1)</f>
-        <v/>
-      </c>
-      <c r="AE24" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF24" s="80" t="n">
-        <v>1</v>
+        <f>ROUND(AVERAGE(G24:AJ24),1)</f>
+        <v/>
+      </c>
+      <c r="I24" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="J24" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="M24" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="N24" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P24" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="R24" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="W24" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X24" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA24" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB24" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC24" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD24" s="80" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="79" t="inlineStr">
         <is>
-          <t>Luigi</t>
+          <t>Luxor</t>
         </is>
       </c>
       <c r="B25" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="79" t="n">
         <v>7</v>
       </c>
       <c r="E25" s="68">
-        <f>SUM(G25:AH25)</f>
+        <f>SUM(G25:AJ25)</f>
         <v/>
       </c>
       <c r="F25" s="68">
-        <f>ROUND(AVERAGE(G25:AH25),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G25:AJ25),1)</f>
+        <v/>
+      </c>
+      <c r="G25" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="H25" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
       <c r="I25" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="J25" s="80" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="J25" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="K25" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L25" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U25" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V25" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="W25" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X25" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="M25" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="N25" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="O25" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P25" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q25" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="R25" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="W25" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X25" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA25" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB25" s="80" t="n">
-        <v>2</v>
+      <c r="Y25" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z25" s="80" t="n">
+        <v>3</v>
       </c>
       <c r="AC25" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD25" s="80" t="n">
         <v>3</v>
@@ -13291,144 +13389,170 @@
     <row r="26">
       <c r="A26" s="79" t="inlineStr">
         <is>
-          <t>Luxor</t>
+          <t>maikol_lix</t>
         </is>
       </c>
       <c r="B26" s="79" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C26" s="68" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E26" s="68">
-        <f>SUM(G26:AH26)</f>
+        <f>SUM(G26:AJ26)</f>
         <v/>
       </c>
       <c r="F26" s="68">
-        <f>ROUND(AVERAGE(G26:AH26),1)</f>
-        <v/>
-      </c>
-      <c r="G26" s="79" t="inlineStr">
+        <f>ROUND(AVERAGE(G26:AJ26),1)</f>
+        <v/>
+      </c>
+      <c r="G26" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="H26" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="J26" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="O26" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P26" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="H26" s="80" t="inlineStr">
+      <c r="S26" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="T26" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="I26" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="J26" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="K26" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L26" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U26" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V26" s="80" t="n">
-        <v>3</v>
-      </c>
       <c r="W26" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X26" s="80" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="X26" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA26" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB26" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="Y26" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z26" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC26" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD26" s="80" t="n">
-        <v>3</v>
+      <c r="AE26" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF26" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AI26" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ26" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="79" t="inlineStr">
         <is>
-          <t>maikol_lix</t>
+          <t>piegian99</t>
         </is>
       </c>
       <c r="B27" s="79" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C27" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="79" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E27" s="68">
-        <f>SUM(G27:AH27)</f>
+        <f>SUM(G27:AJ27)</f>
         <v/>
       </c>
       <c r="F27" s="68">
-        <f>ROUND(AVERAGE(G27:AH27),1)</f>
+        <f>ROUND(AVERAGE(G27:AJ27),1)</f>
         <v/>
       </c>
       <c r="G27" s="79" t="n">
         <v>3</v>
       </c>
       <c r="H27" s="80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I27" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J27" s="80" t="n">
         <v>3</v>
       </c>
+      <c r="K27" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L27" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="M27" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="N27" s="80" t="n">
+        <v>2</v>
+      </c>
       <c r="O27" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="P27" s="80" t="inlineStr">
+      <c r="P27" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q27" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R27" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="S27" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="T27" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U27" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V27" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE27" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF27" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI27" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="S27" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="T27" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="W27" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X27" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA27" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB27" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AE27" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF27" s="80" t="inlineStr">
+      <c r="AJ27" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
@@ -13437,49 +13561,37 @@
     <row r="28">
       <c r="A28" s="79" t="inlineStr">
         <is>
-          <t>piegian99</t>
+          <t>pigiamone99</t>
         </is>
       </c>
       <c r="B28" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C28" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="79" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E28" s="68">
-        <f>SUM(G28:AH28)</f>
+        <f>SUM(G28:AJ28)</f>
         <v/>
       </c>
       <c r="F28" s="68">
-        <f>ROUND(AVERAGE(G28:AH28),1)</f>
-        <v/>
-      </c>
-      <c r="G28" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="H28" s="80" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G28:AJ28),1)</f>
+        <v/>
       </c>
       <c r="I28" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J28" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="K28" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L28" s="80" t="n">
-        <v>3</v>
-      </c>
       <c r="M28" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N28" s="80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O28" s="79" t="n">
         <v>3</v>
@@ -13493,86 +13605,74 @@
       <c r="R28" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="S28" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="T28" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U28" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V28" s="80" t="n">
+      <c r="W28" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="X28" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y28" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z28" s="80" t="n">
         <v>3</v>
       </c>
       <c r="AE28" s="79" t="n">
         <v>3</v>
       </c>
       <c r="AF28" s="80" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="AI28" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ28" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="79" t="inlineStr">
         <is>
-          <t>pigiamone99</t>
+          <t>PIPPII</t>
         </is>
       </c>
       <c r="B29" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="79" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E29" s="68">
-        <f>SUM(G29:AH29)</f>
+        <f>SUM(G29:AJ29)</f>
         <v/>
       </c>
       <c r="F29" s="68">
-        <f>ROUND(AVERAGE(G29:AH29),1)</f>
-        <v/>
-      </c>
-      <c r="I29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="J29" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="N29" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="O29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P29" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R29" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X29" s="80" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G29:AJ29),1)</f>
+        <v/>
       </c>
       <c r="Y29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z29" s="80" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="Z29" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AC29" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD29" s="80" t="n">
+        <v>2</v>
       </c>
       <c r="AE29" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF29" s="80" t="n">
         <v>3</v>
@@ -13581,51 +13681,81 @@
     <row r="30">
       <c r="A30" s="79" t="inlineStr">
         <is>
-          <t>PIPPII</t>
+          <t>revolver</t>
         </is>
       </c>
       <c r="B30" s="79" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C30" s="68" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" s="79" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E30" s="68">
-        <f>SUM(G30:AH30)</f>
+        <f>SUM(G30:AJ30)</f>
         <v/>
       </c>
       <c r="F30" s="68">
-        <f>ROUND(AVERAGE(G30:AH30),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G30:AJ30),1)</f>
+        <v/>
+      </c>
+      <c r="S30" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="T30" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U30" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="V30" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="W30" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="X30" s="80" t="n">
+        <v>3</v>
       </c>
       <c r="Y30" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z30" s="80" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="Z30" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC30" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD30" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE30" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF30" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI30" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="AC30" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD30" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE30" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF30" s="80" t="n">
-        <v>3</v>
+      <c r="AJ30" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="79" t="inlineStr">
         <is>
-          <t>revolver</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B31" s="79" t="n">
@@ -13635,32 +13765,54 @@
         <v>1</v>
       </c>
       <c r="D31" s="79" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E31" s="68">
-        <f>SUM(G31:AH31)</f>
+        <f>SUM(G31:AJ31)</f>
         <v/>
       </c>
       <c r="F31" s="68">
-        <f>ROUND(AVERAGE(G31:AH31),1)</f>
-        <v/>
-      </c>
-      <c r="S31" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="T31" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U31" s="79" t="inlineStr">
+        <f>ROUND(AVERAGE(G31:AJ31),1)</f>
+        <v/>
+      </c>
+      <c r="I31" s="79" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="V31" s="80" t="inlineStr">
+      <c r="J31" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
+      <c r="K31" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L31" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="M31" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="Q31" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="R31" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
       <c r="W31" s="79" t="n">
         <v>3</v>
       </c>
@@ -13671,117 +13823,55 @@
         <v>3</v>
       </c>
       <c r="Z31" s="80" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="AA31" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB31" s="80" t="n">
+        <v>1</v>
       </c>
       <c r="AC31" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AD31" s="80" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AE31" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF31" s="80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="79" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>Roberta</t>
         </is>
       </c>
       <c r="B32" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C32" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="79" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E32" s="68">
-        <f>SUM(G32:AH32)</f>
+        <f>SUM(G32:AJ32)</f>
         <v/>
       </c>
       <c r="F32" s="68">
-        <f>ROUND(AVERAGE(G32:AH32),1)</f>
-        <v/>
-      </c>
-      <c r="I32" s="79" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="J32" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="K32" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L32" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M32" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="N32" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="O32" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="Q32" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="R32" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="W32" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X32" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y32" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z32" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA32" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB32" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC32" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD32" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE32" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF32" s="80" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G32:AJ32),1)</f>
+        <v/>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="79" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>serra008</t>
         </is>
       </c>
       <c r="B33" s="79" t="n">
@@ -13791,21 +13881,99 @@
         <v>0</v>
       </c>
       <c r="D33" s="79" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E33" s="68">
-        <f>SUM(G33:AH33)</f>
+        <f>SUM(G33:AJ33)</f>
         <v/>
       </c>
       <c r="F33" s="68">
-        <f>ROUND(AVERAGE(G33:AH33),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G33:AJ33),1)</f>
+        <v/>
+      </c>
+      <c r="G33" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="I33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="J33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="K33" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="M33" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="N33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="O33" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="S33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="T33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="W33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="X33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z33" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD33" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF33" s="80" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="79" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B34" s="79" t="n">
@@ -13815,42 +13983,30 @@
         <v>0</v>
       </c>
       <c r="D34" s="79" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E34" s="68">
-        <f>SUM(G34:AH34)</f>
+        <f>SUM(G34:AJ34)</f>
         <v/>
       </c>
       <c r="F34" s="68">
-        <f>ROUND(AVERAGE(G34:AH34),1)</f>
+        <f>ROUND(AVERAGE(G34:AJ34),1)</f>
         <v/>
       </c>
       <c r="G34" s="79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H34" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I34" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J34" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="K34" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="L34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M34" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="N34" s="80" t="n">
-        <v>3</v>
-      </c>
       <c r="O34" s="79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P34" s="80" t="n">
         <v>3</v>
@@ -13859,103 +14015,101 @@
         <v>3</v>
       </c>
       <c r="R34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="S34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="T34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z34" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB34" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD34" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF34" s="80" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="79" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B35" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C35" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="79" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E35" s="68">
-        <f>SUM(G35:AH35)</f>
+        <f>SUM(G35:AJ35)</f>
         <v/>
       </c>
       <c r="F35" s="68">
-        <f>ROUND(AVERAGE(G35:AH35),1)</f>
+        <f>ROUND(AVERAGE(G35:AJ35),1)</f>
         <v/>
       </c>
       <c r="G35" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H35" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I35" s="79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J35" s="80" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="K35" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L35" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="M35" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" s="80" t="n">
+        <v>2</v>
       </c>
       <c r="O35" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P35" s="80" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q35" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R35" s="80" t="n">
         <v>3</v>
+      </c>
+      <c r="U35" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V35" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y35" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z35" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA35" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB35" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI35" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ35" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="79" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B36" s="79" t="n">
@@ -13965,75 +14119,21 @@
         <v>0</v>
       </c>
       <c r="D36" s="79" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E36" s="68">
-        <f>SUM(G36:AH36)</f>
+        <f>SUM(G36:AJ36)</f>
         <v/>
       </c>
       <c r="F36" s="68">
-        <f>ROUND(AVERAGE(G36:AH36),1)</f>
-        <v/>
-      </c>
-      <c r="G36" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="H36" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="I36" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J36" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="K36" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L36" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="M36" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="N36" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="O36" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="P36" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="R36" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U36" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V36" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y36" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z36" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA36" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB36" s="80" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G36:AJ36),1)</f>
+        <v/>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="79" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>tazio</t>
         </is>
       </c>
       <c r="B37" s="79" t="n">
@@ -14046,114 +14146,152 @@
         <v>0</v>
       </c>
       <c r="E37" s="68">
-        <f>SUM(G37:AH37)</f>
+        <f>SUM(G37:AJ37)</f>
         <v/>
       </c>
       <c r="F37" s="68">
-        <f>ROUND(AVERAGE(G37:AH37),1)</f>
+        <f>ROUND(AVERAGE(G37:AJ37),1)</f>
         <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="79" t="inlineStr">
         <is>
-          <t>tazio</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B38" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C38" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="79" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E38" s="68">
-        <f>SUM(G38:AH38)</f>
+        <f>SUM(G38:AJ38)</f>
         <v/>
       </c>
       <c r="F38" s="68">
-        <f>ROUND(AVERAGE(G38:AH38),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G38:AJ38),1)</f>
+        <v/>
+      </c>
+      <c r="O38" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P38" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q38" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R38" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="W38" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X38" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC38" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD38" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE38" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF38" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI38" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ38" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="79" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>Valh</t>
         </is>
       </c>
       <c r="B39" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C39" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="79" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E39" s="68">
-        <f>SUM(G39:AH39)</f>
+        <f>SUM(G39:AJ39)</f>
         <v/>
       </c>
       <c r="F39" s="68">
-        <f>ROUND(AVERAGE(G39:AH39),1)</f>
-        <v/>
-      </c>
-      <c r="O39" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P39" s="80" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G39:AJ39),1)</f>
+        <v/>
+      </c>
+      <c r="K39" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="L39" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
       <c r="Q39" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R39" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="W39" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X39" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC39" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD39" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE39" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF39" s="80" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="79" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B40" s="79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C40" s="68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="79" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E40" s="68">
-        <f>SUM(G40:AH40)</f>
+        <f>SUM(G40:AJ40)</f>
         <v/>
       </c>
       <c r="F40" s="68">
-        <f>ROUND(AVERAGE(G40:AH40),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G40:AJ40),1)</f>
+        <v/>
+      </c>
+      <c r="G40" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="H40" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="I40" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="J40" s="80" t="n">
+        <v>3</v>
       </c>
       <c r="K40" s="79" t="inlineStr">
         <is>
@@ -14165,167 +14303,171 @@
           <t>SKIP</t>
         </is>
       </c>
+      <c r="O40" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P40" s="80" t="n">
+        <v>2</v>
+      </c>
       <c r="Q40" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R40" s="80" t="n">
         <v>3</v>
+      </c>
+      <c r="S40" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="T40" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="W40" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="X40" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y40" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z40" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA40" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB40" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC40" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD40" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI40" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ40" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="79" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B41" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" s="68" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="79" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E41" s="68">
-        <f>SUM(G41:AH41)</f>
+        <f>SUM(G41:AJ41)</f>
         <v/>
       </c>
       <c r="F41" s="68">
-        <f>ROUND(AVERAGE(G41:AH41),1)</f>
-        <v/>
-      </c>
-      <c r="G41" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="H41" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="I41" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="J41" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="K41" s="79" t="inlineStr">
+        <f>ROUND(AVERAGE(G41:AJ41),1)</f>
+        <v/>
+      </c>
+      <c r="U41" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V41" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="W41" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X41" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="L41" s="80" t="inlineStr">
+      <c r="Y41" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z41" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA41" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB41" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC41" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD41" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE41" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF41" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI41" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="O41" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P41" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q41" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R41" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="S41" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="T41" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="W41" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X41" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y41" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z41" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA41" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB41" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC41" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD41" s="80" t="n">
-        <v>3</v>
+      <c r="AJ41" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="79" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B42" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D42" s="79" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E42" s="68">
-        <f>SUM(G42:AH42)</f>
+        <f>SUM(G42:AJ42)</f>
         <v/>
       </c>
       <c r="F42" s="68">
-        <f>ROUND(AVERAGE(G42:AH42),1)</f>
-        <v/>
-      </c>
-      <c r="U42" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V42" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="W42" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X42" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="Y42" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z42" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA42" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB42" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC42" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD42" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE42" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF42" s="80" t="n">
-        <v>2</v>
-      </c>
+        <f>ROUND(AVERAGE(G42:AJ42),1)</f>
+        <v/>
+      </c>
+      <c r="U42" s="79" t="n"/>
+      <c r="V42" s="80" t="n"/>
+      <c r="W42" s="79" t="n"/>
+      <c r="X42" s="80" t="n"/>
+      <c r="Y42" s="79" t="n"/>
+      <c r="Z42" s="80" t="n"/>
+      <c r="AA42" s="79" t="n"/>
+      <c r="AB42" s="80" t="n"/>
+      <c r="AC42" s="79" t="n"/>
+      <c r="AD42" s="80" t="n"/>
+      <c r="AE42" s="79" t="n"/>
+      <c r="AF42" s="80" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="79" t="inlineStr">
         <is>
-          <t>LucFir3</t>
+          <t>Leonida</t>
         </is>
       </c>
       <c r="B43" s="79" t="n">
@@ -14338,11 +14480,11 @@
         <v>0</v>
       </c>
       <c r="E43" s="68">
-        <f>SUM(G43:AH43)</f>
+        <f>SUM(G43:AJ43)</f>
         <v/>
       </c>
       <c r="F43" s="68">
-        <f>ROUND(AVERAGE(G43:AH43),1)</f>
+        <f>ROUND(AVERAGE(G43:AJ43),1)</f>
         <v/>
       </c>
       <c r="U43" s="79" t="n"/>
@@ -14361,24 +14503,24 @@
     <row r="44">
       <c r="A44" s="79" t="inlineStr">
         <is>
-          <t>The_Boff01</t>
+          <t>tuspostati</t>
         </is>
       </c>
       <c r="B44" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C44" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="68">
-        <f>SUM(G44:AH44)</f>
+        <f>SUM(G44:AJ44)</f>
         <v/>
       </c>
       <c r="F44" s="68">
-        <f>ROUND(AVERAGE(G44:AH44),1)</f>
+        <f>ROUND(AVERAGE(G44:AJ44),1)</f>
         <v/>
       </c>
       <c r="U44" s="79" t="n"/>
@@ -14393,11 +14535,21 @@
       <c r="AD44" s="80" t="n"/>
       <c r="AE44" s="79" t="n"/>
       <c r="AF44" s="80" t="n"/>
+      <c r="AI44" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ44" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="79" t="inlineStr">
         <is>
-          <t>Leonida</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B45" s="79" t="n">
@@ -14410,11 +14562,11 @@
         <v>0</v>
       </c>
       <c r="E45" s="68">
-        <f>SUM(G45:AH45)</f>
+        <f>SUM(G45:AJ45)</f>
         <v/>
       </c>
       <c r="F45" s="68">
-        <f>ROUND(AVERAGE(G45:AH45),1)</f>
+        <f>ROUND(AVERAGE(G45:AJ45),1)</f>
         <v/>
       </c>
       <c r="U45" s="79" t="n"/>
@@ -14433,24 +14585,24 @@
     <row r="46">
       <c r="A46" s="79" t="inlineStr">
         <is>
-          <t>tuspostati</t>
+          <t>IL MAGO NERO</t>
         </is>
       </c>
       <c r="B46" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C46" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="68">
-        <f>SUM(G46:AH46)</f>
+        <f>SUM(G46:AJ46)</f>
         <v/>
       </c>
       <c r="F46" s="68">
-        <f>ROUND(AVERAGE(G46:AH46),1)</f>
+        <f>ROUND(AVERAGE(G46:AJ46),1)</f>
         <v/>
       </c>
       <c r="U46" s="79" t="n"/>
@@ -14465,11 +14617,21 @@
       <c r="AD46" s="80" t="n"/>
       <c r="AE46" s="79" t="n"/>
       <c r="AF46" s="80" t="n"/>
+      <c r="AI46" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ46" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="79" t="inlineStr">
         <is>
-          <t>Kle</t>
+          <t>dast</t>
         </is>
       </c>
       <c r="B47" s="79" t="n">
@@ -14482,11 +14644,11 @@
         <v>0</v>
       </c>
       <c r="E47" s="68">
-        <f>SUM(G47:AH47)</f>
+        <f>SUM(G47:AJ47)</f>
         <v/>
       </c>
       <c r="F47" s="68">
-        <f>ROUND(AVERAGE(G47:AH47),1)</f>
+        <f>ROUND(AVERAGE(G47:AJ47),1)</f>
         <v/>
       </c>
       <c r="U47" s="79" t="n"/>
@@ -14505,7 +14667,7 @@
     <row r="48">
       <c r="A48" s="79" t="inlineStr">
         <is>
-          <t>Rixxy</t>
+          <t>NITHING</t>
         </is>
       </c>
       <c r="B48" s="79" t="n">
@@ -14518,11 +14680,11 @@
         <v>0</v>
       </c>
       <c r="E48" s="68">
-        <f>SUM(G48:AH48)</f>
+        <f>SUM(G48:AJ48)</f>
         <v/>
       </c>
       <c r="F48" s="68">
-        <f>ROUND(AVERAGE(G48:AH48),1)</f>
+        <f>ROUND(AVERAGE(G48:AJ48),1)</f>
         <v/>
       </c>
       <c r="U48" s="79" t="n"/>
@@ -14538,78 +14700,6 @@
       <c r="AE48" s="79" t="n"/>
       <c r="AF48" s="80" t="n"/>
     </row>
-    <row r="49">
-      <c r="A49" s="79" t="inlineStr">
-        <is>
-          <t>Killer46</t>
-        </is>
-      </c>
-      <c r="B49" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="68">
-        <f>SUM(G49:AH49)</f>
-        <v/>
-      </c>
-      <c r="F49" s="68">
-        <f>ROUND(AVERAGE(G49:AH49),1)</f>
-        <v/>
-      </c>
-      <c r="U49" s="79" t="n"/>
-      <c r="V49" s="80" t="n"/>
-      <c r="W49" s="79" t="n"/>
-      <c r="X49" s="80" t="n"/>
-      <c r="Y49" s="79" t="n"/>
-      <c r="Z49" s="80" t="n"/>
-      <c r="AA49" s="79" t="n"/>
-      <c r="AB49" s="80" t="n"/>
-      <c r="AC49" s="79" t="n"/>
-      <c r="AD49" s="80" t="n"/>
-      <c r="AE49" s="79" t="n"/>
-      <c r="AF49" s="80" t="n"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="79" t="inlineStr">
-        <is>
-          <t>IL MAGO NERO</t>
-        </is>
-      </c>
-      <c r="B50" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="C50" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="68">
-        <f>SUM(G50:AH50)</f>
-        <v/>
-      </c>
-      <c r="F50" s="68">
-        <f>ROUND(AVERAGE(G50:AH50),1)</f>
-        <v/>
-      </c>
-      <c r="U50" s="79" t="n"/>
-      <c r="V50" s="80" t="n"/>
-      <c r="W50" s="79" t="n"/>
-      <c r="X50" s="80" t="n"/>
-      <c r="Y50" s="79" t="n"/>
-      <c r="Z50" s="80" t="n"/>
-      <c r="AA50" s="79" t="n"/>
-      <c r="AB50" s="80" t="n"/>
-      <c r="AC50" s="79" t="n"/>
-      <c r="AD50" s="80" t="n"/>
-      <c r="AE50" s="79" t="n"/>
-      <c r="AF50" s="80" t="n"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:CL1">
     <sortState ref="A2:CL51">

</xml_diff>

<commit_message>
Update WAR data - 2026-02-01
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -11632,7 +11632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI48"/>
+  <dimension ref="A1:CI51"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -11879,12 +11879,12 @@
       </c>
       <c r="AK1" s="107" t="inlineStr">
         <is>
-          <t>Colonna37</t>
+          <t>WAR-16 (1)</t>
         </is>
       </c>
       <c r="AL1" s="112" t="inlineStr">
         <is>
-          <t>Colonna38</t>
+          <t>WAR-16 (2)</t>
         </is>
       </c>
       <c r="AM1" s="107" t="inlineStr">
@@ -12149,11 +12149,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="111">
-        <f>SUM(G2:AJ2)</f>
+        <f>SUM(G2:AL2)</f>
         <v/>
       </c>
       <c r="F2" s="68">
-        <f>ROUND(AVERAGE(G2:AJ2),1)</f>
+        <f>ROUND(AVERAGE(G2:AL2),1)</f>
         <v/>
       </c>
       <c r="G2" s="110" t="n"/>
@@ -12268,11 +12268,11 @@
         <v>0</v>
       </c>
       <c r="E3" s="68">
-        <f>SUM(G3:AJ3)</f>
+        <f>SUM(G3:AL3)</f>
         <v/>
       </c>
       <c r="F3" s="68">
-        <f>ROUND(AVERAGE(G3:AJ3),1)</f>
+        <f>ROUND(AVERAGE(G3:AL3),1)</f>
         <v/>
       </c>
     </row>
@@ -12289,14 +12289,14 @@
         <v>1</v>
       </c>
       <c r="D4" s="79" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="68">
-        <f>SUM(G4:AJ4)</f>
+        <f>SUM(G4:AL4)</f>
         <v/>
       </c>
       <c r="F4" s="68">
-        <f>ROUND(AVERAGE(G4:AJ4),1)</f>
+        <f>ROUND(AVERAGE(G4:AL4),1)</f>
         <v/>
       </c>
       <c r="I4" s="79" t="n">
@@ -12320,6 +12320,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -12338,11 +12344,11 @@
         <v>0</v>
       </c>
       <c r="E5" s="68">
-        <f>SUM(G5:AJ5)</f>
+        <f>SUM(G5:AL5)</f>
         <v/>
       </c>
       <c r="F5" s="68">
-        <f>ROUND(AVERAGE(G5:AJ5),1)</f>
+        <f>ROUND(AVERAGE(G5:AL5),1)</f>
         <v/>
       </c>
     </row>
@@ -12362,11 +12368,11 @@
         <v>0</v>
       </c>
       <c r="E6" s="68">
-        <f>SUM(G6:AJ6)</f>
+        <f>SUM(G6:AL6)</f>
         <v/>
       </c>
       <c r="F6" s="68">
-        <f>ROUND(AVERAGE(G6:AJ6),1)</f>
+        <f>ROUND(AVERAGE(G6:AL6),1)</f>
         <v/>
       </c>
     </row>
@@ -12386,11 +12392,11 @@
         <v>3</v>
       </c>
       <c r="E7" s="68">
-        <f>SUM(G7:AJ7)</f>
+        <f>SUM(G7:AL7)</f>
         <v/>
       </c>
       <c r="F7" s="68">
-        <f>ROUND(AVERAGE(G7:AJ7),1)</f>
+        <f>ROUND(AVERAGE(G7:AL7),1)</f>
         <v/>
       </c>
       <c r="U7" s="79" t="n">
@@ -12419,20 +12425,20 @@
         </is>
       </c>
       <c r="B8" s="79" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="68" t="n">
         <v>4</v>
       </c>
       <c r="D8" s="79" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="68">
-        <f>SUM(G8:AJ8)</f>
+        <f>SUM(G8:AL8)</f>
         <v/>
       </c>
       <c r="F8" s="68">
-        <f>ROUND(AVERAGE(G8:AJ8),1)</f>
+        <f>ROUND(AVERAGE(G8:AL8),1)</f>
         <v/>
       </c>
       <c r="G8" s="79" t="n">
@@ -12513,6 +12519,14 @@
         </is>
       </c>
       <c r="AJ8" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL8" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
@@ -12534,11 +12548,11 @@
         <v>4</v>
       </c>
       <c r="E9" s="68">
-        <f>SUM(G9:AJ9)</f>
+        <f>SUM(G9:AL9)</f>
         <v/>
       </c>
       <c r="F9" s="68">
-        <f>ROUND(AVERAGE(G9:AJ9),1)</f>
+        <f>ROUND(AVERAGE(G9:AL9),1)</f>
         <v/>
       </c>
       <c r="K9" s="79" t="n">
@@ -12582,11 +12596,11 @@
         <v>0</v>
       </c>
       <c r="E10" s="68">
-        <f>SUM(G10:AJ10)</f>
+        <f>SUM(G10:AL10)</f>
         <v/>
       </c>
       <c r="F10" s="68">
-        <f>ROUND(AVERAGE(G10:AJ10),1)</f>
+        <f>ROUND(AVERAGE(G10:AL10),1)</f>
         <v/>
       </c>
     </row>
@@ -12606,11 +12620,11 @@
         <v>11</v>
       </c>
       <c r="E11" s="68">
-        <f>SUM(G11:AJ11)</f>
+        <f>SUM(G11:AL11)</f>
         <v/>
       </c>
       <c r="F11" s="68">
-        <f>ROUND(AVERAGE(G11:AJ11),1)</f>
+        <f>ROUND(AVERAGE(G11:AL11),1)</f>
         <v/>
       </c>
       <c r="G11" s="79" t="n">
@@ -12696,11 +12710,11 @@
         <v>0</v>
       </c>
       <c r="E12" s="68">
-        <f>SUM(G12:AJ12)</f>
+        <f>SUM(G12:AL12)</f>
         <v/>
       </c>
       <c r="F12" s="68">
-        <f>ROUND(AVERAGE(G12:AJ12),1)</f>
+        <f>ROUND(AVERAGE(G12:AL12),1)</f>
         <v/>
       </c>
     </row>
@@ -12717,14 +12731,14 @@
         <v>2</v>
       </c>
       <c r="D13" s="79" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" s="68">
-        <f>SUM(G13:AJ13)</f>
+        <f>SUM(G13:AL13)</f>
         <v/>
       </c>
       <c r="F13" s="68">
-        <f>ROUND(AVERAGE(G13:AJ13),1)</f>
+        <f>ROUND(AVERAGE(G13:AL13),1)</f>
         <v/>
       </c>
       <c r="I13" s="79" t="n">
@@ -12760,6 +12774,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -12778,11 +12798,11 @@
         <v>5</v>
       </c>
       <c r="E14" s="68">
-        <f>SUM(G14:AJ14)</f>
+        <f>SUM(G14:AL14)</f>
         <v/>
       </c>
       <c r="F14" s="68">
-        <f>ROUND(AVERAGE(G14:AJ14),1)</f>
+        <f>ROUND(AVERAGE(G14:AL14),1)</f>
         <v/>
       </c>
       <c r="Q14" s="79" t="n">
@@ -12834,11 +12854,11 @@
         <v>1</v>
       </c>
       <c r="E15" s="68">
-        <f>SUM(G15:AJ15)</f>
+        <f>SUM(G15:AL15)</f>
         <v/>
       </c>
       <c r="F15" s="68">
-        <f>ROUND(AVERAGE(G15:AJ15),1)</f>
+        <f>ROUND(AVERAGE(G15:AL15),1)</f>
         <v/>
       </c>
       <c r="Y15" s="79" t="n">
@@ -12866,11 +12886,11 @@
         <v>4</v>
       </c>
       <c r="E16" s="68">
-        <f>SUM(G16:AJ16)</f>
+        <f>SUM(G16:AL16)</f>
         <v/>
       </c>
       <c r="F16" s="68">
-        <f>ROUND(AVERAGE(G16:AJ16),1)</f>
+        <f>ROUND(AVERAGE(G16:AL16),1)</f>
         <v/>
       </c>
       <c r="Y16" s="79" t="n">
@@ -12914,11 +12934,11 @@
         <v>8</v>
       </c>
       <c r="E17" s="68">
-        <f>SUM(G17:AJ17)</f>
+        <f>SUM(G17:AL17)</f>
         <v/>
       </c>
       <c r="F17" s="68">
-        <f>ROUND(AVERAGE(G17:AJ17),1)</f>
+        <f>ROUND(AVERAGE(G17:AL17),1)</f>
         <v/>
       </c>
       <c r="G17" s="79" t="n">
@@ -12986,11 +13006,11 @@
         <v>0</v>
       </c>
       <c r="E18" s="68">
-        <f>SUM(G18:AJ18)</f>
+        <f>SUM(G18:AL18)</f>
         <v/>
       </c>
       <c r="F18" s="68">
-        <f>ROUND(AVERAGE(G18:AJ18),1)</f>
+        <f>ROUND(AVERAGE(G18:AL18),1)</f>
         <v/>
       </c>
     </row>
@@ -13007,14 +13027,14 @@
         <v>1</v>
       </c>
       <c r="D19" s="79" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19" s="68">
-        <f>SUM(G19:AJ19)</f>
+        <f>SUM(G19:AL19)</f>
         <v/>
       </c>
       <c r="F19" s="68">
-        <f>ROUND(AVERAGE(G19:AJ19),1)</f>
+        <f>ROUND(AVERAGE(G19:AL19),1)</f>
         <v/>
       </c>
       <c r="I19" s="79" t="n">
@@ -13076,6 +13096,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK19" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -13094,11 +13120,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="68">
-        <f>SUM(G20:AJ20)</f>
+        <f>SUM(G20:AL20)</f>
         <v/>
       </c>
       <c r="F20" s="68">
-        <f>ROUND(AVERAGE(G20:AJ20),1)</f>
+        <f>ROUND(AVERAGE(G20:AL20),1)</f>
         <v/>
       </c>
       <c r="AE20" s="79" t="n">
@@ -13121,14 +13147,14 @@
         <v>1</v>
       </c>
       <c r="D21" s="79" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" s="68">
-        <f>SUM(G21:AJ21)</f>
+        <f>SUM(G21:AL21)</f>
         <v/>
       </c>
       <c r="F21" s="68">
-        <f>ROUND(AVERAGE(G21:AJ21),1)</f>
+        <f>ROUND(AVERAGE(G21:AL21),1)</f>
         <v/>
       </c>
       <c r="S21" s="79" t="n">
@@ -13170,6 +13196,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -13188,11 +13220,11 @@
         <v>3</v>
       </c>
       <c r="E22" s="68">
-        <f>SUM(G22:AJ22)</f>
+        <f>SUM(G22:AL22)</f>
         <v/>
       </c>
       <c r="F22" s="68">
-        <f>ROUND(AVERAGE(G22:AJ22),1)</f>
+        <f>ROUND(AVERAGE(G22:AL22),1)</f>
         <v/>
       </c>
       <c r="G22" s="79" t="n">
@@ -13230,11 +13262,11 @@
         <v>1</v>
       </c>
       <c r="E23" s="68">
-        <f>SUM(G23:AJ23)</f>
+        <f>SUM(G23:AL23)</f>
         <v/>
       </c>
       <c r="F23" s="68">
-        <f>ROUND(AVERAGE(G23:AJ23),1)</f>
+        <f>ROUND(AVERAGE(G23:AL23),1)</f>
         <v/>
       </c>
       <c r="AE23" s="79" t="n">
@@ -13260,11 +13292,11 @@
         <v>7</v>
       </c>
       <c r="E24" s="68">
-        <f>SUM(G24:AJ24)</f>
+        <f>SUM(G24:AL24)</f>
         <v/>
       </c>
       <c r="F24" s="68">
-        <f>ROUND(AVERAGE(G24:AJ24),1)</f>
+        <f>ROUND(AVERAGE(G24:AL24),1)</f>
         <v/>
       </c>
       <c r="I24" s="79" t="n">
@@ -13330,11 +13362,11 @@
         <v>7</v>
       </c>
       <c r="E25" s="68">
-        <f>SUM(G25:AJ25)</f>
+        <f>SUM(G25:AL25)</f>
         <v/>
       </c>
       <c r="F25" s="68">
-        <f>ROUND(AVERAGE(G25:AJ25),1)</f>
+        <f>ROUND(AVERAGE(G25:AL25),1)</f>
         <v/>
       </c>
       <c r="G25" s="79" t="inlineStr">
@@ -13399,14 +13431,14 @@
         <v>1</v>
       </c>
       <c r="D26" s="79" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E26" s="68">
-        <f>SUM(G26:AJ26)</f>
+        <f>SUM(G26:AL26)</f>
         <v/>
       </c>
       <c r="F26" s="68">
-        <f>ROUND(AVERAGE(G26:AJ26),1)</f>
+        <f>ROUND(AVERAGE(G26:AL26),1)</f>
         <v/>
       </c>
       <c r="G26" s="79" t="n">
@@ -13468,6 +13500,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK26" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -13483,14 +13521,14 @@
         <v>1</v>
       </c>
       <c r="D27" s="79" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E27" s="68">
-        <f>SUM(G27:AJ27)</f>
+        <f>SUM(G27:AL27)</f>
         <v/>
       </c>
       <c r="F27" s="68">
-        <f>ROUND(AVERAGE(G27:AJ27),1)</f>
+        <f>ROUND(AVERAGE(G27:AL27),1)</f>
         <v/>
       </c>
       <c r="G27" s="79" t="n">
@@ -13556,6 +13594,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK27" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -13571,14 +13615,14 @@
         <v>1</v>
       </c>
       <c r="D28" s="79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E28" s="68">
-        <f>SUM(G28:AJ28)</f>
+        <f>SUM(G28:AL28)</f>
         <v/>
       </c>
       <c r="F28" s="68">
-        <f>ROUND(AVERAGE(G28:AJ28),1)</f>
+        <f>ROUND(AVERAGE(G28:AL28),1)</f>
         <v/>
       </c>
       <c r="I28" s="79" t="n">
@@ -13632,6 +13676,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -13650,11 +13700,11 @@
         <v>3</v>
       </c>
       <c r="E29" s="68">
-        <f>SUM(G29:AJ29)</f>
+        <f>SUM(G29:AL29)</f>
         <v/>
       </c>
       <c r="F29" s="68">
-        <f>ROUND(AVERAGE(G29:AJ29),1)</f>
+        <f>ROUND(AVERAGE(G29:AL29),1)</f>
         <v/>
       </c>
       <c r="Y29" s="79" t="n">
@@ -13685,20 +13735,20 @@
         </is>
       </c>
       <c r="B30" s="79" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" s="68" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E30" s="68">
-        <f>SUM(G30:AJ30)</f>
+        <f>SUM(G30:AL30)</f>
         <v/>
       </c>
       <c r="F30" s="68">
-        <f>ROUND(AVERAGE(G30:AJ30),1)</f>
+        <f>ROUND(AVERAGE(G30:AL30),1)</f>
         <v/>
       </c>
       <c r="S30" s="79" t="n">
@@ -13747,6 +13797,14 @@
         </is>
       </c>
       <c r="AJ30" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL30" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
@@ -13768,11 +13826,11 @@
         <v>9</v>
       </c>
       <c r="E31" s="68">
-        <f>SUM(G31:AJ31)</f>
+        <f>SUM(G31:AL31)</f>
         <v/>
       </c>
       <c r="F31" s="68">
-        <f>ROUND(AVERAGE(G31:AJ31),1)</f>
+        <f>ROUND(AVERAGE(G31:AL31),1)</f>
         <v/>
       </c>
       <c r="I31" s="79" t="inlineStr">
@@ -13860,11 +13918,11 @@
         <v>0</v>
       </c>
       <c r="E32" s="68">
-        <f>SUM(G32:AJ32)</f>
+        <f>SUM(G32:AL32)</f>
         <v/>
       </c>
       <c r="F32" s="68">
-        <f>ROUND(AVERAGE(G32:AJ32),1)</f>
+        <f>ROUND(AVERAGE(G32:AL32),1)</f>
         <v/>
       </c>
     </row>
@@ -13884,11 +13942,11 @@
         <v>13</v>
       </c>
       <c r="E33" s="68">
-        <f>SUM(G33:AJ33)</f>
+        <f>SUM(G33:AL33)</f>
         <v/>
       </c>
       <c r="F33" s="68">
-        <f>ROUND(AVERAGE(G33:AJ33),1)</f>
+        <f>ROUND(AVERAGE(G33:AL33),1)</f>
         <v/>
       </c>
       <c r="G33" s="79" t="n">
@@ -13986,11 +14044,11 @@
         <v>4</v>
       </c>
       <c r="E34" s="68">
-        <f>SUM(G34:AJ34)</f>
+        <f>SUM(G34:AL34)</f>
         <v/>
       </c>
       <c r="F34" s="68">
-        <f>ROUND(AVERAGE(G34:AJ34),1)</f>
+        <f>ROUND(AVERAGE(G34:AL34),1)</f>
         <v/>
       </c>
       <c r="G34" s="79" t="n">
@@ -14031,14 +14089,14 @@
         <v>1</v>
       </c>
       <c r="D35" s="79" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E35" s="68">
-        <f>SUM(G35:AJ35)</f>
+        <f>SUM(G35:AL35)</f>
         <v/>
       </c>
       <c r="F35" s="68">
-        <f>ROUND(AVERAGE(G35:AJ35),1)</f>
+        <f>ROUND(AVERAGE(G35:AL35),1)</f>
         <v/>
       </c>
       <c r="G35" s="79" t="n">
@@ -14104,6 +14162,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK35" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="36">
@@ -14122,11 +14186,11 @@
         <v>0</v>
       </c>
       <c r="E36" s="68">
-        <f>SUM(G36:AJ36)</f>
+        <f>SUM(G36:AL36)</f>
         <v/>
       </c>
       <c r="F36" s="68">
-        <f>ROUND(AVERAGE(G36:AJ36),1)</f>
+        <f>ROUND(AVERAGE(G36:AL36),1)</f>
         <v/>
       </c>
     </row>
@@ -14146,11 +14210,11 @@
         <v>0</v>
       </c>
       <c r="E37" s="68">
-        <f>SUM(G37:AJ37)</f>
+        <f>SUM(G37:AL37)</f>
         <v/>
       </c>
       <c r="F37" s="68">
-        <f>ROUND(AVERAGE(G37:AJ37),1)</f>
+        <f>ROUND(AVERAGE(G37:AL37),1)</f>
         <v/>
       </c>
     </row>
@@ -14167,14 +14231,14 @@
         <v>1</v>
       </c>
       <c r="D38" s="79" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E38" s="68">
-        <f>SUM(G38:AJ38)</f>
+        <f>SUM(G38:AL38)</f>
         <v/>
       </c>
       <c r="F38" s="68">
-        <f>ROUND(AVERAGE(G38:AJ38),1)</f>
+        <f>ROUND(AVERAGE(G38:AL38),1)</f>
         <v/>
       </c>
       <c r="O38" s="79" t="n">
@@ -14216,6 +14280,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK38" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL38" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -14234,11 +14304,11 @@
         <v>2</v>
       </c>
       <c r="E39" s="68">
-        <f>SUM(G39:AJ39)</f>
+        <f>SUM(G39:AL39)</f>
         <v/>
       </c>
       <c r="F39" s="68">
-        <f>ROUND(AVERAGE(G39:AJ39),1)</f>
+        <f>ROUND(AVERAGE(G39:AL39),1)</f>
         <v/>
       </c>
       <c r="K39" s="79" t="inlineStr">
@@ -14271,14 +14341,14 @@
         <v>2</v>
       </c>
       <c r="D40" s="79" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E40" s="68">
-        <f>SUM(G40:AJ40)</f>
+        <f>SUM(G40:AL40)</f>
         <v/>
       </c>
       <c r="F40" s="68">
-        <f>ROUND(AVERAGE(G40:AJ40),1)</f>
+        <f>ROUND(AVERAGE(G40:AL40),1)</f>
         <v/>
       </c>
       <c r="G40" s="79" t="n">
@@ -14354,6 +14424,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AK40" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL40" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="41">
@@ -14363,20 +14439,20 @@
         </is>
       </c>
       <c r="B41" s="79" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41" s="68" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E41" s="68">
-        <f>SUM(G41:AJ41)</f>
+        <f>SUM(G41:AL41)</f>
         <v/>
       </c>
       <c r="F41" s="68">
-        <f>ROUND(AVERAGE(G41:AJ41),1)</f>
+        <f>ROUND(AVERAGE(G41:AL41),1)</f>
         <v/>
       </c>
       <c r="U41" s="79" t="n">
@@ -14423,6 +14499,14 @@
         </is>
       </c>
       <c r="AJ41" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK41" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL41" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
@@ -14444,11 +14528,11 @@
         <v>0</v>
       </c>
       <c r="E42" s="68">
-        <f>SUM(G42:AJ42)</f>
+        <f>SUM(G42:AL42)</f>
         <v/>
       </c>
       <c r="F42" s="68">
-        <f>ROUND(AVERAGE(G42:AJ42),1)</f>
+        <f>ROUND(AVERAGE(G42:AL42),1)</f>
         <v/>
       </c>
       <c r="U42" s="79" t="n"/>
@@ -14480,11 +14564,11 @@
         <v>0</v>
       </c>
       <c r="E43" s="68">
-        <f>SUM(G43:AJ43)</f>
+        <f>SUM(G43:AL43)</f>
         <v/>
       </c>
       <c r="F43" s="68">
-        <f>ROUND(AVERAGE(G43:AJ43),1)</f>
+        <f>ROUND(AVERAGE(G43:AL43),1)</f>
         <v/>
       </c>
       <c r="U43" s="79" t="n"/>
@@ -14507,20 +14591,20 @@
         </is>
       </c>
       <c r="B44" s="79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C44" s="68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" s="79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="68">
-        <f>SUM(G44:AJ44)</f>
+        <f>SUM(G44:AL44)</f>
         <v/>
       </c>
       <c r="F44" s="68">
-        <f>ROUND(AVERAGE(G44:AJ44),1)</f>
+        <f>ROUND(AVERAGE(G44:AL44),1)</f>
         <v/>
       </c>
       <c r="U44" s="79" t="n"/>
@@ -14545,6 +14629,16 @@
           <t>SKIP</t>
         </is>
       </c>
+      <c r="AK44" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AL44" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="79" t="inlineStr">
@@ -14562,11 +14656,11 @@
         <v>0</v>
       </c>
       <c r="E45" s="68">
-        <f>SUM(G45:AJ45)</f>
+        <f>SUM(G45:AL45)</f>
         <v/>
       </c>
       <c r="F45" s="68">
-        <f>ROUND(AVERAGE(G45:AJ45),1)</f>
+        <f>ROUND(AVERAGE(G45:AL45),1)</f>
         <v/>
       </c>
       <c r="U45" s="79" t="n"/>
@@ -14589,20 +14683,20 @@
         </is>
       </c>
       <c r="B46" s="79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C46" s="68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" s="79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46" s="68">
-        <f>SUM(G46:AJ46)</f>
+        <f>SUM(G46:AL46)</f>
         <v/>
       </c>
       <c r="F46" s="68">
-        <f>ROUND(AVERAGE(G46:AJ46),1)</f>
+        <f>ROUND(AVERAGE(G46:AL46),1)</f>
         <v/>
       </c>
       <c r="U46" s="79" t="n"/>
@@ -14627,6 +14721,16 @@
           <t>SKIP</t>
         </is>
       </c>
+      <c r="AK46" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AL46" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="79" t="inlineStr">
@@ -14644,11 +14748,11 @@
         <v>0</v>
       </c>
       <c r="E47" s="68">
-        <f>SUM(G47:AJ47)</f>
+        <f>SUM(G47:AL47)</f>
         <v/>
       </c>
       <c r="F47" s="68">
-        <f>ROUND(AVERAGE(G47:AJ47),1)</f>
+        <f>ROUND(AVERAGE(G47:AL47),1)</f>
         <v/>
       </c>
       <c r="U47" s="79" t="n"/>
@@ -14680,11 +14784,11 @@
         <v>0</v>
       </c>
       <c r="E48" s="68">
-        <f>SUM(G48:AJ48)</f>
+        <f>SUM(G48:AL48)</f>
         <v/>
       </c>
       <c r="F48" s="68">
-        <f>ROUND(AVERAGE(G48:AJ48),1)</f>
+        <f>ROUND(AVERAGE(G48:AL48),1)</f>
         <v/>
       </c>
       <c r="U48" s="79" t="n"/>
@@ -14700,6 +14804,114 @@
       <c r="AE48" s="79" t="n"/>
       <c r="AF48" s="80" t="n"/>
     </row>
+    <row r="49">
+      <c r="A49" s="79" t="inlineStr">
+        <is>
+          <t>Darvix27</t>
+        </is>
+      </c>
+      <c r="B49" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="68">
+        <f>SUM(G49:AL49)</f>
+        <v/>
+      </c>
+      <c r="F49" s="68">
+        <f>ROUND(AVERAGE(G49:AL49),1)</f>
+        <v/>
+      </c>
+      <c r="U49" s="79" t="n"/>
+      <c r="V49" s="80" t="n"/>
+      <c r="W49" s="79" t="n"/>
+      <c r="X49" s="80" t="n"/>
+      <c r="Y49" s="79" t="n"/>
+      <c r="Z49" s="80" t="n"/>
+      <c r="AA49" s="79" t="n"/>
+      <c r="AB49" s="80" t="n"/>
+      <c r="AC49" s="79" t="n"/>
+      <c r="AD49" s="80" t="n"/>
+      <c r="AE49" s="79" t="n"/>
+      <c r="AF49" s="80" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="79" t="inlineStr">
+        <is>
+          <t>Diti</t>
+        </is>
+      </c>
+      <c r="B50" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="68">
+        <f>SUM(G50:AL50)</f>
+        <v/>
+      </c>
+      <c r="F50" s="68">
+        <f>ROUND(AVERAGE(G50:AL50),1)</f>
+        <v/>
+      </c>
+      <c r="U50" s="79" t="n"/>
+      <c r="V50" s="80" t="n"/>
+      <c r="W50" s="79" t="n"/>
+      <c r="X50" s="80" t="n"/>
+      <c r="Y50" s="79" t="n"/>
+      <c r="Z50" s="80" t="n"/>
+      <c r="AA50" s="79" t="n"/>
+      <c r="AB50" s="80" t="n"/>
+      <c r="AC50" s="79" t="n"/>
+      <c r="AD50" s="80" t="n"/>
+      <c r="AE50" s="79" t="n"/>
+      <c r="AF50" s="80" t="n"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="79" t="inlineStr">
+        <is>
+          <t>K A N E K I</t>
+        </is>
+      </c>
+      <c r="B51" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="68">
+        <f>SUM(G51:AL51)</f>
+        <v/>
+      </c>
+      <c r="F51" s="68">
+        <f>ROUND(AVERAGE(G51:AL51),1)</f>
+        <v/>
+      </c>
+      <c r="U51" s="79" t="n"/>
+      <c r="V51" s="80" t="n"/>
+      <c r="W51" s="79" t="n"/>
+      <c r="X51" s="80" t="n"/>
+      <c r="Y51" s="79" t="n"/>
+      <c r="Z51" s="80" t="n"/>
+      <c r="AA51" s="79" t="n"/>
+      <c r="AB51" s="80" t="n"/>
+      <c r="AC51" s="79" t="n"/>
+      <c r="AD51" s="80" t="n"/>
+      <c r="AE51" s="79" t="n"/>
+      <c r="AF51" s="80" t="n"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:CL1">
     <sortState ref="A2:CL51">

</xml_diff>

<commit_message>
updated clan capital yaml and different excels
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piegi\Documents\GitHub\clashMacacos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B7D7F1-E1D2-4B04-8B76-AE28AFAC2B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC5C51D-B9C9-4494-8E88-D19ED69CC904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -861,7 +861,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -991,6 +991,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1163,7 +1169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1503,9 +1509,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1527,6 +1530,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3892,41 +3901,41 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="61"/>
-      <c r="C1" s="122">
-        <v>1</v>
-      </c>
-      <c r="D1" s="123"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="122">
-        <v>2</v>
-      </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="122">
-        <v>3</v>
-      </c>
-      <c r="J1" s="123"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="122">
+      <c r="C1" s="121">
+        <v>1</v>
+      </c>
+      <c r="D1" s="122"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="121">
+        <v>2</v>
+      </c>
+      <c r="G1" s="122"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="121">
+        <v>3</v>
+      </c>
+      <c r="J1" s="122"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="121">
         <v>4</v>
       </c>
-      <c r="M1" s="123"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="122">
+      <c r="M1" s="122"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="121">
         <v>5</v>
       </c>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="122">
+      <c r="P1" s="122"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="121">
         <v>6</v>
       </c>
-      <c r="S1" s="123"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="122">
+      <c r="S1" s="122"/>
+      <c r="T1" s="123"/>
+      <c r="U1" s="121">
         <v>7</v>
       </c>
-      <c r="V1" s="123"/>
-      <c r="W1" s="124"/>
+      <c r="V1" s="122"/>
+      <c r="W1" s="123"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36"/>
@@ -6100,41 +6109,41 @@
     <row r="1" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39"/>
       <c r="B1" s="61"/>
-      <c r="C1" s="122">
-        <v>1</v>
-      </c>
-      <c r="D1" s="123"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="122">
-        <v>2</v>
-      </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="122">
-        <v>3</v>
-      </c>
-      <c r="J1" s="123"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="122">
+      <c r="C1" s="121">
+        <v>1</v>
+      </c>
+      <c r="D1" s="122"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="121">
+        <v>2</v>
+      </c>
+      <c r="G1" s="122"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="121">
+        <v>3</v>
+      </c>
+      <c r="J1" s="122"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="121">
         <v>4</v>
       </c>
-      <c r="M1" s="123"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="122">
+      <c r="M1" s="122"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="121">
         <v>5</v>
       </c>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="122">
+      <c r="P1" s="122"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="121">
         <v>6</v>
       </c>
-      <c r="S1" s="123"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="122">
+      <c r="S1" s="122"/>
+      <c r="T1" s="123"/>
+      <c r="U1" s="121">
         <v>7</v>
       </c>
-      <c r="V1" s="123"/>
-      <c r="W1" s="124"/>
+      <c r="V1" s="122"/>
+      <c r="W1" s="123"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36"/>
@@ -8423,56 +8432,56 @@
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.7109375" style="93" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="116"/>
-    <col min="11" max="11" width="9.140625" style="117"/>
-    <col min="12" max="12" width="9.140625" style="116"/>
-    <col min="14" max="14" width="9.140625" style="117"/>
+    <col min="9" max="9" width="9.140625" style="115"/>
+    <col min="11" max="11" width="9.140625" style="116"/>
+    <col min="12" max="12" width="9.140625" style="115"/>
+    <col min="14" max="14" width="9.140625" style="116"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39"/>
       <c r="B1" s="61"/>
-      <c r="C1" s="122">
-        <v>1</v>
-      </c>
-      <c r="D1" s="123"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="122">
-        <v>2</v>
-      </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="122">
-        <v>3</v>
-      </c>
-      <c r="J1" s="123"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="122">
+      <c r="C1" s="121">
+        <v>1</v>
+      </c>
+      <c r="D1" s="122"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="121">
+        <v>2</v>
+      </c>
+      <c r="G1" s="122"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="121">
+        <v>3</v>
+      </c>
+      <c r="J1" s="122"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="121">
         <v>4</v>
       </c>
-      <c r="M1" s="123"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="122">
+      <c r="M1" s="122"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="121">
         <v>5</v>
       </c>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="122">
+      <c r="P1" s="122"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="121">
         <v>6</v>
       </c>
-      <c r="S1" s="123"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="122">
+      <c r="S1" s="122"/>
+      <c r="T1" s="123"/>
+      <c r="U1" s="121">
         <v>7</v>
       </c>
-      <c r="V1" s="123"/>
-      <c r="W1" s="124"/>
+      <c r="V1" s="122"/>
+      <c r="W1" s="123"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36"/>
@@ -8558,8 +8567,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="40"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="G3" s="125">
+        <v>1</v>
+      </c>
+      <c r="H3" s="39">
+        <v>3</v>
+      </c>
       <c r="I3" s="40"/>
       <c r="J3" s="39"/>
       <c r="K3" s="41"/>
@@ -8590,9 +8603,15 @@
       <c r="E4" s="41">
         <v>2</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="F4" s="40">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="39">
+        <v>0</v>
+      </c>
+      <c r="H4" s="39">
+        <v>3</v>
+      </c>
       <c r="I4" s="40"/>
       <c r="J4" s="39"/>
       <c r="K4" s="41"/>
@@ -8613,19 +8632,23 @@
       <c r="A5" s="39">
         <v>14</v>
       </c>
-      <c r="B5" s="119" t="s">
+      <c r="B5" s="118" t="s">
         <v>255</v>
       </c>
       <c r="C5" s="39"/>
-      <c r="D5" s="118">
+      <c r="D5" s="117">
         <v>1</v>
       </c>
       <c r="E5" s="41">
         <v>3</v>
       </c>
       <c r="F5" s="40"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="G5" s="125">
+        <v>1</v>
+      </c>
+      <c r="H5" s="39">
+        <v>3</v>
+      </c>
       <c r="I5" s="40"/>
       <c r="J5" s="39"/>
       <c r="K5" s="41"/>
@@ -8657,8 +8680,12 @@
         <v>2</v>
       </c>
       <c r="F6" s="40"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="G6" s="39">
+        <v>1</v>
+      </c>
+      <c r="H6" s="39">
+        <v>2</v>
+      </c>
       <c r="I6" s="40"/>
       <c r="J6" s="39"/>
       <c r="K6" s="41"/>
@@ -8690,8 +8717,12 @@
         <v>2</v>
       </c>
       <c r="F7" s="40"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="G7" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="39">
+        <v>3</v>
+      </c>
       <c r="I7" s="40"/>
       <c r="J7" s="39"/>
       <c r="K7" s="41"/>
@@ -8723,8 +8754,12 @@
         <v>3</v>
       </c>
       <c r="F8" s="40"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+      <c r="G8" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="39">
+        <v>3</v>
+      </c>
       <c r="I8" s="40"/>
       <c r="J8" s="39"/>
       <c r="K8" s="41"/>
@@ -8756,7 +8791,9 @@
         <v>3</v>
       </c>
       <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
+      <c r="G9" s="39">
+        <v>-1</v>
+      </c>
       <c r="H9" s="39">
         <v>3</v>
       </c>
@@ -8780,7 +8817,7 @@
       <c r="A10" s="39">
         <v>14</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="104" t="s">
         <v>61</v>
       </c>
       <c r="C10" s="39"/>
@@ -8791,13 +8828,19 @@
         <v>3</v>
       </c>
       <c r="F10" s="40"/>
-      <c r="G10" s="39"/>
+      <c r="G10" s="39">
+        <v>-1</v>
+      </c>
       <c r="H10" s="39">
         <v>3</v>
       </c>
       <c r="I10" s="40"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="41"/>
+      <c r="J10" s="39">
+        <v>0</v>
+      </c>
+      <c r="K10" s="41">
+        <v>2</v>
+      </c>
       <c r="L10" s="40"/>
       <c r="M10" s="39"/>
       <c r="N10" s="41"/>
@@ -8815,7 +8858,7 @@
       <c r="A11" s="39">
         <v>14</v>
       </c>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="104" t="s">
         <v>120</v>
       </c>
       <c r="C11" s="39"/>
@@ -8826,8 +8869,12 @@
         <v>2</v>
       </c>
       <c r="F11" s="40"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="G11" s="96">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="39">
+        <v>2</v>
+      </c>
       <c r="I11" s="40"/>
       <c r="J11" s="39"/>
       <c r="K11" s="41"/>
@@ -8859,8 +8906,12 @@
         <v>3</v>
       </c>
       <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+      <c r="G12" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="39">
+        <v>3</v>
+      </c>
       <c r="I12" s="40"/>
       <c r="J12" s="39"/>
       <c r="K12" s="41"/>
@@ -8881,7 +8932,7 @@
       <c r="A13" s="39">
         <v>14</v>
       </c>
-      <c r="B13" s="120" t="s">
+      <c r="B13" s="119" t="s">
         <v>114</v>
       </c>
       <c r="C13" s="39"/>
@@ -8892,8 +8943,12 @@
         <v>0</v>
       </c>
       <c r="F13" s="40"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+      <c r="G13" s="96">
+        <v>-1</v>
+      </c>
+      <c r="H13" s="39">
+        <v>1</v>
+      </c>
       <c r="I13" s="40"/>
       <c r="J13" s="39"/>
       <c r="K13" s="41"/>
@@ -8925,8 +8980,12 @@
         <v>3</v>
       </c>
       <c r="F14" s="40"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
+      <c r="G14" s="39">
+        <v>0</v>
+      </c>
+      <c r="H14" s="39">
+        <v>3</v>
+      </c>
       <c r="I14" s="40"/>
       <c r="J14" s="39"/>
       <c r="K14" s="41"/>
@@ -8947,14 +9006,14 @@
       <c r="A15" s="39">
         <v>13</v>
       </c>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="94" t="s">
         <v>246</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="101"/>
       <c r="E15" s="101"/>
       <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="G15" s="55"/>
       <c r="H15" s="39"/>
       <c r="I15" s="40"/>
       <c r="J15" s="39"/>
@@ -8972,11 +9031,11 @@
       <c r="V15" s="39"/>
       <c r="W15" s="41"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="39">
         <v>14</v>
       </c>
-      <c r="B16" s="115" t="s">
+      <c r="B16" s="126" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="39"/>
@@ -8987,7 +9046,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="40"/>
-      <c r="G16" s="39"/>
+      <c r="G16" s="55"/>
       <c r="H16" s="39"/>
       <c r="I16" s="40"/>
       <c r="J16" s="39"/>
@@ -9005,25 +9064,25 @@
       <c r="V16" s="39"/>
       <c r="W16" s="41"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39">
         <v>13</v>
       </c>
-      <c r="B17" s="91" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39">
-        <v>-1</v>
+      <c r="B17" s="95" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="39">
+        <v>-12</v>
+      </c>
+      <c r="D17" s="50">
+        <v>-2</v>
       </c>
       <c r="E17" s="41">
         <v>3</v>
       </c>
       <c r="F17" s="40"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39">
-        <v>3</v>
-      </c>
+      <c r="G17" s="101"/>
+      <c r="H17" s="101"/>
       <c r="I17" s="40"/>
       <c r="J17" s="39"/>
       <c r="K17" s="41"/>
@@ -9045,7 +9104,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="91" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="C18" s="39"/>
       <c r="D18" s="39">
@@ -9054,12 +9113,20 @@
       <c r="E18" s="41">
         <v>3</v>
       </c>
-      <c r="F18" s="83"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H18" s="39">
+        <v>3</v>
+      </c>
       <c r="I18" s="40"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="41"/>
+      <c r="J18" s="117">
+        <v>1</v>
+      </c>
+      <c r="K18" s="41">
+        <v>3</v>
+      </c>
       <c r="L18" s="40"/>
       <c r="M18" s="39"/>
       <c r="N18" s="41"/>
@@ -9078,7 +9145,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="91" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C19" s="39"/>
       <c r="D19" s="39">
@@ -9087,12 +9154,20 @@
       <c r="E19" s="41">
         <v>3</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="39">
+        <v>3</v>
+      </c>
       <c r="I19" s="40"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="41"/>
+      <c r="J19" s="39">
+        <v>-1</v>
+      </c>
+      <c r="K19" s="41">
+        <v>3</v>
+      </c>
       <c r="L19" s="40"/>
       <c r="M19" s="39"/>
       <c r="N19" s="41"/>
@@ -9111,7 +9186,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="91" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C20" s="39"/>
       <c r="D20" s="39">
@@ -9120,9 +9195,13 @@
       <c r="E20" s="41">
         <v>3</v>
       </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H20" s="39">
+        <v>3</v>
+      </c>
       <c r="I20" s="40"/>
       <c r="J20" s="39"/>
       <c r="K20" s="41"/>
@@ -9144,7 +9223,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="91" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C21" s="39"/>
       <c r="D21" s="39">
@@ -9154,30 +9233,34 @@
         <v>3</v>
       </c>
       <c r="F21" s="40"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
+      <c r="G21" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H21" s="39">
+        <v>3</v>
+      </c>
       <c r="I21" s="40"/>
       <c r="J21" s="39"/>
-      <c r="K21" s="42"/>
+      <c r="K21" s="41"/>
       <c r="L21" s="40"/>
       <c r="M21" s="39"/>
       <c r="N21" s="41"/>
       <c r="O21" s="39"/>
       <c r="P21" s="39"/>
-      <c r="Q21" s="42"/>
+      <c r="Q21" s="41"/>
       <c r="R21" s="40"/>
       <c r="S21" s="39"/>
       <c r="T21" s="39"/>
       <c r="U21" s="40"/>
       <c r="V21" s="39"/>
-      <c r="W21" s="42"/>
+      <c r="W21" s="41"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>13</v>
       </c>
       <c r="B22" s="91" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39">
@@ -9187,30 +9270,34 @@
         <v>3</v>
       </c>
       <c r="F22" s="40"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
+      <c r="G22" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H22" s="39">
+        <v>3</v>
+      </c>
       <c r="I22" s="40"/>
       <c r="J22" s="39"/>
-      <c r="K22" s="41"/>
+      <c r="K22" s="42"/>
       <c r="L22" s="40"/>
       <c r="M22" s="39"/>
       <c r="N22" s="41"/>
       <c r="O22" s="39"/>
       <c r="P22" s="39"/>
-      <c r="Q22" s="41"/>
+      <c r="Q22" s="42"/>
       <c r="R22" s="40"/>
       <c r="S22" s="39"/>
       <c r="T22" s="39"/>
       <c r="U22" s="40"/>
       <c r="V22" s="39"/>
-      <c r="W22" s="41"/>
+      <c r="W22" s="42"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="39">
         <v>13</v>
       </c>
       <c r="B23" s="91" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="C23" s="39"/>
       <c r="D23" s="39">
@@ -9220,8 +9307,12 @@
         <v>3</v>
       </c>
       <c r="F23" s="40"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
+      <c r="G23" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H23" s="39">
+        <v>3</v>
+      </c>
       <c r="I23" s="40"/>
       <c r="J23" s="39"/>
       <c r="K23" s="41"/>
@@ -9243,20 +9334,22 @@
         <v>13</v>
       </c>
       <c r="B24" s="91" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="39">
-        <v>12</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C24" s="39"/>
       <c r="D24" s="39">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E24" s="41">
         <v>3</v>
       </c>
       <c r="F24" s="40"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
+      <c r="G24" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H24" s="39">
+        <v>3</v>
+      </c>
       <c r="I24" s="40"/>
       <c r="J24" s="39"/>
       <c r="K24" s="41"/>
@@ -9278,18 +9371,24 @@
         <v>13</v>
       </c>
       <c r="B25" s="91" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="39"/>
+        <v>74</v>
+      </c>
+      <c r="C25" s="39">
+        <v>12</v>
+      </c>
       <c r="D25" s="39">
+        <v>0</v>
+      </c>
+      <c r="E25" s="41">
+        <v>3</v>
+      </c>
+      <c r="F25" s="40"/>
+      <c r="G25" s="39">
         <v>-1</v>
       </c>
-      <c r="E25" s="41">
-        <v>3</v>
-      </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
+      <c r="H25" s="39">
+        <v>3</v>
+      </c>
       <c r="I25" s="40"/>
       <c r="J25" s="39"/>
       <c r="K25" s="41"/>
@@ -9298,7 +9397,7 @@
       <c r="N25" s="41"/>
       <c r="O25" s="39"/>
       <c r="P25" s="39"/>
-      <c r="Q25" s="39"/>
+      <c r="Q25" s="41"/>
       <c r="R25" s="40"/>
       <c r="S25" s="39"/>
       <c r="T25" s="39"/>
@@ -9311,7 +9410,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C26" s="39"/>
       <c r="D26" s="39">
@@ -9321,19 +9420,25 @@
         <v>3</v>
       </c>
       <c r="F26" s="40"/>
-      <c r="G26" s="39"/>
+      <c r="G26" s="39">
+        <v>-1</v>
+      </c>
       <c r="H26" s="39">
         <v>3</v>
       </c>
       <c r="I26" s="40"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="41"/>
+      <c r="J26" s="39">
+        <v>-2</v>
+      </c>
+      <c r="K26" s="41">
+        <v>3</v>
+      </c>
       <c r="L26" s="40"/>
       <c r="M26" s="39"/>
       <c r="N26" s="41"/>
       <c r="O26" s="39"/>
       <c r="P26" s="39"/>
-      <c r="Q26" s="41"/>
+      <c r="Q26" s="39"/>
       <c r="R26" s="40"/>
       <c r="S26" s="39"/>
       <c r="T26" s="39"/>
@@ -9343,26 +9448,32 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="39">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B27" s="91" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C27" s="39"/>
       <c r="D27" s="39">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E27" s="41">
         <v>3</v>
       </c>
       <c r="F27" s="40"/>
-      <c r="G27" s="39"/>
+      <c r="G27" s="39">
+        <v>-1</v>
+      </c>
       <c r="H27" s="39">
         <v>3</v>
       </c>
       <c r="I27" s="40"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="41"/>
+      <c r="J27" s="39">
+        <v>-2</v>
+      </c>
+      <c r="K27" s="41">
+        <v>3</v>
+      </c>
       <c r="L27" s="40"/>
       <c r="M27" s="39"/>
       <c r="N27" s="41"/>
@@ -9381,23 +9492,29 @@
         <v>12</v>
       </c>
       <c r="B28" s="91" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C28" s="39"/>
       <c r="D28" s="39">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="41">
         <v>3</v>
       </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="39">
+        <v>0</v>
+      </c>
       <c r="H28" s="39">
         <v>3</v>
       </c>
       <c r="I28" s="40"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="41"/>
+      <c r="J28" s="39">
+        <v>-2</v>
+      </c>
+      <c r="K28" s="41">
+        <v>3</v>
+      </c>
       <c r="L28" s="40"/>
       <c r="M28" s="39"/>
       <c r="N28" s="41"/>
@@ -9416,7 +9533,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="39"/>
       <c r="D29" s="39">
@@ -9425,14 +9542,20 @@
       <c r="E29" s="41">
         <v>3</v>
       </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39">
+        <v>0</v>
+      </c>
       <c r="H29" s="39">
         <v>3</v>
       </c>
       <c r="I29" s="40"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="41"/>
+      <c r="J29" s="39">
+        <v>-2</v>
+      </c>
+      <c r="K29" s="41">
+        <v>3</v>
+      </c>
       <c r="L29" s="40"/>
       <c r="M29" s="39"/>
       <c r="N29" s="41"/>
@@ -9444,25 +9567,29 @@
       <c r="T29" s="39"/>
       <c r="U29" s="40"/>
       <c r="V29" s="39"/>
-      <c r="W29" s="77"/>
-    </row>
-    <row r="30" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W29" s="41"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="39">
         <v>12</v>
       </c>
       <c r="B30" s="91" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" s="39"/>
       <c r="D30" s="39">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="E30" s="41">
         <v>3</v>
       </c>
       <c r="F30" s="40"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
+      <c r="G30" s="39">
+        <v>-1</v>
+      </c>
+      <c r="H30" s="39">
+        <v>3</v>
+      </c>
       <c r="I30" s="40"/>
       <c r="J30" s="39"/>
       <c r="K30" s="41"/>
@@ -9477,26 +9604,36 @@
       <c r="T30" s="39"/>
       <c r="U30" s="40"/>
       <c r="V30" s="39"/>
-      <c r="W30" s="41"/>
-    </row>
-    <row r="31" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W30" s="77"/>
+    </row>
+    <row r="31" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="39">
         <v>12</v>
       </c>
       <c r="B31" s="91" t="s">
-        <v>252</v>
+        <v>79</v>
       </c>
       <c r="C31" s="39"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
+      <c r="D31" s="39">
+        <v>-4</v>
+      </c>
+      <c r="E31" s="41">
+        <v>3</v>
+      </c>
+      <c r="F31" s="40"/>
+      <c r="G31" s="39">
+        <v>-1</v>
+      </c>
       <c r="H31" s="39">
         <v>3</v>
       </c>
       <c r="I31" s="40"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="41"/>
+      <c r="J31" s="39">
+        <v>-2</v>
+      </c>
+      <c r="K31" s="41">
+        <v>3</v>
+      </c>
       <c r="L31" s="40"/>
       <c r="M31" s="39"/>
       <c r="N31" s="41"/>
@@ -9512,16 +9649,18 @@
     </row>
     <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="39">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B32" s="91" t="s">
-        <v>80</v>
+        <v>252</v>
       </c>
       <c r="C32" s="39"/>
       <c r="D32" s="101"/>
       <c r="E32" s="101"/>
       <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
+      <c r="G32" s="39">
+        <v>-2</v>
+      </c>
       <c r="H32" s="39">
         <v>3</v>
       </c>
@@ -9591,28 +9730,32 @@
       <c r="V34" s="43"/>
       <c r="W34" s="43"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="39">
-        <v>13</v>
-      </c>
-      <c r="B35" s="94" t="s">
-        <v>109</v>
+        <v>11</v>
+      </c>
+      <c r="B35" s="91" t="s">
+        <v>80</v>
       </c>
       <c r="C35" s="39"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
+      <c r="D35" s="101"/>
+      <c r="E35" s="101"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39">
+        <v>-2</v>
+      </c>
+      <c r="H35" s="39">
+        <v>3</v>
+      </c>
       <c r="I35" s="40"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="41"/>
+      <c r="J35" s="101"/>
+      <c r="K35" s="101"/>
       <c r="L35" s="40"/>
       <c r="M35" s="39"/>
       <c r="N35" s="41"/>
       <c r="O35" s="39"/>
       <c r="P35" s="39"/>
-      <c r="Q35" s="39"/>
+      <c r="Q35" s="41"/>
       <c r="R35" s="40"/>
       <c r="S35" s="39"/>
       <c r="T35" s="39"/>
@@ -9622,10 +9765,10 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="39">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B36" s="94" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="C36" s="39"/>
       <c r="D36" s="55"/>
@@ -9641,7 +9784,7 @@
       <c r="N36" s="41"/>
       <c r="O36" s="39"/>
       <c r="P36" s="39"/>
-      <c r="Q36" s="41"/>
+      <c r="Q36" s="39"/>
       <c r="R36" s="40"/>
       <c r="S36" s="39"/>
       <c r="T36" s="39"/>
@@ -9651,20 +9794,14 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="39">
-        <v>13</v>
-      </c>
-      <c r="B37" s="95" t="s">
-        <v>113</v>
-      </c>
-      <c r="C37" s="39">
-        <v>-12</v>
-      </c>
-      <c r="D37" s="50">
-        <v>-2</v>
-      </c>
-      <c r="E37" s="41">
-        <v>3</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B37" s="94" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="39"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="41"/>
       <c r="F37" s="40"/>
       <c r="G37" s="39"/>
       <c r="H37" s="39"/>
@@ -9688,7 +9825,7 @@
       <c r="A38" s="39">
         <v>13</v>
       </c>
-      <c r="B38" s="121" t="s">
+      <c r="B38" s="120" t="s">
         <v>251</v>
       </c>
       <c r="C38" s="39"/>
@@ -9717,7 +9854,7 @@
       <c r="A39" s="39">
         <v>13</v>
       </c>
-      <c r="B39" s="121" t="s">
+      <c r="B39" s="120" t="s">
         <v>257</v>
       </c>
       <c r="C39" s="39"/>
@@ -9746,7 +9883,7 @@
       <c r="A40" s="39">
         <v>13</v>
       </c>
-      <c r="B40" s="121" t="s">
+      <c r="B40" s="120" t="s">
         <v>244</v>
       </c>
       <c r="C40" s="39"/>
@@ -10771,16 +10908,16 @@
       <c r="H31" s="76"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="125" t="s">
+      <c r="A32" s="124" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="123"/>
-      <c r="C32" s="123"/>
-      <c r="D32" s="123"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="123"/>
-      <c r="G32" s="123"/>
-      <c r="H32" s="124"/>
+      <c r="B32" s="122"/>
+      <c r="C32" s="122"/>
+      <c r="D32" s="122"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="122"/>
+      <c r="G32" s="122"/>
+      <c r="H32" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update WAR data - 2026-02-15
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -11384,7 +11384,6 @@
           <t>GX king</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr"/>
       <c r="X1" s="114" t="inlineStr">
         <is>
           <t>CWL 4</t>
@@ -12754,12 +12753,12 @@
       </c>
       <c r="AO1" s="107" t="inlineStr">
         <is>
-          <t>Colonna41</t>
+          <t>WAR-18 (1)</t>
         </is>
       </c>
       <c r="AP1" s="112" t="inlineStr">
         <is>
-          <t>Colonna42</t>
+          <t>WAR-18 (2)</t>
         </is>
       </c>
       <c r="AQ1" s="107" t="inlineStr">
@@ -13004,11 +13003,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="111">
-        <f>SUM(G2:AN2)</f>
+        <f>SUM(G2:AP2)</f>
         <v/>
       </c>
       <c r="F2" s="68">
-        <f>ROUND(AVERAGE(G2:AN2),1)</f>
+        <f>ROUND(AVERAGE(G2:AP2),1)</f>
         <v/>
       </c>
       <c r="G2" s="110" t="n"/>
@@ -13123,11 +13122,11 @@
         <v>0</v>
       </c>
       <c r="E3" s="68">
-        <f>SUM(G3:AN3)</f>
+        <f>SUM(G3:AP3)</f>
         <v/>
       </c>
       <c r="F3" s="68">
-        <f>ROUND(AVERAGE(G3:AN3),1)</f>
+        <f>ROUND(AVERAGE(G3:AP3),1)</f>
         <v/>
       </c>
     </row>
@@ -13147,11 +13146,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="68">
-        <f>SUM(G4:AN4)</f>
+        <f>SUM(G4:AP4)</f>
         <v/>
       </c>
       <c r="F4" s="68">
-        <f>ROUND(AVERAGE(G4:AN4),1)</f>
+        <f>ROUND(AVERAGE(G4:AP4),1)</f>
         <v/>
       </c>
       <c r="I4" s="79" t="n">
@@ -13190,21 +13189,29 @@
         </is>
       </c>
       <c r="B5" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="68">
-        <f>SUM(G5:AN5)</f>
+        <f>SUM(G5:AP5)</f>
         <v/>
       </c>
       <c r="F5" s="68">
-        <f>ROUND(AVERAGE(G5:AN5),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G5:AP5),1)</f>
+        <v/>
+      </c>
+      <c r="AO5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -13223,11 +13230,11 @@
         <v>4</v>
       </c>
       <c r="E6" s="68">
-        <f>SUM(G6:AN6)</f>
+        <f>SUM(G6:AP6)</f>
         <v/>
       </c>
       <c r="F6" s="68">
-        <f>ROUND(AVERAGE(G6:AN6),1)</f>
+        <f>ROUND(AVERAGE(G6:AP6),1)</f>
         <v/>
       </c>
       <c r="U6" s="79" t="n">
@@ -13264,20 +13271,20 @@
         </is>
       </c>
       <c r="B7" s="79" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="68" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="79" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="68">
-        <f>SUM(G7:AN7)</f>
+        <f>SUM(G7:AP7)</f>
         <v/>
       </c>
       <c r="F7" s="68">
-        <f>ROUND(AVERAGE(G7:AN7),1)</f>
+        <f>ROUND(AVERAGE(G7:AP7),1)</f>
         <v/>
       </c>
       <c r="G7" s="79" t="n">
@@ -13375,6 +13382,14 @@
       </c>
       <c r="AN7" t="n">
         <v>1</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP7" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -13393,11 +13408,11 @@
         <v>5</v>
       </c>
       <c r="E8" s="68">
-        <f>SUM(G8:AN8)</f>
+        <f>SUM(G8:AP8)</f>
         <v/>
       </c>
       <c r="F8" s="68">
-        <f>ROUND(AVERAGE(G8:AN8),1)</f>
+        <f>ROUND(AVERAGE(G8:AP8),1)</f>
         <v/>
       </c>
       <c r="K8" s="79" t="n">
@@ -13447,11 +13462,11 @@
         <v>0</v>
       </c>
       <c r="E9" s="68">
-        <f>SUM(G9:AN9)</f>
+        <f>SUM(G9:AP9)</f>
         <v/>
       </c>
       <c r="F9" s="68">
-        <f>ROUND(AVERAGE(G9:AN9),1)</f>
+        <f>ROUND(AVERAGE(G9:AP9),1)</f>
         <v/>
       </c>
     </row>
@@ -13471,11 +13486,11 @@
         <v>12</v>
       </c>
       <c r="E10" s="68">
-        <f>SUM(G10:AN10)</f>
+        <f>SUM(G10:AP10)</f>
         <v/>
       </c>
       <c r="F10" s="68">
-        <f>ROUND(AVERAGE(G10:AN10),1)</f>
+        <f>ROUND(AVERAGE(G10:AP10),1)</f>
         <v/>
       </c>
       <c r="G10" s="79" t="n">
@@ -13567,11 +13582,11 @@
         <v>0</v>
       </c>
       <c r="E11" s="68">
-        <f>SUM(G11:AN11)</f>
+        <f>SUM(G11:AP11)</f>
         <v/>
       </c>
       <c r="F11" s="68">
-        <f>ROUND(AVERAGE(G11:AN11),1)</f>
+        <f>ROUND(AVERAGE(G11:AP11),1)</f>
         <v/>
       </c>
     </row>
@@ -13591,11 +13606,11 @@
         <v>6</v>
       </c>
       <c r="E12" s="68">
-        <f>SUM(G12:AN12)</f>
+        <f>SUM(G12:AP12)</f>
         <v/>
       </c>
       <c r="F12" s="68">
-        <f>ROUND(AVERAGE(G12:AN12),1)</f>
+        <f>ROUND(AVERAGE(G12:AP12),1)</f>
         <v/>
       </c>
       <c r="I12" s="79" t="n">
@@ -13665,11 +13680,11 @@
         <v>5</v>
       </c>
       <c r="E13" s="68">
-        <f>SUM(G13:AN13)</f>
+        <f>SUM(G13:AP13)</f>
         <v/>
       </c>
       <c r="F13" s="68">
-        <f>ROUND(AVERAGE(G13:AN13),1)</f>
+        <f>ROUND(AVERAGE(G13:AP13),1)</f>
         <v/>
       </c>
       <c r="Q13" s="79" t="n">
@@ -13718,14 +13733,14 @@
         <v>0</v>
       </c>
       <c r="D14" s="79" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14" s="68">
-        <f>SUM(G14:AN14)</f>
+        <f>SUM(G14:AP14)</f>
         <v/>
       </c>
       <c r="F14" s="68">
-        <f>ROUND(AVERAGE(G14:AN14),1)</f>
+        <f>ROUND(AVERAGE(G14:AP14),1)</f>
         <v/>
       </c>
       <c r="G14" s="79" t="n">
@@ -13781,6 +13796,12 @@
       </c>
       <c r="AN14" t="n">
         <v>1</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -13799,11 +13820,11 @@
         <v>0</v>
       </c>
       <c r="E15" s="68">
-        <f>SUM(G15:AN15)</f>
+        <f>SUM(G15:AP15)</f>
         <v/>
       </c>
       <c r="F15" s="68">
-        <f>ROUND(AVERAGE(G15:AN15),1)</f>
+        <f>ROUND(AVERAGE(G15:AP15),1)</f>
         <v/>
       </c>
     </row>
@@ -13820,14 +13841,14 @@
         <v>1</v>
       </c>
       <c r="D16" s="79" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="68">
-        <f>SUM(G16:AN16)</f>
+        <f>SUM(G16:AP16)</f>
         <v/>
       </c>
       <c r="F16" s="68">
-        <f>ROUND(AVERAGE(G16:AN16),1)</f>
+        <f>ROUND(AVERAGE(G16:AP16),1)</f>
         <v/>
       </c>
       <c r="I16" s="79" t="n">
@@ -13901,6 +13922,12 @@
       </c>
       <c r="AN16" t="n">
         <v>3</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -13919,11 +13946,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="68">
-        <f>SUM(G17:AN17)</f>
+        <f>SUM(G17:AP17)</f>
         <v/>
       </c>
       <c r="F17" s="68">
-        <f>ROUND(AVERAGE(G17:AN17),1)</f>
+        <f>ROUND(AVERAGE(G17:AP17),1)</f>
         <v/>
       </c>
       <c r="AE17" s="79" t="n">
@@ -13949,11 +13976,11 @@
         <v>8</v>
       </c>
       <c r="E18" s="68">
-        <f>SUM(G18:AN18)</f>
+        <f>SUM(G18:AP18)</f>
         <v/>
       </c>
       <c r="F18" s="68">
-        <f>ROUND(AVERAGE(G18:AN18),1)</f>
+        <f>ROUND(AVERAGE(G18:AP18),1)</f>
         <v/>
       </c>
       <c r="S18" s="79" t="n">
@@ -14025,11 +14052,11 @@
         <v>3</v>
       </c>
       <c r="E19" s="68">
-        <f>SUM(G19:AN19)</f>
+        <f>SUM(G19:AP19)</f>
         <v/>
       </c>
       <c r="F19" s="68">
-        <f>ROUND(AVERAGE(G19:AN19),1)</f>
+        <f>ROUND(AVERAGE(G19:AP19),1)</f>
         <v/>
       </c>
       <c r="G19" s="79" t="n">
@@ -14067,11 +14094,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="68">
-        <f>SUM(G20:AN20)</f>
+        <f>SUM(G20:AP20)</f>
         <v/>
       </c>
       <c r="F20" s="68">
-        <f>ROUND(AVERAGE(G20:AN20),1)</f>
+        <f>ROUND(AVERAGE(G20:AP20),1)</f>
         <v/>
       </c>
       <c r="AE20" s="79" t="n">
@@ -14094,14 +14121,14 @@
         <v>0</v>
       </c>
       <c r="D21" s="79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E21" s="68">
-        <f>SUM(G21:AN21)</f>
+        <f>SUM(G21:AP21)</f>
         <v/>
       </c>
       <c r="F21" s="68">
-        <f>ROUND(AVERAGE(G21:AN21),1)</f>
+        <f>ROUND(AVERAGE(G21:AP21),1)</f>
         <v/>
       </c>
       <c r="I21" s="79" t="n">
@@ -14149,6 +14176,12 @@
       </c>
       <c r="AD21" s="80" t="n">
         <v>3</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -14167,11 +14200,11 @@
         <v>8</v>
       </c>
       <c r="E22" s="68">
-        <f>SUM(G22:AN22)</f>
+        <f>SUM(G22:AP22)</f>
         <v/>
       </c>
       <c r="F22" s="68">
-        <f>ROUND(AVERAGE(G22:AN22),1)</f>
+        <f>ROUND(AVERAGE(G22:AP22),1)</f>
         <v/>
       </c>
       <c r="G22" s="79" t="inlineStr">
@@ -14236,20 +14269,20 @@
         </is>
       </c>
       <c r="B23" s="79" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" s="68" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="79" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23" s="68">
-        <f>SUM(G23:AN23)</f>
+        <f>SUM(G23:AP23)</f>
         <v/>
       </c>
       <c r="F23" s="68">
-        <f>ROUND(AVERAGE(G23:AN23),1)</f>
+        <f>ROUND(AVERAGE(G23:AP23),1)</f>
         <v/>
       </c>
       <c r="G23" s="79" t="n">
@@ -14317,6 +14350,14 @@
       </c>
       <c r="AL23" t="n">
         <v>3</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP23" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -14335,11 +14376,11 @@
         <v>11</v>
       </c>
       <c r="E24" s="68">
-        <f>SUM(G24:AN24)</f>
+        <f>SUM(G24:AP24)</f>
         <v/>
       </c>
       <c r="F24" s="68">
-        <f>ROUND(AVERAGE(G24:AN24),1)</f>
+        <f>ROUND(AVERAGE(G24:AP24),1)</f>
         <v/>
       </c>
       <c r="G24" s="79" t="n">
@@ -14429,11 +14470,11 @@
         <v>8</v>
       </c>
       <c r="E25" s="68">
-        <f>SUM(G25:AN25)</f>
+        <f>SUM(G25:AP25)</f>
         <v/>
       </c>
       <c r="F25" s="68">
-        <f>ROUND(AVERAGE(G25:AN25),1)</f>
+        <f>ROUND(AVERAGE(G25:AP25),1)</f>
         <v/>
       </c>
       <c r="I25" s="79" t="n">
@@ -14511,11 +14552,11 @@
         <v>3</v>
       </c>
       <c r="E26" s="68">
-        <f>SUM(G26:AN26)</f>
+        <f>SUM(G26:AP26)</f>
         <v/>
       </c>
       <c r="F26" s="68">
-        <f>ROUND(AVERAGE(G26:AN26),1)</f>
+        <f>ROUND(AVERAGE(G26:AP26),1)</f>
         <v/>
       </c>
       <c r="Y26" s="79" t="n">
@@ -14555,11 +14596,11 @@
         <v>8</v>
       </c>
       <c r="E27" s="68">
-        <f>SUM(G27:AN27)</f>
+        <f>SUM(G27:AP27)</f>
         <v/>
       </c>
       <c r="F27" s="68">
-        <f>ROUND(AVERAGE(G27:AN27),1)</f>
+        <f>ROUND(AVERAGE(G27:AP27),1)</f>
         <v/>
       </c>
       <c r="S27" s="79" t="n">
@@ -14637,11 +14678,11 @@
         <v>10</v>
       </c>
       <c r="E28" s="68">
-        <f>SUM(G28:AN28)</f>
+        <f>SUM(G28:AP28)</f>
         <v/>
       </c>
       <c r="F28" s="68">
-        <f>ROUND(AVERAGE(G28:AN28),1)</f>
+        <f>ROUND(AVERAGE(G28:AP28),1)</f>
         <v/>
       </c>
       <c r="I28" s="79" t="inlineStr">
@@ -14732,15 +14773,21 @@
         <v>0</v>
       </c>
       <c r="D29" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="68">
-        <f>SUM(G29:AN29)</f>
+        <f>SUM(G29:AP29)</f>
         <v/>
       </c>
       <c r="F29" s="68">
-        <f>ROUND(AVERAGE(G29:AN29),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G29:AP29),1)</f>
+        <v/>
+      </c>
+      <c r="AO29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -14756,14 +14803,14 @@
         <v>0</v>
       </c>
       <c r="D30" s="79" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E30" s="68">
-        <f>SUM(G30:AN30)</f>
+        <f>SUM(G30:AP30)</f>
         <v/>
       </c>
       <c r="F30" s="68">
-        <f>ROUND(AVERAGE(G30:AN30),1)</f>
+        <f>ROUND(AVERAGE(G30:AP30),1)</f>
         <v/>
       </c>
       <c r="G30" s="79" t="n">
@@ -14848,6 +14895,12 @@
         <v>3</v>
       </c>
       <c r="AN30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP30" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14867,11 +14920,11 @@
         <v>4</v>
       </c>
       <c r="E31" s="68">
-        <f>SUM(G31:AN31)</f>
+        <f>SUM(G31:AP31)</f>
         <v/>
       </c>
       <c r="F31" s="68">
-        <f>ROUND(AVERAGE(G31:AN31),1)</f>
+        <f>ROUND(AVERAGE(G31:AP31),1)</f>
         <v/>
       </c>
       <c r="G31" s="79" t="n">
@@ -14915,11 +14968,11 @@
         <v>11</v>
       </c>
       <c r="E32" s="68">
-        <f>SUM(G32:AN32)</f>
+        <f>SUM(G32:AP32)</f>
         <v/>
       </c>
       <c r="F32" s="68">
-        <f>ROUND(AVERAGE(G32:AN32),1)</f>
+        <f>ROUND(AVERAGE(G32:AP32),1)</f>
         <v/>
       </c>
       <c r="G32" s="79" t="n">
@@ -15015,11 +15068,11 @@
         <v>0</v>
       </c>
       <c r="E33" s="68">
-        <f>SUM(G33:AN33)</f>
+        <f>SUM(G33:AP33)</f>
         <v/>
       </c>
       <c r="F33" s="68">
-        <f>ROUND(AVERAGE(G33:AN33),1)</f>
+        <f>ROUND(AVERAGE(G33:AP33),1)</f>
         <v/>
       </c>
     </row>
@@ -15036,14 +15089,14 @@
         <v>1</v>
       </c>
       <c r="D34" s="79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E34" s="68">
-        <f>SUM(G34:AN34)</f>
+        <f>SUM(G34:AP34)</f>
         <v/>
       </c>
       <c r="F34" s="68">
-        <f>ROUND(AVERAGE(G34:AN34),1)</f>
+        <f>ROUND(AVERAGE(G34:AP34),1)</f>
         <v/>
       </c>
       <c r="O34" s="79" t="n">
@@ -15091,6 +15144,12 @@
       </c>
       <c r="AL34" t="n">
         <v>3</v>
+      </c>
+      <c r="AO34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP34" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -15109,11 +15168,11 @@
         <v>2</v>
       </c>
       <c r="E35" s="68">
-        <f>SUM(G35:AN35)</f>
+        <f>SUM(G35:AP35)</f>
         <v/>
       </c>
       <c r="F35" s="68">
-        <f>ROUND(AVERAGE(G35:AN35),1)</f>
+        <f>ROUND(AVERAGE(G35:AP35),1)</f>
         <v/>
       </c>
       <c r="K35" s="79" t="inlineStr">
@@ -15149,11 +15208,11 @@
         <v>13</v>
       </c>
       <c r="E36" s="68">
-        <f>SUM(G36:AN36)</f>
+        <f>SUM(G36:AP36)</f>
         <v/>
       </c>
       <c r="F36" s="68">
-        <f>ROUND(AVERAGE(G36:AN36),1)</f>
+        <f>ROUND(AVERAGE(G36:AP36),1)</f>
         <v/>
       </c>
       <c r="G36" s="79" t="n">
@@ -15256,14 +15315,14 @@
         <v>1</v>
       </c>
       <c r="D37" s="79" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E37" s="68">
-        <f>SUM(G37:AN37)</f>
+        <f>SUM(G37:AP37)</f>
         <v/>
       </c>
       <c r="F37" s="68">
-        <f>ROUND(AVERAGE(G37:AN37),1)</f>
+        <f>ROUND(AVERAGE(G37:AP37),1)</f>
         <v/>
       </c>
       <c r="U37" s="79" t="n">
@@ -15326,6 +15385,12 @@
         <v>3</v>
       </c>
       <c r="AN37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO37" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP37" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15336,20 +15401,20 @@
         </is>
       </c>
       <c r="B38" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D38" s="79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="68">
-        <f>SUM(G38:AN38)</f>
+        <f>SUM(G38:AP38)</f>
         <v/>
       </c>
       <c r="F38" s="68">
-        <f>ROUND(AVERAGE(G38:AN38),1)</f>
+        <f>ROUND(AVERAGE(G38:AP38),1)</f>
         <v/>
       </c>
       <c r="AM38" t="n">
@@ -15357,6 +15422,14 @@
       </c>
       <c r="AN38" t="n">
         <v>3</v>
+      </c>
+      <c r="AO38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP38" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -15372,14 +15445,14 @@
         <v>0</v>
       </c>
       <c r="D39" s="79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="68">
-        <f>SUM(G39:AN39)</f>
+        <f>SUM(G39:AP39)</f>
         <v/>
       </c>
       <c r="F39" s="68">
-        <f>ROUND(AVERAGE(G39:AN39),1)</f>
+        <f>ROUND(AVERAGE(G39:AP39),1)</f>
         <v/>
       </c>
       <c r="AM39" t="n">
@@ -15387,6 +15460,12 @@
       </c>
       <c r="AN39" t="n">
         <v>2</v>
+      </c>
+      <c r="AO39" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP39" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -15402,14 +15481,14 @@
         <v>0</v>
       </c>
       <c r="D40" s="79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" s="68">
-        <f>SUM(G40:AN40)</f>
+        <f>SUM(G40:AP40)</f>
         <v/>
       </c>
       <c r="F40" s="68">
-        <f>ROUND(AVERAGE(G40:AN40),1)</f>
+        <f>ROUND(AVERAGE(G40:AP40),1)</f>
         <v/>
       </c>
       <c r="AM40" t="n">
@@ -15417,12 +15496,18 @@
       </c>
       <c r="AN40" t="n">
         <v>3</v>
+      </c>
+      <c r="AO40" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP40" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="79" t="inlineStr">
         <is>
-          <t>~Oblivion~</t>
+          <t>terracrom</t>
         </is>
       </c>
       <c r="B41" s="79" t="n">
@@ -15435,18 +15520,18 @@
         <v>0</v>
       </c>
       <c r="E41" s="68">
-        <f>SUM(G41:AN41)</f>
+        <f>SUM(G41:AP41)</f>
         <v/>
       </c>
       <c r="F41" s="68">
-        <f>ROUND(AVERAGE(G41:AN41),1)</f>
+        <f>ROUND(AVERAGE(G41:AP41),1)</f>
         <v/>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="79" t="inlineStr">
         <is>
-          <t>terracrom</t>
+          <t>MIRIAM MIRIAM</t>
         </is>
       </c>
       <c r="B42" s="79" t="n">
@@ -15456,21 +15541,33 @@
         <v>0</v>
       </c>
       <c r="D42" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E42" s="68">
-        <f>SUM(G42:AN42)</f>
+        <f>SUM(G42:AP42)</f>
         <v/>
       </c>
       <c r="F42" s="68">
-        <f>ROUND(AVERAGE(G42:AN42),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G42:AP42),1)</f>
+        <v/>
+      </c>
+      <c r="AM42" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN42" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO42" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP42" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="79" t="inlineStr">
         <is>
-          <t>Ahmo</t>
+          <t>cucco</t>
         </is>
       </c>
       <c r="B43" s="79" t="n">
@@ -15480,21 +15577,33 @@
         <v>0</v>
       </c>
       <c r="D43" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E43" s="68">
-        <f>SUM(G43:AN43)</f>
+        <f>SUM(G43:AP43)</f>
         <v/>
       </c>
       <c r="F43" s="68">
-        <f>ROUND(AVERAGE(G43:AN43),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G43:AP43),1)</f>
+        <v/>
+      </c>
+      <c r="AM43" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN43" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO43" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP43" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="79" t="inlineStr">
         <is>
-          <t>MIRIAM MIRIAM</t>
+          <t>KingVanze98</t>
         </is>
       </c>
       <c r="B44" s="79" t="n">
@@ -15504,27 +15613,21 @@
         <v>0</v>
       </c>
       <c r="D44" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" s="68">
-        <f>SUM(G44:AN44)</f>
+        <f>SUM(G44:AP44)</f>
         <v/>
       </c>
       <c r="F44" s="68">
-        <f>ROUND(AVERAGE(G44:AN44),1)</f>
-        <v/>
-      </c>
-      <c r="AM44" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN44" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G44:AP44),1)</f>
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="79" t="inlineStr">
         <is>
-          <t>cucco</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="B45" s="79" t="n">
@@ -15534,27 +15637,21 @@
         <v>0</v>
       </c>
       <c r="D45" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" s="68">
-        <f>SUM(G45:AN45)</f>
+        <f>SUM(G45:AP45)</f>
         <v/>
       </c>
       <c r="F45" s="68">
-        <f>ROUND(AVERAGE(G45:AN45),1)</f>
-        <v/>
-      </c>
-      <c r="AM45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN45" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G45:AP45),1)</f>
+        <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="79" t="inlineStr">
         <is>
-          <t>KingVanze98</t>
+          <t>fede61mito</t>
         </is>
       </c>
       <c r="B46" s="79" t="n">
@@ -15567,46 +15664,36 @@
         <v>0</v>
       </c>
       <c r="E46" s="68">
-        <f>SUM(G46:AN46)</f>
+        <f>SUM(G46:AP46)</f>
         <v/>
       </c>
       <c r="F46" s="68">
-        <f>ROUND(AVERAGE(G46:AN46),1)</f>
+        <f>ROUND(AVERAGE(G46:AP46),1)</f>
         <v/>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="79" t="inlineStr">
         <is>
-          <t>thor</t>
+          <t>Dasters79</t>
         </is>
       </c>
       <c r="B47" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C47" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" s="68">
-        <f>SUM(G47:AN47)</f>
+        <f>SUM(G47:AP47)</f>
         <v/>
       </c>
       <c r="F47" s="68">
-        <f>ROUND(AVERAGE(G47:AN47),1)</f>
-        <v/>
-      </c>
-      <c r="AM47" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AN47" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+        <f>ROUND(AVERAGE(G47:AP47),1)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update WAR data - 2026-02-18
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -12486,7 +12486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI47"/>
+  <dimension ref="A1:CI46"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -12763,12 +12763,12 @@
       </c>
       <c r="AQ1" s="107" t="inlineStr">
         <is>
-          <t>Colonna43</t>
+          <t>WAR-19 (1)</t>
         </is>
       </c>
       <c r="AR1" s="112" t="inlineStr">
         <is>
-          <t>Colonna44</t>
+          <t>WAR-19 (2)</t>
         </is>
       </c>
       <c r="AS1" s="107" t="inlineStr">
@@ -13003,11 +13003,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="111">
-        <f>SUM(G2:AP2)</f>
+        <f>SUM(G2:AR2)</f>
         <v/>
       </c>
       <c r="F2" s="68">
-        <f>ROUND(AVERAGE(G2:AP2),1)</f>
+        <f>ROUND(AVERAGE(G2:AR2),1)</f>
         <v/>
       </c>
       <c r="G2" s="110" t="n"/>
@@ -13122,11 +13122,11 @@
         <v>0</v>
       </c>
       <c r="E3" s="68">
-        <f>SUM(G3:AP3)</f>
+        <f>SUM(G3:AR3)</f>
         <v/>
       </c>
       <c r="F3" s="68">
-        <f>ROUND(AVERAGE(G3:AP3),1)</f>
+        <f>ROUND(AVERAGE(G3:AR3),1)</f>
         <v/>
       </c>
     </row>
@@ -13146,11 +13146,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="68">
-        <f>SUM(G4:AP4)</f>
+        <f>SUM(G4:AR4)</f>
         <v/>
       </c>
       <c r="F4" s="68">
-        <f>ROUND(AVERAGE(G4:AP4),1)</f>
+        <f>ROUND(AVERAGE(G4:AR4),1)</f>
         <v/>
       </c>
       <c r="I4" s="79" t="n">
@@ -13198,11 +13198,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="68">
-        <f>SUM(G5:AP5)</f>
+        <f>SUM(G5:AR5)</f>
         <v/>
       </c>
       <c r="F5" s="68">
-        <f>ROUND(AVERAGE(G5:AP5),1)</f>
+        <f>ROUND(AVERAGE(G5:AR5),1)</f>
         <v/>
       </c>
       <c r="AO5" t="n">
@@ -13230,11 +13230,11 @@
         <v>4</v>
       </c>
       <c r="E6" s="68">
-        <f>SUM(G6:AP6)</f>
+        <f>SUM(G6:AR6)</f>
         <v/>
       </c>
       <c r="F6" s="68">
-        <f>ROUND(AVERAGE(G6:AP6),1)</f>
+        <f>ROUND(AVERAGE(G6:AR6),1)</f>
         <v/>
       </c>
       <c r="U6" s="79" t="n">
@@ -13280,11 +13280,11 @@
         <v>14</v>
       </c>
       <c r="E7" s="68">
-        <f>SUM(G7:AP7)</f>
+        <f>SUM(G7:AR7)</f>
         <v/>
       </c>
       <c r="F7" s="68">
-        <f>ROUND(AVERAGE(G7:AP7),1)</f>
+        <f>ROUND(AVERAGE(G7:AR7),1)</f>
         <v/>
       </c>
       <c r="G7" s="79" t="n">
@@ -13408,11 +13408,11 @@
         <v>5</v>
       </c>
       <c r="E8" s="68">
-        <f>SUM(G8:AP8)</f>
+        <f>SUM(G8:AR8)</f>
         <v/>
       </c>
       <c r="F8" s="68">
-        <f>ROUND(AVERAGE(G8:AP8),1)</f>
+        <f>ROUND(AVERAGE(G8:AR8),1)</f>
         <v/>
       </c>
       <c r="K8" s="79" t="n">
@@ -13462,11 +13462,11 @@
         <v>0</v>
       </c>
       <c r="E9" s="68">
-        <f>SUM(G9:AP9)</f>
+        <f>SUM(G9:AR9)</f>
         <v/>
       </c>
       <c r="F9" s="68">
-        <f>ROUND(AVERAGE(G9:AP9),1)</f>
+        <f>ROUND(AVERAGE(G9:AR9),1)</f>
         <v/>
       </c>
     </row>
@@ -13486,11 +13486,11 @@
         <v>12</v>
       </c>
       <c r="E10" s="68">
-        <f>SUM(G10:AP10)</f>
+        <f>SUM(G10:AR10)</f>
         <v/>
       </c>
       <c r="F10" s="68">
-        <f>ROUND(AVERAGE(G10:AP10),1)</f>
+        <f>ROUND(AVERAGE(G10:AR10),1)</f>
         <v/>
       </c>
       <c r="G10" s="79" t="n">
@@ -13582,11 +13582,11 @@
         <v>0</v>
       </c>
       <c r="E11" s="68">
-        <f>SUM(G11:AP11)</f>
+        <f>SUM(G11:AR11)</f>
         <v/>
       </c>
       <c r="F11" s="68">
-        <f>ROUND(AVERAGE(G11:AP11),1)</f>
+        <f>ROUND(AVERAGE(G11:AR11),1)</f>
         <v/>
       </c>
     </row>
@@ -13606,11 +13606,11 @@
         <v>6</v>
       </c>
       <c r="E12" s="68">
-        <f>SUM(G12:AP12)</f>
+        <f>SUM(G12:AR12)</f>
         <v/>
       </c>
       <c r="F12" s="68">
-        <f>ROUND(AVERAGE(G12:AP12),1)</f>
+        <f>ROUND(AVERAGE(G12:AR12),1)</f>
         <v/>
       </c>
       <c r="I12" s="79" t="n">
@@ -13680,11 +13680,11 @@
         <v>5</v>
       </c>
       <c r="E13" s="68">
-        <f>SUM(G13:AP13)</f>
+        <f>SUM(G13:AR13)</f>
         <v/>
       </c>
       <c r="F13" s="68">
-        <f>ROUND(AVERAGE(G13:AP13),1)</f>
+        <f>ROUND(AVERAGE(G13:AR13),1)</f>
         <v/>
       </c>
       <c r="Q13" s="79" t="n">
@@ -13736,11 +13736,11 @@
         <v>10</v>
       </c>
       <c r="E14" s="68">
-        <f>SUM(G14:AP14)</f>
+        <f>SUM(G14:AR14)</f>
         <v/>
       </c>
       <c r="F14" s="68">
-        <f>ROUND(AVERAGE(G14:AP14),1)</f>
+        <f>ROUND(AVERAGE(G14:AR14),1)</f>
         <v/>
       </c>
       <c r="G14" s="79" t="n">
@@ -13820,11 +13820,11 @@
         <v>0</v>
       </c>
       <c r="E15" s="68">
-        <f>SUM(G15:AP15)</f>
+        <f>SUM(G15:AR15)</f>
         <v/>
       </c>
       <c r="F15" s="68">
-        <f>ROUND(AVERAGE(G15:AP15),1)</f>
+        <f>ROUND(AVERAGE(G15:AR15),1)</f>
         <v/>
       </c>
     </row>
@@ -13844,11 +13844,11 @@
         <v>12</v>
       </c>
       <c r="E16" s="68">
-        <f>SUM(G16:AP16)</f>
+        <f>SUM(G16:AR16)</f>
         <v/>
       </c>
       <c r="F16" s="68">
-        <f>ROUND(AVERAGE(G16:AP16),1)</f>
+        <f>ROUND(AVERAGE(G16:AR16),1)</f>
         <v/>
       </c>
       <c r="I16" s="79" t="n">
@@ -13946,11 +13946,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="68">
-        <f>SUM(G17:AP17)</f>
+        <f>SUM(G17:AR17)</f>
         <v/>
       </c>
       <c r="F17" s="68">
-        <f>ROUND(AVERAGE(G17:AP17),1)</f>
+        <f>ROUND(AVERAGE(G17:AR17),1)</f>
         <v/>
       </c>
       <c r="AE17" s="79" t="n">
@@ -13976,11 +13976,11 @@
         <v>8</v>
       </c>
       <c r="E18" s="68">
-        <f>SUM(G18:AP18)</f>
+        <f>SUM(G18:AR18)</f>
         <v/>
       </c>
       <c r="F18" s="68">
-        <f>ROUND(AVERAGE(G18:AP18),1)</f>
+        <f>ROUND(AVERAGE(G18:AR18),1)</f>
         <v/>
       </c>
       <c r="S18" s="79" t="n">
@@ -14052,11 +14052,11 @@
         <v>3</v>
       </c>
       <c r="E19" s="68">
-        <f>SUM(G19:AP19)</f>
+        <f>SUM(G19:AR19)</f>
         <v/>
       </c>
       <c r="F19" s="68">
-        <f>ROUND(AVERAGE(G19:AP19),1)</f>
+        <f>ROUND(AVERAGE(G19:AR19),1)</f>
         <v/>
       </c>
       <c r="G19" s="79" t="n">
@@ -14094,11 +14094,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="68">
-        <f>SUM(G20:AP20)</f>
+        <f>SUM(G20:AR20)</f>
         <v/>
       </c>
       <c r="F20" s="68">
-        <f>ROUND(AVERAGE(G20:AP20),1)</f>
+        <f>ROUND(AVERAGE(G20:AR20),1)</f>
         <v/>
       </c>
       <c r="AE20" s="79" t="n">
@@ -14124,11 +14124,11 @@
         <v>8</v>
       </c>
       <c r="E21" s="68">
-        <f>SUM(G21:AP21)</f>
+        <f>SUM(G21:AR21)</f>
         <v/>
       </c>
       <c r="F21" s="68">
-        <f>ROUND(AVERAGE(G21:AP21),1)</f>
+        <f>ROUND(AVERAGE(G21:AR21),1)</f>
         <v/>
       </c>
       <c r="I21" s="79" t="n">
@@ -14200,11 +14200,11 @@
         <v>8</v>
       </c>
       <c r="E22" s="68">
-        <f>SUM(G22:AP22)</f>
+        <f>SUM(G22:AR22)</f>
         <v/>
       </c>
       <c r="F22" s="68">
-        <f>ROUND(AVERAGE(G22:AP22),1)</f>
+        <f>ROUND(AVERAGE(G22:AR22),1)</f>
         <v/>
       </c>
       <c r="G22" s="79" t="inlineStr">
@@ -14278,11 +14278,11 @@
         <v>10</v>
       </c>
       <c r="E23" s="68">
-        <f>SUM(G23:AP23)</f>
+        <f>SUM(G23:AR23)</f>
         <v/>
       </c>
       <c r="F23" s="68">
-        <f>ROUND(AVERAGE(G23:AP23),1)</f>
+        <f>ROUND(AVERAGE(G23:AR23),1)</f>
         <v/>
       </c>
       <c r="G23" s="79" t="n">
@@ -14376,11 +14376,11 @@
         <v>11</v>
       </c>
       <c r="E24" s="68">
-        <f>SUM(G24:AP24)</f>
+        <f>SUM(G24:AR24)</f>
         <v/>
       </c>
       <c r="F24" s="68">
-        <f>ROUND(AVERAGE(G24:AP24),1)</f>
+        <f>ROUND(AVERAGE(G24:AR24),1)</f>
         <v/>
       </c>
       <c r="G24" s="79" t="n">
@@ -14470,11 +14470,11 @@
         <v>8</v>
       </c>
       <c r="E25" s="68">
-        <f>SUM(G25:AP25)</f>
+        <f>SUM(G25:AR25)</f>
         <v/>
       </c>
       <c r="F25" s="68">
-        <f>ROUND(AVERAGE(G25:AP25),1)</f>
+        <f>ROUND(AVERAGE(G25:AR25),1)</f>
         <v/>
       </c>
       <c r="I25" s="79" t="n">
@@ -14552,11 +14552,11 @@
         <v>3</v>
       </c>
       <c r="E26" s="68">
-        <f>SUM(G26:AP26)</f>
+        <f>SUM(G26:AR26)</f>
         <v/>
       </c>
       <c r="F26" s="68">
-        <f>ROUND(AVERAGE(G26:AP26),1)</f>
+        <f>ROUND(AVERAGE(G26:AR26),1)</f>
         <v/>
       </c>
       <c r="Y26" s="79" t="n">
@@ -14596,11 +14596,11 @@
         <v>8</v>
       </c>
       <c r="E27" s="68">
-        <f>SUM(G27:AP27)</f>
+        <f>SUM(G27:AR27)</f>
         <v/>
       </c>
       <c r="F27" s="68">
-        <f>ROUND(AVERAGE(G27:AP27),1)</f>
+        <f>ROUND(AVERAGE(G27:AR27),1)</f>
         <v/>
       </c>
       <c r="S27" s="79" t="n">
@@ -14678,11 +14678,11 @@
         <v>10</v>
       </c>
       <c r="E28" s="68">
-        <f>SUM(G28:AP28)</f>
+        <f>SUM(G28:AR28)</f>
         <v/>
       </c>
       <c r="F28" s="68">
-        <f>ROUND(AVERAGE(G28:AP28),1)</f>
+        <f>ROUND(AVERAGE(G28:AR28),1)</f>
         <v/>
       </c>
       <c r="I28" s="79" t="inlineStr">
@@ -14776,11 +14776,11 @@
         <v>1</v>
       </c>
       <c r="E29" s="68">
-        <f>SUM(G29:AP29)</f>
+        <f>SUM(G29:AR29)</f>
         <v/>
       </c>
       <c r="F29" s="68">
-        <f>ROUND(AVERAGE(G29:AP29),1)</f>
+        <f>ROUND(AVERAGE(G29:AR29),1)</f>
         <v/>
       </c>
       <c r="AO29" t="n">
@@ -14806,11 +14806,11 @@
         <v>15</v>
       </c>
       <c r="E30" s="68">
-        <f>SUM(G30:AP30)</f>
+        <f>SUM(G30:AR30)</f>
         <v/>
       </c>
       <c r="F30" s="68">
-        <f>ROUND(AVERAGE(G30:AP30),1)</f>
+        <f>ROUND(AVERAGE(G30:AR30),1)</f>
         <v/>
       </c>
       <c r="G30" s="79" t="n">
@@ -14920,11 +14920,11 @@
         <v>4</v>
       </c>
       <c r="E31" s="68">
-        <f>SUM(G31:AP31)</f>
+        <f>SUM(G31:AR31)</f>
         <v/>
       </c>
       <c r="F31" s="68">
-        <f>ROUND(AVERAGE(G31:AP31),1)</f>
+        <f>ROUND(AVERAGE(G31:AR31),1)</f>
         <v/>
       </c>
       <c r="G31" s="79" t="n">
@@ -14968,11 +14968,11 @@
         <v>11</v>
       </c>
       <c r="E32" s="68">
-        <f>SUM(G32:AP32)</f>
+        <f>SUM(G32:AR32)</f>
         <v/>
       </c>
       <c r="F32" s="68">
-        <f>ROUND(AVERAGE(G32:AP32),1)</f>
+        <f>ROUND(AVERAGE(G32:AR32),1)</f>
         <v/>
       </c>
       <c r="G32" s="79" t="n">
@@ -15068,11 +15068,11 @@
         <v>0</v>
       </c>
       <c r="E33" s="68">
-        <f>SUM(G33:AP33)</f>
+        <f>SUM(G33:AR33)</f>
         <v/>
       </c>
       <c r="F33" s="68">
-        <f>ROUND(AVERAGE(G33:AP33),1)</f>
+        <f>ROUND(AVERAGE(G33:AR33),1)</f>
         <v/>
       </c>
     </row>
@@ -15092,11 +15092,11 @@
         <v>8</v>
       </c>
       <c r="E34" s="68">
-        <f>SUM(G34:AP34)</f>
+        <f>SUM(G34:AR34)</f>
         <v/>
       </c>
       <c r="F34" s="68">
-        <f>ROUND(AVERAGE(G34:AP34),1)</f>
+        <f>ROUND(AVERAGE(G34:AR34),1)</f>
         <v/>
       </c>
       <c r="O34" s="79" t="n">
@@ -15168,11 +15168,11 @@
         <v>2</v>
       </c>
       <c r="E35" s="68">
-        <f>SUM(G35:AP35)</f>
+        <f>SUM(G35:AR35)</f>
         <v/>
       </c>
       <c r="F35" s="68">
-        <f>ROUND(AVERAGE(G35:AP35),1)</f>
+        <f>ROUND(AVERAGE(G35:AR35),1)</f>
         <v/>
       </c>
       <c r="K35" s="79" t="inlineStr">
@@ -15208,11 +15208,11 @@
         <v>13</v>
       </c>
       <c r="E36" s="68">
-        <f>SUM(G36:AP36)</f>
+        <f>SUM(G36:AR36)</f>
         <v/>
       </c>
       <c r="F36" s="68">
-        <f>ROUND(AVERAGE(G36:AP36),1)</f>
+        <f>ROUND(AVERAGE(G36:AR36),1)</f>
         <v/>
       </c>
       <c r="G36" s="79" t="n">
@@ -15318,11 +15318,11 @@
         <v>10</v>
       </c>
       <c r="E37" s="68">
-        <f>SUM(G37:AP37)</f>
+        <f>SUM(G37:AR37)</f>
         <v/>
       </c>
       <c r="F37" s="68">
-        <f>ROUND(AVERAGE(G37:AP37),1)</f>
+        <f>ROUND(AVERAGE(G37:AR37),1)</f>
         <v/>
       </c>
       <c r="U37" s="79" t="n">
@@ -15410,11 +15410,11 @@
         <v>2</v>
       </c>
       <c r="E38" s="68">
-        <f>SUM(G38:AP38)</f>
+        <f>SUM(G38:AR38)</f>
         <v/>
       </c>
       <c r="F38" s="68">
-        <f>ROUND(AVERAGE(G38:AP38),1)</f>
+        <f>ROUND(AVERAGE(G38:AR38),1)</f>
         <v/>
       </c>
       <c r="AM38" t="n">
@@ -15448,11 +15448,11 @@
         <v>2</v>
       </c>
       <c r="E39" s="68">
-        <f>SUM(G39:AP39)</f>
+        <f>SUM(G39:AR39)</f>
         <v/>
       </c>
       <c r="F39" s="68">
-        <f>ROUND(AVERAGE(G39:AP39),1)</f>
+        <f>ROUND(AVERAGE(G39:AR39),1)</f>
         <v/>
       </c>
       <c r="AM39" t="n">
@@ -15484,11 +15484,11 @@
         <v>2</v>
       </c>
       <c r="E40" s="68">
-        <f>SUM(G40:AP40)</f>
+        <f>SUM(G40:AR40)</f>
         <v/>
       </c>
       <c r="F40" s="68">
-        <f>ROUND(AVERAGE(G40:AP40),1)</f>
+        <f>ROUND(AVERAGE(G40:AR40),1)</f>
         <v/>
       </c>
       <c r="AM40" t="n">
@@ -15520,11 +15520,11 @@
         <v>0</v>
       </c>
       <c r="E41" s="68">
-        <f>SUM(G41:AP41)</f>
+        <f>SUM(G41:AR41)</f>
         <v/>
       </c>
       <c r="F41" s="68">
-        <f>ROUND(AVERAGE(G41:AP41),1)</f>
+        <f>ROUND(AVERAGE(G41:AR41),1)</f>
         <v/>
       </c>
     </row>
@@ -15544,11 +15544,11 @@
         <v>2</v>
       </c>
       <c r="E42" s="68">
-        <f>SUM(G42:AP42)</f>
+        <f>SUM(G42:AR42)</f>
         <v/>
       </c>
       <c r="F42" s="68">
-        <f>ROUND(AVERAGE(G42:AP42),1)</f>
+        <f>ROUND(AVERAGE(G42:AR42),1)</f>
         <v/>
       </c>
       <c r="AM42" t="n">
@@ -15580,11 +15580,11 @@
         <v>2</v>
       </c>
       <c r="E43" s="68">
-        <f>SUM(G43:AP43)</f>
+        <f>SUM(G43:AR43)</f>
         <v/>
       </c>
       <c r="F43" s="68">
-        <f>ROUND(AVERAGE(G43:AP43),1)</f>
+        <f>ROUND(AVERAGE(G43:AR43),1)</f>
         <v/>
       </c>
       <c r="AM43" t="n">
@@ -15603,7 +15603,7 @@
     <row r="44">
       <c r="A44" s="79" t="inlineStr">
         <is>
-          <t>KingVanze98</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="B44" s="79" t="n">
@@ -15616,18 +15616,18 @@
         <v>0</v>
       </c>
       <c r="E44" s="68">
-        <f>SUM(G44:AP44)</f>
+        <f>SUM(G44:AR44)</f>
         <v/>
       </c>
       <c r="F44" s="68">
-        <f>ROUND(AVERAGE(G44:AP44),1)</f>
+        <f>ROUND(AVERAGE(G44:AR44),1)</f>
         <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="79" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>fede61mito</t>
         </is>
       </c>
       <c r="B45" s="79" t="n">
@@ -15640,18 +15640,18 @@
         <v>0</v>
       </c>
       <c r="E45" s="68">
-        <f>SUM(G45:AP45)</f>
+        <f>SUM(G45:AR45)</f>
         <v/>
       </c>
       <c r="F45" s="68">
-        <f>ROUND(AVERAGE(G45:AP45),1)</f>
+        <f>ROUND(AVERAGE(G45:AR45),1)</f>
         <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="79" t="inlineStr">
         <is>
-          <t>fede61mito</t>
+          <t>Dasters79</t>
         </is>
       </c>
       <c r="B46" s="79" t="n">
@@ -15664,35 +15664,11 @@
         <v>0</v>
       </c>
       <c r="E46" s="68">
-        <f>SUM(G46:AP46)</f>
+        <f>SUM(G46:AR46)</f>
         <v/>
       </c>
       <c r="F46" s="68">
-        <f>ROUND(AVERAGE(G46:AP46),1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="79" t="inlineStr">
-        <is>
-          <t>Dasters79</t>
-        </is>
-      </c>
-      <c r="B47" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="C47" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="68">
-        <f>SUM(G47:AP47)</f>
-        <v/>
-      </c>
-      <c r="F47" s="68">
-        <f>ROUND(AVERAGE(G47:AP47),1)</f>
+        <f>ROUND(AVERAGE(G46:AR46),1)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Update WAR data - 2026-02-20
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -12486,7 +12486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI46"/>
+  <dimension ref="A1:CI48"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -12773,12 +12773,12 @@
       </c>
       <c r="AS1" s="107" t="inlineStr">
         <is>
-          <t>Colonna45</t>
+          <t>WAR-20 (1)</t>
         </is>
       </c>
       <c r="AT1" s="112" t="inlineStr">
         <is>
-          <t>Colonna46</t>
+          <t>WAR-20 (2)</t>
         </is>
       </c>
       <c r="AU1" s="107" t="inlineStr">
@@ -13003,11 +13003,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="111">
-        <f>SUM(G2:AR2)</f>
+        <f>SUM(G2:AT2)</f>
         <v/>
       </c>
       <c r="F2" s="68">
-        <f>ROUND(AVERAGE(G2:AR2),1)</f>
+        <f>ROUND(AVERAGE(G2:AT2),1)</f>
         <v/>
       </c>
       <c r="G2" s="110" t="n"/>
@@ -13122,11 +13122,11 @@
         <v>0</v>
       </c>
       <c r="E3" s="68">
-        <f>SUM(G3:AR3)</f>
+        <f>SUM(G3:AT3)</f>
         <v/>
       </c>
       <c r="F3" s="68">
-        <f>ROUND(AVERAGE(G3:AR3),1)</f>
+        <f>ROUND(AVERAGE(G3:AT3),1)</f>
         <v/>
       </c>
     </row>
@@ -13146,11 +13146,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="68">
-        <f>SUM(G4:AR4)</f>
+        <f>SUM(G4:AT4)</f>
         <v/>
       </c>
       <c r="F4" s="68">
-        <f>ROUND(AVERAGE(G4:AR4),1)</f>
+        <f>ROUND(AVERAGE(G4:AT4),1)</f>
         <v/>
       </c>
       <c r="I4" s="79" t="n">
@@ -13198,11 +13198,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="68">
-        <f>SUM(G5:AR5)</f>
+        <f>SUM(G5:AT5)</f>
         <v/>
       </c>
       <c r="F5" s="68">
-        <f>ROUND(AVERAGE(G5:AR5),1)</f>
+        <f>ROUND(AVERAGE(G5:AT5),1)</f>
         <v/>
       </c>
       <c r="AO5" t="n">
@@ -13230,11 +13230,11 @@
         <v>4</v>
       </c>
       <c r="E6" s="68">
-        <f>SUM(G6:AR6)</f>
+        <f>SUM(G6:AT6)</f>
         <v/>
       </c>
       <c r="F6" s="68">
-        <f>ROUND(AVERAGE(G6:AR6),1)</f>
+        <f>ROUND(AVERAGE(G6:AT6),1)</f>
         <v/>
       </c>
       <c r="U6" s="79" t="n">
@@ -13280,11 +13280,11 @@
         <v>14</v>
       </c>
       <c r="E7" s="68">
-        <f>SUM(G7:AR7)</f>
+        <f>SUM(G7:AT7)</f>
         <v/>
       </c>
       <c r="F7" s="68">
-        <f>ROUND(AVERAGE(G7:AR7),1)</f>
+        <f>ROUND(AVERAGE(G7:AT7),1)</f>
         <v/>
       </c>
       <c r="G7" s="79" t="n">
@@ -13408,11 +13408,11 @@
         <v>5</v>
       </c>
       <c r="E8" s="68">
-        <f>SUM(G8:AR8)</f>
+        <f>SUM(G8:AT8)</f>
         <v/>
       </c>
       <c r="F8" s="68">
-        <f>ROUND(AVERAGE(G8:AR8),1)</f>
+        <f>ROUND(AVERAGE(G8:AT8),1)</f>
         <v/>
       </c>
       <c r="K8" s="79" t="n">
@@ -13462,11 +13462,11 @@
         <v>0</v>
       </c>
       <c r="E9" s="68">
-        <f>SUM(G9:AR9)</f>
+        <f>SUM(G9:AT9)</f>
         <v/>
       </c>
       <c r="F9" s="68">
-        <f>ROUND(AVERAGE(G9:AR9),1)</f>
+        <f>ROUND(AVERAGE(G9:AT9),1)</f>
         <v/>
       </c>
     </row>
@@ -13486,11 +13486,11 @@
         <v>12</v>
       </c>
       <c r="E10" s="68">
-        <f>SUM(G10:AR10)</f>
+        <f>SUM(G10:AT10)</f>
         <v/>
       </c>
       <c r="F10" s="68">
-        <f>ROUND(AVERAGE(G10:AR10),1)</f>
+        <f>ROUND(AVERAGE(G10:AT10),1)</f>
         <v/>
       </c>
       <c r="G10" s="79" t="n">
@@ -13582,11 +13582,11 @@
         <v>0</v>
       </c>
       <c r="E11" s="68">
-        <f>SUM(G11:AR11)</f>
+        <f>SUM(G11:AT11)</f>
         <v/>
       </c>
       <c r="F11" s="68">
-        <f>ROUND(AVERAGE(G11:AR11),1)</f>
+        <f>ROUND(AVERAGE(G11:AT11),1)</f>
         <v/>
       </c>
     </row>
@@ -13606,11 +13606,11 @@
         <v>6</v>
       </c>
       <c r="E12" s="68">
-        <f>SUM(G12:AR12)</f>
+        <f>SUM(G12:AT12)</f>
         <v/>
       </c>
       <c r="F12" s="68">
-        <f>ROUND(AVERAGE(G12:AR12),1)</f>
+        <f>ROUND(AVERAGE(G12:AT12),1)</f>
         <v/>
       </c>
       <c r="I12" s="79" t="n">
@@ -13677,14 +13677,14 @@
         <v>0</v>
       </c>
       <c r="D13" s="79" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" s="68">
-        <f>SUM(G13:AR13)</f>
+        <f>SUM(G13:AT13)</f>
         <v/>
       </c>
       <c r="F13" s="68">
-        <f>ROUND(AVERAGE(G13:AR13),1)</f>
+        <f>ROUND(AVERAGE(G13:AT13),1)</f>
         <v/>
       </c>
       <c r="Q13" s="79" t="n">
@@ -13718,6 +13718,12 @@
       </c>
       <c r="AF13" s="80" t="n">
         <v>1</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -13733,14 +13739,14 @@
         <v>0</v>
       </c>
       <c r="D14" s="79" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E14" s="68">
-        <f>SUM(G14:AR14)</f>
+        <f>SUM(G14:AT14)</f>
         <v/>
       </c>
       <c r="F14" s="68">
-        <f>ROUND(AVERAGE(G14:AR14),1)</f>
+        <f>ROUND(AVERAGE(G14:AT14),1)</f>
         <v/>
       </c>
       <c r="G14" s="79" t="n">
@@ -13801,6 +13807,12 @@
         <v>2</v>
       </c>
       <c r="AP14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT14" t="n">
         <v>2</v>
       </c>
     </row>
@@ -13820,11 +13832,11 @@
         <v>0</v>
       </c>
       <c r="E15" s="68">
-        <f>SUM(G15:AR15)</f>
+        <f>SUM(G15:AT15)</f>
         <v/>
       </c>
       <c r="F15" s="68">
-        <f>ROUND(AVERAGE(G15:AR15),1)</f>
+        <f>ROUND(AVERAGE(G15:AT15),1)</f>
         <v/>
       </c>
     </row>
@@ -13841,14 +13853,14 @@
         <v>1</v>
       </c>
       <c r="D16" s="79" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="68">
-        <f>SUM(G16:AR16)</f>
+        <f>SUM(G16:AT16)</f>
         <v/>
       </c>
       <c r="F16" s="68">
-        <f>ROUND(AVERAGE(G16:AR16),1)</f>
+        <f>ROUND(AVERAGE(G16:AT16),1)</f>
         <v/>
       </c>
       <c r="I16" s="79" t="n">
@@ -13928,6 +13940,12 @@
       </c>
       <c r="AP16" t="n">
         <v>1</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -13946,11 +13964,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="68">
-        <f>SUM(G17:AR17)</f>
+        <f>SUM(G17:AT17)</f>
         <v/>
       </c>
       <c r="F17" s="68">
-        <f>ROUND(AVERAGE(G17:AR17),1)</f>
+        <f>ROUND(AVERAGE(G17:AT17),1)</f>
         <v/>
       </c>
       <c r="AE17" s="79" t="n">
@@ -13976,11 +13994,11 @@
         <v>8</v>
       </c>
       <c r="E18" s="68">
-        <f>SUM(G18:AR18)</f>
+        <f>SUM(G18:AT18)</f>
         <v/>
       </c>
       <c r="F18" s="68">
-        <f>ROUND(AVERAGE(G18:AR18),1)</f>
+        <f>ROUND(AVERAGE(G18:AT18),1)</f>
         <v/>
       </c>
       <c r="S18" s="79" t="n">
@@ -14052,11 +14070,11 @@
         <v>3</v>
       </c>
       <c r="E19" s="68">
-        <f>SUM(G19:AR19)</f>
+        <f>SUM(G19:AT19)</f>
         <v/>
       </c>
       <c r="F19" s="68">
-        <f>ROUND(AVERAGE(G19:AR19),1)</f>
+        <f>ROUND(AVERAGE(G19:AT19),1)</f>
         <v/>
       </c>
       <c r="G19" s="79" t="n">
@@ -14094,11 +14112,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="68">
-        <f>SUM(G20:AR20)</f>
+        <f>SUM(G20:AT20)</f>
         <v/>
       </c>
       <c r="F20" s="68">
-        <f>ROUND(AVERAGE(G20:AR20),1)</f>
+        <f>ROUND(AVERAGE(G20:AT20),1)</f>
         <v/>
       </c>
       <c r="AE20" s="79" t="n">
@@ -14124,11 +14142,11 @@
         <v>8</v>
       </c>
       <c r="E21" s="68">
-        <f>SUM(G21:AR21)</f>
+        <f>SUM(G21:AT21)</f>
         <v/>
       </c>
       <c r="F21" s="68">
-        <f>ROUND(AVERAGE(G21:AR21),1)</f>
+        <f>ROUND(AVERAGE(G21:AT21),1)</f>
         <v/>
       </c>
       <c r="I21" s="79" t="n">
@@ -14197,14 +14215,14 @@
         <v>1</v>
       </c>
       <c r="D22" s="79" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22" s="68">
-        <f>SUM(G22:AR22)</f>
+        <f>SUM(G22:AT22)</f>
         <v/>
       </c>
       <c r="F22" s="68">
-        <f>ROUND(AVERAGE(G22:AR22),1)</f>
+        <f>ROUND(AVERAGE(G22:AT22),1)</f>
         <v/>
       </c>
       <c r="G22" s="79" t="inlineStr">
@@ -14259,6 +14277,12 @@
         <v>3</v>
       </c>
       <c r="AN22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT22" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14275,14 +14299,14 @@
         <v>1</v>
       </c>
       <c r="D23" s="79" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E23" s="68">
-        <f>SUM(G23:AR23)</f>
+        <f>SUM(G23:AT23)</f>
         <v/>
       </c>
       <c r="F23" s="68">
-        <f>ROUND(AVERAGE(G23:AR23),1)</f>
+        <f>ROUND(AVERAGE(G23:AT23),1)</f>
         <v/>
       </c>
       <c r="G23" s="79" t="n">
@@ -14358,6 +14382,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AS23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -14376,11 +14406,11 @@
         <v>11</v>
       </c>
       <c r="E24" s="68">
-        <f>SUM(G24:AR24)</f>
+        <f>SUM(G24:AT24)</f>
         <v/>
       </c>
       <c r="F24" s="68">
-        <f>ROUND(AVERAGE(G24:AR24),1)</f>
+        <f>ROUND(AVERAGE(G24:AT24),1)</f>
         <v/>
       </c>
       <c r="G24" s="79" t="n">
@@ -14470,11 +14500,11 @@
         <v>8</v>
       </c>
       <c r="E25" s="68">
-        <f>SUM(G25:AR25)</f>
+        <f>SUM(G25:AT25)</f>
         <v/>
       </c>
       <c r="F25" s="68">
-        <f>ROUND(AVERAGE(G25:AR25),1)</f>
+        <f>ROUND(AVERAGE(G25:AT25),1)</f>
         <v/>
       </c>
       <c r="I25" s="79" t="n">
@@ -14552,11 +14582,11 @@
         <v>3</v>
       </c>
       <c r="E26" s="68">
-        <f>SUM(G26:AR26)</f>
+        <f>SUM(G26:AT26)</f>
         <v/>
       </c>
       <c r="F26" s="68">
-        <f>ROUND(AVERAGE(G26:AR26),1)</f>
+        <f>ROUND(AVERAGE(G26:AT26),1)</f>
         <v/>
       </c>
       <c r="Y26" s="79" t="n">
@@ -14596,11 +14626,11 @@
         <v>8</v>
       </c>
       <c r="E27" s="68">
-        <f>SUM(G27:AR27)</f>
+        <f>SUM(G27:AT27)</f>
         <v/>
       </c>
       <c r="F27" s="68">
-        <f>ROUND(AVERAGE(G27:AR27),1)</f>
+        <f>ROUND(AVERAGE(G27:AT27),1)</f>
         <v/>
       </c>
       <c r="S27" s="79" t="n">
@@ -14678,11 +14708,11 @@
         <v>10</v>
       </c>
       <c r="E28" s="68">
-        <f>SUM(G28:AR28)</f>
+        <f>SUM(G28:AT28)</f>
         <v/>
       </c>
       <c r="F28" s="68">
-        <f>ROUND(AVERAGE(G28:AR28),1)</f>
+        <f>ROUND(AVERAGE(G28:AT28),1)</f>
         <v/>
       </c>
       <c r="I28" s="79" t="inlineStr">
@@ -14776,11 +14806,11 @@
         <v>1</v>
       </c>
       <c r="E29" s="68">
-        <f>SUM(G29:AR29)</f>
+        <f>SUM(G29:AT29)</f>
         <v/>
       </c>
       <c r="F29" s="68">
-        <f>ROUND(AVERAGE(G29:AR29),1)</f>
+        <f>ROUND(AVERAGE(G29:AT29),1)</f>
         <v/>
       </c>
       <c r="AO29" t="n">
@@ -14803,14 +14833,14 @@
         <v>0</v>
       </c>
       <c r="D30" s="79" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E30" s="68">
-        <f>SUM(G30:AR30)</f>
+        <f>SUM(G30:AT30)</f>
         <v/>
       </c>
       <c r="F30" s="68">
-        <f>ROUND(AVERAGE(G30:AR30),1)</f>
+        <f>ROUND(AVERAGE(G30:AT30),1)</f>
         <v/>
       </c>
       <c r="G30" s="79" t="n">
@@ -14901,6 +14931,12 @@
         <v>3</v>
       </c>
       <c r="AP30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT30" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14920,11 +14956,11 @@
         <v>4</v>
       </c>
       <c r="E31" s="68">
-        <f>SUM(G31:AR31)</f>
+        <f>SUM(G31:AT31)</f>
         <v/>
       </c>
       <c r="F31" s="68">
-        <f>ROUND(AVERAGE(G31:AR31),1)</f>
+        <f>ROUND(AVERAGE(G31:AT31),1)</f>
         <v/>
       </c>
       <c r="G31" s="79" t="n">
@@ -14965,14 +15001,14 @@
         <v>1</v>
       </c>
       <c r="D32" s="79" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E32" s="68">
-        <f>SUM(G32:AR32)</f>
+        <f>SUM(G32:AT32)</f>
         <v/>
       </c>
       <c r="F32" s="68">
-        <f>ROUND(AVERAGE(G32:AR32),1)</f>
+        <f>ROUND(AVERAGE(G32:AT32),1)</f>
         <v/>
       </c>
       <c r="G32" s="79" t="n">
@@ -15049,6 +15085,12 @@
         <v>2</v>
       </c>
       <c r="AN32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT32" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15065,15 +15107,21 @@
         <v>0</v>
       </c>
       <c r="D33" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="68">
-        <f>SUM(G33:AR33)</f>
+        <f>SUM(G33:AT33)</f>
         <v/>
       </c>
       <c r="F33" s="68">
-        <f>ROUND(AVERAGE(G33:AR33),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G33:AT33),1)</f>
+        <v/>
+      </c>
+      <c r="AS33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -15089,14 +15137,14 @@
         <v>1</v>
       </c>
       <c r="D34" s="79" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E34" s="68">
-        <f>SUM(G34:AR34)</f>
+        <f>SUM(G34:AT34)</f>
         <v/>
       </c>
       <c r="F34" s="68">
-        <f>ROUND(AVERAGE(G34:AR34),1)</f>
+        <f>ROUND(AVERAGE(G34:AT34),1)</f>
         <v/>
       </c>
       <c r="O34" s="79" t="n">
@@ -15150,6 +15198,12 @@
       </c>
       <c r="AP34" t="n">
         <v>1</v>
+      </c>
+      <c r="AS34" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT34" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -15168,11 +15222,11 @@
         <v>2</v>
       </c>
       <c r="E35" s="68">
-        <f>SUM(G35:AR35)</f>
+        <f>SUM(G35:AT35)</f>
         <v/>
       </c>
       <c r="F35" s="68">
-        <f>ROUND(AVERAGE(G35:AR35),1)</f>
+        <f>ROUND(AVERAGE(G35:AT35),1)</f>
         <v/>
       </c>
       <c r="K35" s="79" t="inlineStr">
@@ -15205,14 +15259,14 @@
         <v>2</v>
       </c>
       <c r="D36" s="79" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E36" s="68">
-        <f>SUM(G36:AR36)</f>
+        <f>SUM(G36:AT36)</f>
         <v/>
       </c>
       <c r="F36" s="68">
-        <f>ROUND(AVERAGE(G36:AR36),1)</f>
+        <f>ROUND(AVERAGE(G36:AT36),1)</f>
         <v/>
       </c>
       <c r="G36" s="79" t="n">
@@ -15299,6 +15353,12 @@
         <v>2</v>
       </c>
       <c r="AN36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT36" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15318,11 +15378,11 @@
         <v>10</v>
       </c>
       <c r="E37" s="68">
-        <f>SUM(G37:AR37)</f>
+        <f>SUM(G37:AT37)</f>
         <v/>
       </c>
       <c r="F37" s="68">
-        <f>ROUND(AVERAGE(G37:AR37),1)</f>
+        <f>ROUND(AVERAGE(G37:AT37),1)</f>
         <v/>
       </c>
       <c r="U37" s="79" t="n">
@@ -15407,14 +15467,14 @@
         <v>0</v>
       </c>
       <c r="D38" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E38" s="68">
-        <f>SUM(G38:AR38)</f>
+        <f>SUM(G38:AT38)</f>
         <v/>
       </c>
       <c r="F38" s="68">
-        <f>ROUND(AVERAGE(G38:AR38),1)</f>
+        <f>ROUND(AVERAGE(G38:AT38),1)</f>
         <v/>
       </c>
       <c r="AM38" t="n">
@@ -15430,6 +15490,12 @@
         <is>
           <t>SKIP</t>
         </is>
+      </c>
+      <c r="AS38" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT38" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -15445,14 +15511,14 @@
         <v>0</v>
       </c>
       <c r="D39" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E39" s="68">
-        <f>SUM(G39:AR39)</f>
+        <f>SUM(G39:AT39)</f>
         <v/>
       </c>
       <c r="F39" s="68">
-        <f>ROUND(AVERAGE(G39:AR39),1)</f>
+        <f>ROUND(AVERAGE(G39:AT39),1)</f>
         <v/>
       </c>
       <c r="AM39" t="n">
@@ -15466,6 +15532,12 @@
       </c>
       <c r="AP39" t="n">
         <v>3</v>
+      </c>
+      <c r="AS39" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT39" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -15481,14 +15553,14 @@
         <v>0</v>
       </c>
       <c r="D40" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E40" s="68">
-        <f>SUM(G40:AR40)</f>
+        <f>SUM(G40:AT40)</f>
         <v/>
       </c>
       <c r="F40" s="68">
-        <f>ROUND(AVERAGE(G40:AR40),1)</f>
+        <f>ROUND(AVERAGE(G40:AT40),1)</f>
         <v/>
       </c>
       <c r="AM40" t="n">
@@ -15502,6 +15574,12 @@
       </c>
       <c r="AP40" t="n">
         <v>2</v>
+      </c>
+      <c r="AS40" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT40" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="41">
@@ -15520,11 +15598,11 @@
         <v>0</v>
       </c>
       <c r="E41" s="68">
-        <f>SUM(G41:AR41)</f>
+        <f>SUM(G41:AT41)</f>
         <v/>
       </c>
       <c r="F41" s="68">
-        <f>ROUND(AVERAGE(G41:AR41),1)</f>
+        <f>ROUND(AVERAGE(G41:AT41),1)</f>
         <v/>
       </c>
     </row>
@@ -15541,14 +15619,14 @@
         <v>0</v>
       </c>
       <c r="D42" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E42" s="68">
-        <f>SUM(G42:AR42)</f>
+        <f>SUM(G42:AT42)</f>
         <v/>
       </c>
       <c r="F42" s="68">
-        <f>ROUND(AVERAGE(G42:AR42),1)</f>
+        <f>ROUND(AVERAGE(G42:AT42),1)</f>
         <v/>
       </c>
       <c r="AM42" t="n">
@@ -15562,6 +15640,12 @@
       </c>
       <c r="AP42" t="n">
         <v>2</v>
+      </c>
+      <c r="AS42" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT42" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -15577,14 +15661,14 @@
         <v>0</v>
       </c>
       <c r="D43" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" s="68">
-        <f>SUM(G43:AR43)</f>
+        <f>SUM(G43:AT43)</f>
         <v/>
       </c>
       <c r="F43" s="68">
-        <f>ROUND(AVERAGE(G43:AR43),1)</f>
+        <f>ROUND(AVERAGE(G43:AT43),1)</f>
         <v/>
       </c>
       <c r="AM43" t="n">
@@ -15598,12 +15682,18 @@
       </c>
       <c r="AP43" t="n">
         <v>3</v>
+      </c>
+      <c r="AS43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="79" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>fede61mito</t>
         </is>
       </c>
       <c r="B44" s="79" t="n">
@@ -15616,18 +15706,18 @@
         <v>0</v>
       </c>
       <c r="E44" s="68">
-        <f>SUM(G44:AR44)</f>
+        <f>SUM(G44:AT44)</f>
         <v/>
       </c>
       <c r="F44" s="68">
-        <f>ROUND(AVERAGE(G44:AR44),1)</f>
+        <f>ROUND(AVERAGE(G44:AT44),1)</f>
         <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="79" t="inlineStr">
         <is>
-          <t>fede61mito</t>
+          <t>Dasters79</t>
         </is>
       </c>
       <c r="B45" s="79" t="n">
@@ -15640,18 +15730,18 @@
         <v>0</v>
       </c>
       <c r="E45" s="68">
-        <f>SUM(G45:AR45)</f>
+        <f>SUM(G45:AT45)</f>
         <v/>
       </c>
       <c r="F45" s="68">
-        <f>ROUND(AVERAGE(G45:AR45),1)</f>
+        <f>ROUND(AVERAGE(G45:AT45),1)</f>
         <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="79" t="inlineStr">
         <is>
-          <t>Dasters79</t>
+          <t>Artur</t>
         </is>
       </c>
       <c r="B46" s="79" t="n">
@@ -15664,11 +15754,59 @@
         <v>0</v>
       </c>
       <c r="E46" s="68">
-        <f>SUM(G46:AR46)</f>
+        <f>SUM(G46:AT46)</f>
         <v/>
       </c>
       <c r="F46" s="68">
-        <f>ROUND(AVERAGE(G46:AR46),1)</f>
+        <f>ROUND(AVERAGE(G46:AT46),1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="79" t="inlineStr">
+        <is>
+          <t>Xx_Herman_xX</t>
+        </is>
+      </c>
+      <c r="B47" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="68">
+        <f>SUM(G47:AT47)</f>
+        <v/>
+      </c>
+      <c r="F47" s="68">
+        <f>ROUND(AVERAGE(G47:AT47),1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="79" t="inlineStr">
+        <is>
+          <t>dibba10</t>
+        </is>
+      </c>
+      <c r="B48" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="68">
+        <f>SUM(G48:AT48)</f>
+        <v/>
+      </c>
+      <c r="F48" s="68">
+        <f>ROUND(AVERAGE(G48:AT48),1)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Update WAR data - 2026-02-22
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -12486,7 +12486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI48"/>
+  <dimension ref="A1:CI51"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -12783,12 +12783,12 @@
       </c>
       <c r="AU1" s="107" t="inlineStr">
         <is>
-          <t>Colonna47</t>
+          <t>WAR-21 (1)</t>
         </is>
       </c>
       <c r="AV1" s="112" t="inlineStr">
         <is>
-          <t>Colonna48</t>
+          <t>WAR-21 (2)</t>
         </is>
       </c>
       <c r="AW1" s="107" t="inlineStr">
@@ -13003,11 +13003,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="111">
-        <f>SUM(G2:AT2)</f>
+        <f>SUM(G2:AV2)</f>
         <v/>
       </c>
       <c r="F2" s="68">
-        <f>ROUND(AVERAGE(G2:AT2),1)</f>
+        <f>ROUND(AVERAGE(G2:AV2),1)</f>
         <v/>
       </c>
       <c r="G2" s="110" t="n"/>
@@ -13122,11 +13122,11 @@
         <v>0</v>
       </c>
       <c r="E3" s="68">
-        <f>SUM(G3:AT3)</f>
+        <f>SUM(G3:AV3)</f>
         <v/>
       </c>
       <c r="F3" s="68">
-        <f>ROUND(AVERAGE(G3:AT3),1)</f>
+        <f>ROUND(AVERAGE(G3:AV3),1)</f>
         <v/>
       </c>
     </row>
@@ -13146,11 +13146,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="68">
-        <f>SUM(G4:AT4)</f>
+        <f>SUM(G4:AV4)</f>
         <v/>
       </c>
       <c r="F4" s="68">
-        <f>ROUND(AVERAGE(G4:AT4),1)</f>
+        <f>ROUND(AVERAGE(G4:AV4),1)</f>
         <v/>
       </c>
       <c r="I4" s="79" t="n">
@@ -13198,11 +13198,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="68">
-        <f>SUM(G5:AT5)</f>
+        <f>SUM(G5:AV5)</f>
         <v/>
       </c>
       <c r="F5" s="68">
-        <f>ROUND(AVERAGE(G5:AT5),1)</f>
+        <f>ROUND(AVERAGE(G5:AV5),1)</f>
         <v/>
       </c>
       <c r="AO5" t="n">
@@ -13230,11 +13230,11 @@
         <v>4</v>
       </c>
       <c r="E6" s="68">
-        <f>SUM(G6:AT6)</f>
+        <f>SUM(G6:AV6)</f>
         <v/>
       </c>
       <c r="F6" s="68">
-        <f>ROUND(AVERAGE(G6:AT6),1)</f>
+        <f>ROUND(AVERAGE(G6:AV6),1)</f>
         <v/>
       </c>
       <c r="U6" s="79" t="n">
@@ -13271,20 +13271,20 @@
         </is>
       </c>
       <c r="B7" s="79" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="68" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="79" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="68">
-        <f>SUM(G7:AT7)</f>
+        <f>SUM(G7:AV7)</f>
         <v/>
       </c>
       <c r="F7" s="68">
-        <f>ROUND(AVERAGE(G7:AT7),1)</f>
+        <f>ROUND(AVERAGE(G7:AV7),1)</f>
         <v/>
       </c>
       <c r="G7" s="79" t="n">
@@ -13387,6 +13387,16 @@
         <v>2</v>
       </c>
       <c r="AP7" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AU7" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AV7" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
@@ -13405,14 +13415,14 @@
         <v>0</v>
       </c>
       <c r="D8" s="79" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8" s="68">
-        <f>SUM(G8:AT8)</f>
+        <f>SUM(G8:AV8)</f>
         <v/>
       </c>
       <c r="F8" s="68">
-        <f>ROUND(AVERAGE(G8:AT8),1)</f>
+        <f>ROUND(AVERAGE(G8:AV8),1)</f>
         <v/>
       </c>
       <c r="K8" s="79" t="n">
@@ -13443,6 +13453,12 @@
         <v>3</v>
       </c>
       <c r="AN8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -13462,11 +13478,11 @@
         <v>0</v>
       </c>
       <c r="E9" s="68">
-        <f>SUM(G9:AT9)</f>
+        <f>SUM(G9:AV9)</f>
         <v/>
       </c>
       <c r="F9" s="68">
-        <f>ROUND(AVERAGE(G9:AT9),1)</f>
+        <f>ROUND(AVERAGE(G9:AV9),1)</f>
         <v/>
       </c>
     </row>
@@ -13483,14 +13499,14 @@
         <v>0</v>
       </c>
       <c r="D10" s="79" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="68">
-        <f>SUM(G10:AT10)</f>
+        <f>SUM(G10:AV10)</f>
         <v/>
       </c>
       <c r="F10" s="68">
-        <f>ROUND(AVERAGE(G10:AT10),1)</f>
+        <f>ROUND(AVERAGE(G10:AV10),1)</f>
         <v/>
       </c>
       <c r="G10" s="79" t="n">
@@ -13563,6 +13579,12 @@
         <v>3</v>
       </c>
       <c r="AN10" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV10" t="n">
         <v>3</v>
       </c>
     </row>
@@ -13582,11 +13604,11 @@
         <v>0</v>
       </c>
       <c r="E11" s="68">
-        <f>SUM(G11:AT11)</f>
+        <f>SUM(G11:AV11)</f>
         <v/>
       </c>
       <c r="F11" s="68">
-        <f>ROUND(AVERAGE(G11:AT11),1)</f>
+        <f>ROUND(AVERAGE(G11:AV11),1)</f>
         <v/>
       </c>
     </row>
@@ -13606,11 +13628,11 @@
         <v>6</v>
       </c>
       <c r="E12" s="68">
-        <f>SUM(G12:AT12)</f>
+        <f>SUM(G12:AV12)</f>
         <v/>
       </c>
       <c r="F12" s="68">
-        <f>ROUND(AVERAGE(G12:AT12),1)</f>
+        <f>ROUND(AVERAGE(G12:AV12),1)</f>
         <v/>
       </c>
       <c r="I12" s="79" t="n">
@@ -13680,11 +13702,11 @@
         <v>6</v>
       </c>
       <c r="E13" s="68">
-        <f>SUM(G13:AT13)</f>
+        <f>SUM(G13:AV13)</f>
         <v/>
       </c>
       <c r="F13" s="68">
-        <f>ROUND(AVERAGE(G13:AT13),1)</f>
+        <f>ROUND(AVERAGE(G13:AV13),1)</f>
         <v/>
       </c>
       <c r="Q13" s="79" t="n">
@@ -13739,14 +13761,14 @@
         <v>0</v>
       </c>
       <c r="D14" s="79" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="68">
-        <f>SUM(G14:AT14)</f>
+        <f>SUM(G14:AV14)</f>
         <v/>
       </c>
       <c r="F14" s="68">
-        <f>ROUND(AVERAGE(G14:AT14),1)</f>
+        <f>ROUND(AVERAGE(G14:AV14),1)</f>
         <v/>
       </c>
       <c r="G14" s="79" t="n">
@@ -13814,6 +13836,12 @@
       </c>
       <c r="AT14" t="n">
         <v>2</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -13832,11 +13860,11 @@
         <v>0</v>
       </c>
       <c r="E15" s="68">
-        <f>SUM(G15:AT15)</f>
+        <f>SUM(G15:AV15)</f>
         <v/>
       </c>
       <c r="F15" s="68">
-        <f>ROUND(AVERAGE(G15:AT15),1)</f>
+        <f>ROUND(AVERAGE(G15:AV15),1)</f>
         <v/>
       </c>
     </row>
@@ -13853,14 +13881,14 @@
         <v>1</v>
       </c>
       <c r="D16" s="79" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16" s="68">
-        <f>SUM(G16:AT16)</f>
+        <f>SUM(G16:AV16)</f>
         <v/>
       </c>
       <c r="F16" s="68">
-        <f>ROUND(AVERAGE(G16:AT16),1)</f>
+        <f>ROUND(AVERAGE(G16:AV16),1)</f>
         <v/>
       </c>
       <c r="I16" s="79" t="n">
@@ -13945,6 +13973,12 @@
         <v>3</v>
       </c>
       <c r="AT16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV16" t="n">
         <v>3</v>
       </c>
     </row>
@@ -13964,11 +13998,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="68">
-        <f>SUM(G17:AT17)</f>
+        <f>SUM(G17:AV17)</f>
         <v/>
       </c>
       <c r="F17" s="68">
-        <f>ROUND(AVERAGE(G17:AT17),1)</f>
+        <f>ROUND(AVERAGE(G17:AV17),1)</f>
         <v/>
       </c>
       <c r="AE17" s="79" t="n">
@@ -13991,14 +14025,14 @@
         <v>1</v>
       </c>
       <c r="D18" s="79" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" s="68">
-        <f>SUM(G18:AT18)</f>
+        <f>SUM(G18:AV18)</f>
         <v/>
       </c>
       <c r="F18" s="68">
-        <f>ROUND(AVERAGE(G18:AT18),1)</f>
+        <f>ROUND(AVERAGE(G18:AV18),1)</f>
         <v/>
       </c>
       <c r="S18" s="79" t="n">
@@ -14052,6 +14086,12 @@
       </c>
       <c r="AN18" t="n">
         <v>2</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV18" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -14070,11 +14110,11 @@
         <v>3</v>
       </c>
       <c r="E19" s="68">
-        <f>SUM(G19:AT19)</f>
+        <f>SUM(G19:AV19)</f>
         <v/>
       </c>
       <c r="F19" s="68">
-        <f>ROUND(AVERAGE(G19:AT19),1)</f>
+        <f>ROUND(AVERAGE(G19:AV19),1)</f>
         <v/>
       </c>
       <c r="G19" s="79" t="n">
@@ -14112,11 +14152,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="68">
-        <f>SUM(G20:AT20)</f>
+        <f>SUM(G20:AV20)</f>
         <v/>
       </c>
       <c r="F20" s="68">
-        <f>ROUND(AVERAGE(G20:AT20),1)</f>
+        <f>ROUND(AVERAGE(G20:AV20),1)</f>
         <v/>
       </c>
       <c r="AE20" s="79" t="n">
@@ -14139,14 +14179,14 @@
         <v>0</v>
       </c>
       <c r="D21" s="79" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" s="68">
-        <f>SUM(G21:AT21)</f>
+        <f>SUM(G21:AV21)</f>
         <v/>
       </c>
       <c r="F21" s="68">
-        <f>ROUND(AVERAGE(G21:AT21),1)</f>
+        <f>ROUND(AVERAGE(G21:AV21),1)</f>
         <v/>
       </c>
       <c r="I21" s="79" t="n">
@@ -14199,6 +14239,12 @@
         <v>0</v>
       </c>
       <c r="AP21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -14215,14 +14261,14 @@
         <v>1</v>
       </c>
       <c r="D22" s="79" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E22" s="68">
-        <f>SUM(G22:AT22)</f>
+        <f>SUM(G22:AV22)</f>
         <v/>
       </c>
       <c r="F22" s="68">
-        <f>ROUND(AVERAGE(G22:AT22),1)</f>
+        <f>ROUND(AVERAGE(G22:AV22),1)</f>
         <v/>
       </c>
       <c r="G22" s="79" t="inlineStr">
@@ -14284,6 +14330,12 @@
       </c>
       <c r="AT22" t="n">
         <v>3</v>
+      </c>
+      <c r="AU22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV22" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -14302,11 +14354,11 @@
         <v>11</v>
       </c>
       <c r="E23" s="68">
-        <f>SUM(G23:AT23)</f>
+        <f>SUM(G23:AV23)</f>
         <v/>
       </c>
       <c r="F23" s="68">
-        <f>ROUND(AVERAGE(G23:AT23),1)</f>
+        <f>ROUND(AVERAGE(G23:AV23),1)</f>
         <v/>
       </c>
       <c r="G23" s="79" t="n">
@@ -14406,11 +14458,11 @@
         <v>11</v>
       </c>
       <c r="E24" s="68">
-        <f>SUM(G24:AT24)</f>
+        <f>SUM(G24:AV24)</f>
         <v/>
       </c>
       <c r="F24" s="68">
-        <f>ROUND(AVERAGE(G24:AT24),1)</f>
+        <f>ROUND(AVERAGE(G24:AV24),1)</f>
         <v/>
       </c>
       <c r="G24" s="79" t="n">
@@ -14500,11 +14552,11 @@
         <v>8</v>
       </c>
       <c r="E25" s="68">
-        <f>SUM(G25:AT25)</f>
+        <f>SUM(G25:AV25)</f>
         <v/>
       </c>
       <c r="F25" s="68">
-        <f>ROUND(AVERAGE(G25:AT25),1)</f>
+        <f>ROUND(AVERAGE(G25:AV25),1)</f>
         <v/>
       </c>
       <c r="I25" s="79" t="n">
@@ -14582,11 +14634,11 @@
         <v>3</v>
       </c>
       <c r="E26" s="68">
-        <f>SUM(G26:AT26)</f>
+        <f>SUM(G26:AV26)</f>
         <v/>
       </c>
       <c r="F26" s="68">
-        <f>ROUND(AVERAGE(G26:AT26),1)</f>
+        <f>ROUND(AVERAGE(G26:AV26),1)</f>
         <v/>
       </c>
       <c r="Y26" s="79" t="n">
@@ -14626,11 +14678,11 @@
         <v>8</v>
       </c>
       <c r="E27" s="68">
-        <f>SUM(G27:AT27)</f>
+        <f>SUM(G27:AV27)</f>
         <v/>
       </c>
       <c r="F27" s="68">
-        <f>ROUND(AVERAGE(G27:AT27),1)</f>
+        <f>ROUND(AVERAGE(G27:AV27),1)</f>
         <v/>
       </c>
       <c r="S27" s="79" t="n">
@@ -14708,11 +14760,11 @@
         <v>10</v>
       </c>
       <c r="E28" s="68">
-        <f>SUM(G28:AT28)</f>
+        <f>SUM(G28:AV28)</f>
         <v/>
       </c>
       <c r="F28" s="68">
-        <f>ROUND(AVERAGE(G28:AT28),1)</f>
+        <f>ROUND(AVERAGE(G28:AV28),1)</f>
         <v/>
       </c>
       <c r="I28" s="79" t="inlineStr">
@@ -14806,11 +14858,11 @@
         <v>1</v>
       </c>
       <c r="E29" s="68">
-        <f>SUM(G29:AT29)</f>
+        <f>SUM(G29:AV29)</f>
         <v/>
       </c>
       <c r="F29" s="68">
-        <f>ROUND(AVERAGE(G29:AT29),1)</f>
+        <f>ROUND(AVERAGE(G29:AV29),1)</f>
         <v/>
       </c>
       <c r="AO29" t="n">
@@ -14833,14 +14885,14 @@
         <v>0</v>
       </c>
       <c r="D30" s="79" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="68">
-        <f>SUM(G30:AT30)</f>
+        <f>SUM(G30:AV30)</f>
         <v/>
       </c>
       <c r="F30" s="68">
-        <f>ROUND(AVERAGE(G30:AT30),1)</f>
+        <f>ROUND(AVERAGE(G30:AV30),1)</f>
         <v/>
       </c>
       <c r="G30" s="79" t="n">
@@ -14938,6 +14990,12 @@
       </c>
       <c r="AT30" t="n">
         <v>3</v>
+      </c>
+      <c r="AU30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV30" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -14953,14 +15011,14 @@
         <v>0</v>
       </c>
       <c r="D31" s="79" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E31" s="68">
-        <f>SUM(G31:AT31)</f>
+        <f>SUM(G31:AV31)</f>
         <v/>
       </c>
       <c r="F31" s="68">
-        <f>ROUND(AVERAGE(G31:AT31),1)</f>
+        <f>ROUND(AVERAGE(G31:AV31),1)</f>
         <v/>
       </c>
       <c r="G31" s="79" t="n">
@@ -14985,6 +15043,12 @@
         <v>3</v>
       </c>
       <c r="R31" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV31" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15004,11 +15068,11 @@
         <v>12</v>
       </c>
       <c r="E32" s="68">
-        <f>SUM(G32:AT32)</f>
+        <f>SUM(G32:AV32)</f>
         <v/>
       </c>
       <c r="F32" s="68">
-        <f>ROUND(AVERAGE(G32:AT32),1)</f>
+        <f>ROUND(AVERAGE(G32:AV32),1)</f>
         <v/>
       </c>
       <c r="G32" s="79" t="n">
@@ -15110,11 +15174,11 @@
         <v>1</v>
       </c>
       <c r="E33" s="68">
-        <f>SUM(G33:AT33)</f>
+        <f>SUM(G33:AV33)</f>
         <v/>
       </c>
       <c r="F33" s="68">
-        <f>ROUND(AVERAGE(G33:AT33),1)</f>
+        <f>ROUND(AVERAGE(G33:AV33),1)</f>
         <v/>
       </c>
       <c r="AS33" t="n">
@@ -15140,11 +15204,11 @@
         <v>9</v>
       </c>
       <c r="E34" s="68">
-        <f>SUM(G34:AT34)</f>
+        <f>SUM(G34:AV34)</f>
         <v/>
       </c>
       <c r="F34" s="68">
-        <f>ROUND(AVERAGE(G34:AT34),1)</f>
+        <f>ROUND(AVERAGE(G34:AV34),1)</f>
         <v/>
       </c>
       <c r="O34" s="79" t="n">
@@ -15222,11 +15286,11 @@
         <v>2</v>
       </c>
       <c r="E35" s="68">
-        <f>SUM(G35:AT35)</f>
+        <f>SUM(G35:AV35)</f>
         <v/>
       </c>
       <c r="F35" s="68">
-        <f>ROUND(AVERAGE(G35:AT35),1)</f>
+        <f>ROUND(AVERAGE(G35:AV35),1)</f>
         <v/>
       </c>
       <c r="K35" s="79" t="inlineStr">
@@ -15259,14 +15323,14 @@
         <v>2</v>
       </c>
       <c r="D36" s="79" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E36" s="68">
-        <f>SUM(G36:AT36)</f>
+        <f>SUM(G36:AV36)</f>
         <v/>
       </c>
       <c r="F36" s="68">
-        <f>ROUND(AVERAGE(G36:AT36),1)</f>
+        <f>ROUND(AVERAGE(G36:AV36),1)</f>
         <v/>
       </c>
       <c r="G36" s="79" t="n">
@@ -15359,6 +15423,12 @@
         <v>3</v>
       </c>
       <c r="AT36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV36" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15378,11 +15448,11 @@
         <v>10</v>
       </c>
       <c r="E37" s="68">
-        <f>SUM(G37:AT37)</f>
+        <f>SUM(G37:AV37)</f>
         <v/>
       </c>
       <c r="F37" s="68">
-        <f>ROUND(AVERAGE(G37:AT37),1)</f>
+        <f>ROUND(AVERAGE(G37:AV37),1)</f>
         <v/>
       </c>
       <c r="U37" s="79" t="n">
@@ -15467,14 +15537,14 @@
         <v>0</v>
       </c>
       <c r="D38" s="79" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E38" s="68">
-        <f>SUM(G38:AT38)</f>
+        <f>SUM(G38:AV38)</f>
         <v/>
       </c>
       <c r="F38" s="68">
-        <f>ROUND(AVERAGE(G38:AT38),1)</f>
+        <f>ROUND(AVERAGE(G38:AV38),1)</f>
         <v/>
       </c>
       <c r="AM38" t="n">
@@ -15496,6 +15566,12 @@
       </c>
       <c r="AT38" t="n">
         <v>3</v>
+      </c>
+      <c r="AU38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -15514,11 +15590,11 @@
         <v>3</v>
       </c>
       <c r="E39" s="68">
-        <f>SUM(G39:AT39)</f>
+        <f>SUM(G39:AV39)</f>
         <v/>
       </c>
       <c r="F39" s="68">
-        <f>ROUND(AVERAGE(G39:AT39),1)</f>
+        <f>ROUND(AVERAGE(G39:AV39),1)</f>
         <v/>
       </c>
       <c r="AM39" t="n">
@@ -15553,14 +15629,14 @@
         <v>0</v>
       </c>
       <c r="D40" s="79" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" s="68">
-        <f>SUM(G40:AT40)</f>
+        <f>SUM(G40:AV40)</f>
         <v/>
       </c>
       <c r="F40" s="68">
-        <f>ROUND(AVERAGE(G40:AT40),1)</f>
+        <f>ROUND(AVERAGE(G40:AV40),1)</f>
         <v/>
       </c>
       <c r="AM40" t="n">
@@ -15579,6 +15655,12 @@
         <v>3</v>
       </c>
       <c r="AT40" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU40" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV40" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15598,11 +15680,11 @@
         <v>0</v>
       </c>
       <c r="E41" s="68">
-        <f>SUM(G41:AT41)</f>
+        <f>SUM(G41:AV41)</f>
         <v/>
       </c>
       <c r="F41" s="68">
-        <f>ROUND(AVERAGE(G41:AT41),1)</f>
+        <f>ROUND(AVERAGE(G41:AV41),1)</f>
         <v/>
       </c>
     </row>
@@ -15622,11 +15704,11 @@
         <v>3</v>
       </c>
       <c r="E42" s="68">
-        <f>SUM(G42:AT42)</f>
+        <f>SUM(G42:AV42)</f>
         <v/>
       </c>
       <c r="F42" s="68">
-        <f>ROUND(AVERAGE(G42:AT42),1)</f>
+        <f>ROUND(AVERAGE(G42:AV42),1)</f>
         <v/>
       </c>
       <c r="AM42" t="n">
@@ -15661,14 +15743,14 @@
         <v>0</v>
       </c>
       <c r="D43" s="79" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E43" s="68">
-        <f>SUM(G43:AT43)</f>
+        <f>SUM(G43:AV43)</f>
         <v/>
       </c>
       <c r="F43" s="68">
-        <f>ROUND(AVERAGE(G43:AT43),1)</f>
+        <f>ROUND(AVERAGE(G43:AV43),1)</f>
         <v/>
       </c>
       <c r="AM43" t="n">
@@ -15688,6 +15770,12 @@
       </c>
       <c r="AT43" t="n">
         <v>0</v>
+      </c>
+      <c r="AU43" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV43" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="44">
@@ -15706,11 +15794,11 @@
         <v>0</v>
       </c>
       <c r="E44" s="68">
-        <f>SUM(G44:AT44)</f>
+        <f>SUM(G44:AV44)</f>
         <v/>
       </c>
       <c r="F44" s="68">
-        <f>ROUND(AVERAGE(G44:AT44),1)</f>
+        <f>ROUND(AVERAGE(G44:AV44),1)</f>
         <v/>
       </c>
     </row>
@@ -15730,11 +15818,11 @@
         <v>0</v>
       </c>
       <c r="E45" s="68">
-        <f>SUM(G45:AT45)</f>
+        <f>SUM(G45:AV45)</f>
         <v/>
       </c>
       <c r="F45" s="68">
-        <f>ROUND(AVERAGE(G45:AT45),1)</f>
+        <f>ROUND(AVERAGE(G45:AV45),1)</f>
         <v/>
       </c>
     </row>
@@ -15754,11 +15842,11 @@
         <v>0</v>
       </c>
       <c r="E46" s="68">
-        <f>SUM(G46:AT46)</f>
+        <f>SUM(G46:AV46)</f>
         <v/>
       </c>
       <c r="F46" s="68">
-        <f>ROUND(AVERAGE(G46:AT46),1)</f>
+        <f>ROUND(AVERAGE(G46:AV46),1)</f>
         <v/>
       </c>
     </row>
@@ -15778,11 +15866,11 @@
         <v>0</v>
       </c>
       <c r="E47" s="68">
-        <f>SUM(G47:AT47)</f>
+        <f>SUM(G47:AV47)</f>
         <v/>
       </c>
       <c r="F47" s="68">
-        <f>ROUND(AVERAGE(G47:AT47),1)</f>
+        <f>ROUND(AVERAGE(G47:AV47),1)</f>
         <v/>
       </c>
     </row>
@@ -15802,12 +15890,94 @@
         <v>0</v>
       </c>
       <c r="E48" s="68">
-        <f>SUM(G48:AT48)</f>
+        <f>SUM(G48:AV48)</f>
         <v/>
       </c>
       <c r="F48" s="68">
-        <f>ROUND(AVERAGE(G48:AT48),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G48:AV48),1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="79" t="inlineStr">
+        <is>
+          <t>SanBucaツ</t>
+        </is>
+      </c>
+      <c r="B49" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="68">
+        <f>SUM(G49:AV49)</f>
+        <v/>
+      </c>
+      <c r="F49" s="68">
+        <f>ROUND(AVERAGE(G49:AV49),1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="79" t="inlineStr">
+        <is>
+          <t>Anto</t>
+        </is>
+      </c>
+      <c r="B50" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="68">
+        <f>SUM(G50:AV50)</f>
+        <v/>
+      </c>
+      <c r="F50" s="68">
+        <f>ROUND(AVERAGE(G50:AV50),1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="79" t="inlineStr">
+        <is>
+          <t>Michele</t>
+        </is>
+      </c>
+      <c r="B51" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" s="68">
+        <f>SUM(G51:AV51)</f>
+        <v/>
+      </c>
+      <c r="F51" s="68">
+        <f>ROUND(AVERAGE(G51:AV51),1)</f>
+        <v/>
+      </c>
+      <c r="AU51" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AV51" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update WAR data - 2026-02-25
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -12793,12 +12793,12 @@
       </c>
       <c r="AW1" s="107" t="inlineStr">
         <is>
-          <t>Colonna49</t>
+          <t>WAR-22 (1)</t>
         </is>
       </c>
       <c r="AX1" s="112" t="inlineStr">
         <is>
-          <t>Colonna50</t>
+          <t>WAR-22 (2)</t>
         </is>
       </c>
       <c r="AY1" s="109" t="inlineStr">
@@ -13003,11 +13003,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="111">
-        <f>SUM(G2:AV2)</f>
+        <f>SUM(G2:AX2)</f>
         <v/>
       </c>
       <c r="F2" s="68">
-        <f>ROUND(AVERAGE(G2:AV2),1)</f>
+        <f>ROUND(AVERAGE(G2:AX2),1)</f>
         <v/>
       </c>
       <c r="G2" s="110" t="n"/>
@@ -13122,11 +13122,11 @@
         <v>0</v>
       </c>
       <c r="E3" s="68">
-        <f>SUM(G3:AV3)</f>
+        <f>SUM(G3:AX3)</f>
         <v/>
       </c>
       <c r="F3" s="68">
-        <f>ROUND(AVERAGE(G3:AV3),1)</f>
+        <f>ROUND(AVERAGE(G3:AX3),1)</f>
         <v/>
       </c>
     </row>
@@ -13146,11 +13146,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="68">
-        <f>SUM(G4:AV4)</f>
+        <f>SUM(G4:AX4)</f>
         <v/>
       </c>
       <c r="F4" s="68">
-        <f>ROUND(AVERAGE(G4:AV4),1)</f>
+        <f>ROUND(AVERAGE(G4:AX4),1)</f>
         <v/>
       </c>
       <c r="I4" s="79" t="n">
@@ -13198,11 +13198,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="68">
-        <f>SUM(G5:AV5)</f>
+        <f>SUM(G5:AX5)</f>
         <v/>
       </c>
       <c r="F5" s="68">
-        <f>ROUND(AVERAGE(G5:AV5),1)</f>
+        <f>ROUND(AVERAGE(G5:AX5),1)</f>
         <v/>
       </c>
       <c r="AO5" t="n">
@@ -13217,48 +13217,136 @@
     <row r="6">
       <c r="A6" s="79" t="inlineStr">
         <is>
-          <t>andriu07</t>
+          <t>BigMc23</t>
         </is>
       </c>
       <c r="B6" s="79" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C6" s="68" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="79" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E6" s="68">
-        <f>SUM(G6:AV6)</f>
+        <f>SUM(G6:AX6)</f>
         <v/>
       </c>
       <c r="F6" s="68">
-        <f>ROUND(AVERAGE(G6:AV6),1)</f>
-        <v/>
-      </c>
-      <c r="U6" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="V6" s="80" t="n">
-        <v>1</v>
+        <f>ROUND(AVERAGE(G6:AX6),1)</f>
+        <v/>
+      </c>
+      <c r="G6" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="R6" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="W6" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="X6" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
       <c r="Y6" s="79" t="n">
         <v>3</v>
       </c>
       <c r="Z6" s="80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA6" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB6" s="80" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AC6" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AD6" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
       <c r="AM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AV6" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
@@ -13267,145 +13355,67 @@
     <row r="7">
       <c r="A7" s="79" t="inlineStr">
         <is>
-          <t>BigMc23</t>
+          <t>buff x-bow</t>
         </is>
       </c>
       <c r="B7" s="79" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C7" s="68" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D7" s="79" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E7" s="68">
-        <f>SUM(G7:AV7)</f>
+        <f>SUM(G7:AX7)</f>
         <v/>
       </c>
       <c r="F7" s="68">
-        <f>ROUND(AVERAGE(G7:AV7),1)</f>
-        <v/>
-      </c>
-      <c r="G7" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="80" t="n">
-        <v>0</v>
+        <f>ROUND(AVERAGE(G7:AX7),1)</f>
+        <v/>
       </c>
       <c r="K7" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L7" s="80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M7" s="79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N7" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="P7" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="79" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="R7" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="W7" s="79" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="X7" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="Y7" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z7" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA7" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB7" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC7" s="79" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AD7" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AI7" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ7" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL7" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="Q7" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R7" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="80" t="n">
+        <v>2</v>
       </c>
       <c r="AM7" t="n">
         <v>3</v>
       </c>
       <c r="AN7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP7" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AU7" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AV7" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="79" t="inlineStr">
         <is>
-          <t>buff x-bow</t>
+          <t>Chabby</t>
         </is>
       </c>
       <c r="B8" s="79" t="n">
@@ -13415,57 +13425,21 @@
         <v>0</v>
       </c>
       <c r="D8" s="79" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E8" s="68">
-        <f>SUM(G8:AV8)</f>
+        <f>SUM(G8:AX8)</f>
         <v/>
       </c>
       <c r="F8" s="68">
-        <f>ROUND(AVERAGE(G8:AV8),1)</f>
-        <v/>
-      </c>
-      <c r="K8" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L8" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M8" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="N8" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R8" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC8" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD8" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU8" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV8" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G8:AX8),1)</f>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="79" t="inlineStr">
         <is>
-          <t>Chabby</t>
+          <t>dado</t>
         </is>
       </c>
       <c r="B9" s="79" t="n">
@@ -13475,21 +13449,99 @@
         <v>0</v>
       </c>
       <c r="D9" s="79" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E9" s="68">
-        <f>SUM(G9:AV9)</f>
+        <f>SUM(G9:AX9)</f>
         <v/>
       </c>
       <c r="F9" s="68">
-        <f>ROUND(AVERAGE(G9:AV9),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G9:AX9),1)</f>
+        <v/>
+      </c>
+      <c r="G9" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="L9" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="O9" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P9" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R9" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="S9" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="T9" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="U9" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V9" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="W9" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="X9" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB9" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="79" t="inlineStr">
         <is>
-          <t>dado</t>
+          <t>EdoDodo</t>
         </is>
       </c>
       <c r="B10" s="79" t="n">
@@ -13499,259 +13551,253 @@
         <v>0</v>
       </c>
       <c r="D10" s="79" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E10" s="68">
-        <f>SUM(G10:AV10)</f>
+        <f>SUM(G10:AX10)</f>
         <v/>
       </c>
       <c r="F10" s="68">
-        <f>ROUND(AVERAGE(G10:AV10),1)</f>
-        <v/>
-      </c>
-      <c r="G10" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="H10" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="I10" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="J10" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="L10" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="O10" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P10" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R10" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="S10" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="T10" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="U10" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V10" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W10" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X10" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y10" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB10" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC10" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD10" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM10" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN10" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU10" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV10" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G10:AX10),1)</f>
+        <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="79" t="inlineStr">
         <is>
-          <t>EdoDodo</t>
+          <t>ER DANDI 1927</t>
         </is>
       </c>
       <c r="B11" s="79" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C11" s="68" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11" s="79" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E11" s="68">
-        <f>SUM(G11:AV11)</f>
+        <f>SUM(G11:AX11)</f>
         <v/>
       </c>
       <c r="F11" s="68">
-        <f>ROUND(AVERAGE(G11:AV11),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G11:AX11),1)</f>
+        <v/>
+      </c>
+      <c r="I11" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="O11" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="P11" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="S11" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="T11" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM11" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AN11" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="79" t="inlineStr">
         <is>
-          <t>ER DANDI 1927</t>
+          <t>Floky23</t>
         </is>
       </c>
       <c r="B12" s="79" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C12" s="68" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12" s="79" t="n">
         <v>6</v>
       </c>
       <c r="E12" s="68">
-        <f>SUM(G12:AV12)</f>
+        <f>SUM(G12:AX12)</f>
         <v/>
       </c>
       <c r="F12" s="68">
-        <f>ROUND(AVERAGE(G12:AV12),1)</f>
-        <v/>
-      </c>
-      <c r="I12" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="J12" s="80" t="inlineStr">
+        <f>ROUND(AVERAGE(G12:AX12),1)</f>
+        <v/>
+      </c>
+      <c r="Q12" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R12" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="U12" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V12" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="O12" s="79" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="P12" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="S12" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="T12" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI12" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ12" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK12" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL12" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM12" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AN12" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+      <c r="AE12" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF12" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="79" t="inlineStr">
         <is>
-          <t>Floky23</t>
+          <t>gionny</t>
         </is>
       </c>
       <c r="B13" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D13" s="79" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E13" s="68">
-        <f>SUM(G13:AV13)</f>
+        <f>SUM(G13:AX13)</f>
         <v/>
       </c>
       <c r="F13" s="68">
-        <f>ROUND(AVERAGE(G13:AV13),1)</f>
-        <v/>
-      </c>
-      <c r="Q13" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R13" s="80" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G13:AX13),1)</f>
+        <v/>
+      </c>
+      <c r="G13" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="M13" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="O13" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P13" s="80" t="n">
+        <v>3</v>
       </c>
       <c r="U13" s="79" t="n">
         <v>3</v>
       </c>
       <c r="V13" s="80" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="W13" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="X13" s="80" t="n">
+        <v>2</v>
       </c>
       <c r="Y13" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z13" s="80" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA13" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB13" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AE13" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF13" s="80" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AB13" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>2</v>
       </c>
       <c r="AS13" t="n">
         <v>1</v>
       </c>
       <c r="AT13" t="n">
         <v>2</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="79" t="inlineStr">
         <is>
-          <t>gionny</t>
+          <t>Giorgio</t>
         </is>
       </c>
       <c r="B14" s="79" t="n">
@@ -13761,343 +13807,289 @@
         <v>0</v>
       </c>
       <c r="D14" s="79" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E14" s="68">
-        <f>SUM(G14:AV14)</f>
+        <f>SUM(G14:AX14)</f>
         <v/>
       </c>
       <c r="F14" s="68">
-        <f>ROUND(AVERAGE(G14:AV14),1)</f>
-        <v/>
-      </c>
-      <c r="G14" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M14" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="O14" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P14" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U14" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V14" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W14" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="X14" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y14" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z14" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB14" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AS14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AU14" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV14" t="n">
-        <v>1</v>
+        <f>ROUND(AVERAGE(G14:AX14),1)</f>
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="79" t="inlineStr">
         <is>
-          <t>Giorgio</t>
+          <t>GiornoBrando</t>
         </is>
       </c>
       <c r="B15" s="79" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C15" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="79" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E15" s="68">
-        <f>SUM(G15:AV15)</f>
+        <f>SUM(G15:AX15)</f>
         <v/>
       </c>
       <c r="F15" s="68">
-        <f>ROUND(AVERAGE(G15:AV15),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G15:AX15),1)</f>
+        <v/>
+      </c>
+      <c r="I15" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="O15" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P15" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R15" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U15" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V15" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB15" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC15" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD15" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF15" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AI15" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV15" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="79" t="inlineStr">
         <is>
-          <t>GiornoBrando</t>
+          <t>GioStyle</t>
         </is>
       </c>
       <c r="B16" s="79" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="79" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E16" s="68">
-        <f>SUM(G16:AV16)</f>
+        <f>SUM(G16:AX16)</f>
         <v/>
       </c>
       <c r="F16" s="68">
-        <f>ROUND(AVERAGE(G16:AV16),1)</f>
-        <v/>
-      </c>
-      <c r="I16" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="J16" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L16" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="O16" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P16" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R16" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U16" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V16" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB16" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC16" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD16" s="80" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G16:AX16),1)</f>
+        <v/>
       </c>
       <c r="AE16" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="AF16" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AI16" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ16" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK16" t="n">
-        <v>3</v>
-      </c>
-      <c r="AL16" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM16" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN16" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS16" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT16" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU16" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV16" t="n">
+      <c r="AF16" s="80" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="79" t="inlineStr">
         <is>
-          <t>GioStyle</t>
+          <t>haha</t>
         </is>
       </c>
       <c r="B17" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="79" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E17" s="68">
-        <f>SUM(G17:AV17)</f>
+        <f>SUM(G17:AX17)</f>
         <v/>
       </c>
       <c r="F17" s="68">
-        <f>ROUND(AVERAGE(G17:AV17),1)</f>
-        <v/>
-      </c>
-      <c r="AE17" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF17" s="80" t="n">
+        <f>ROUND(AVERAGE(G17:AX17),1)</f>
+        <v/>
+      </c>
+      <c r="S17" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="T17" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="W17" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X17" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y17" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z17" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA17" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB17" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI17" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK17" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV17" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="79" t="inlineStr">
         <is>
-          <t>haha</t>
+          <t>HikariNoRob</t>
         </is>
       </c>
       <c r="B18" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="79" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E18" s="68">
-        <f>SUM(G18:AV18)</f>
+        <f>SUM(G18:AX18)</f>
         <v/>
       </c>
       <c r="F18" s="68">
-        <f>ROUND(AVERAGE(G18:AV18),1)</f>
-        <v/>
-      </c>
-      <c r="S18" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="T18" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W18" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X18" s="80" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G18:AX18),1)</f>
+        <v/>
+      </c>
+      <c r="G18" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="J18" s="80" t="n">
+        <v>3</v>
       </c>
       <c r="Y18" s="79" t="n">
         <v>3</v>
       </c>
       <c r="Z18" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA18" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB18" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC18" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD18" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AI18" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ18" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK18" t="n">
-        <v>3</v>
-      </c>
-      <c r="AL18" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM18" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN18" t="n">
-        <v>2</v>
-      </c>
-      <c r="AU18" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV18" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="79" t="inlineStr">
         <is>
-          <t>HikariNoRob</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B19" s="79" t="n">
@@ -14107,245 +14099,307 @@
         <v>0</v>
       </c>
       <c r="D19" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" s="68">
-        <f>SUM(G19:AV19)</f>
+        <f>SUM(G19:AX19)</f>
         <v/>
       </c>
       <c r="F19" s="68">
-        <f>ROUND(AVERAGE(G19:AV19),1)</f>
-        <v/>
-      </c>
-      <c r="G19" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="I19" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="J19" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y19" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z19" s="80" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G19:AX19),1)</f>
+        <v/>
+      </c>
+      <c r="AE19" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF19" s="80" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="79" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>Luigi</t>
         </is>
       </c>
       <c r="B20" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C20" s="68" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="79" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E20" s="68">
-        <f>SUM(G20:AV20)</f>
+        <f>SUM(G20:AX20)</f>
         <v/>
       </c>
       <c r="F20" s="68">
-        <f>ROUND(AVERAGE(G20:AV20),1)</f>
-        <v/>
-      </c>
-      <c r="AE20" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF20" s="80" t="n">
+        <f>ROUND(AVERAGE(G20:AX20),1)</f>
+        <v/>
+      </c>
+      <c r="I20" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="M20" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="N20" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P20" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="R20" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="W20" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X20" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA20" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB20" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC20" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD20" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU20" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="79" t="inlineStr">
         <is>
-          <t>Luigi</t>
+          <t>Luxor</t>
         </is>
       </c>
       <c r="B21" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="79" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E21" s="68">
-        <f>SUM(G21:AV21)</f>
+        <f>SUM(G21:AX21)</f>
         <v/>
       </c>
       <c r="F21" s="68">
-        <f>ROUND(AVERAGE(G21:AV21),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G21:AX21),1)</f>
+        <v/>
+      </c>
+      <c r="G21" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="H21" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
       <c r="I21" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="J21" s="80" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="J21" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="K21" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L21" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U21" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V21" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="W21" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X21" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="M21" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="N21" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="O21" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P21" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="R21" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="W21" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X21" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA21" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB21" s="80" t="n">
-        <v>2</v>
+      <c r="Y21" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="80" t="n">
+        <v>3</v>
       </c>
       <c r="AC21" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD21" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="AO21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP21" t="n">
-        <v>1</v>
+      <c r="AM21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT21" t="n">
+        <v>3</v>
       </c>
       <c r="AU21" t="n">
         <v>3</v>
       </c>
       <c r="AV21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="79" t="inlineStr">
         <is>
-          <t>Luxor</t>
+          <t>maikol_lix</t>
         </is>
       </c>
       <c r="B22" s="79" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C22" s="68" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="79" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E22" s="68">
-        <f>SUM(G22:AV22)</f>
+        <f>SUM(G22:AX22)</f>
         <v/>
       </c>
       <c r="F22" s="68">
-        <f>ROUND(AVERAGE(G22:AV22),1)</f>
-        <v/>
-      </c>
-      <c r="G22" s="79" t="inlineStr">
+        <f>ROUND(AVERAGE(G22:AX22),1)</f>
+        <v/>
+      </c>
+      <c r="G22" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="H22" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="J22" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="O22" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P22" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="H22" s="80" t="inlineStr">
+      <c r="S22" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="T22" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="I22" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="J22" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="K22" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L22" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U22" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V22" s="80" t="n">
-        <v>3</v>
-      </c>
       <c r="W22" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X22" s="80" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="X22" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA22" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB22" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="Y22" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z22" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC22" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD22" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM22" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN22" t="n">
-        <v>3</v>
+      <c r="AE22" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF22" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AI22" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ22" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP22" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
       <c r="AS22" t="n">
         <v>3</v>
       </c>
       <c r="AT22" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU22" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV22" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="79" t="inlineStr">
         <is>
-          <t>maikol_lix</t>
+          <t>piegian99</t>
         </is>
       </c>
       <c r="B23" s="79" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C23" s="68" t="n">
         <v>1</v>
@@ -14354,98 +14408,88 @@
         <v>11</v>
       </c>
       <c r="E23" s="68">
-        <f>SUM(G23:AV23)</f>
+        <f>SUM(G23:AX23)</f>
         <v/>
       </c>
       <c r="F23" s="68">
-        <f>ROUND(AVERAGE(G23:AV23),1)</f>
+        <f>ROUND(AVERAGE(G23:AX23),1)</f>
         <v/>
       </c>
       <c r="G23" s="79" t="n">
         <v>3</v>
       </c>
       <c r="H23" s="80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I23" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J23" s="80" t="n">
         <v>3</v>
       </c>
+      <c r="K23" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L23" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="M23" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="N23" s="80" t="n">
+        <v>2</v>
+      </c>
       <c r="O23" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="P23" s="80" t="inlineStr">
+      <c r="P23" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R23" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="S23" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="T23" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U23" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V23" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE23" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF23" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI23" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="S23" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="T23" s="80" t="inlineStr">
+      <c r="AJ23" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="W23" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X23" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA23" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB23" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AE23" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF23" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AI23" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ23" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
       <c r="AK23" t="n">
         <v>3</v>
       </c>
       <c r="AL23" t="n">
         <v>3</v>
-      </c>
-      <c r="AO23" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP23" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AS23" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT23" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="79" t="inlineStr">
         <is>
-          <t>piegian99</t>
+          <t>pigiamone99</t>
         </is>
       </c>
       <c r="B24" s="79" t="n">
@@ -14455,39 +14499,27 @@
         <v>1</v>
       </c>
       <c r="D24" s="79" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E24" s="68">
-        <f>SUM(G24:AV24)</f>
+        <f>SUM(G24:AX24)</f>
         <v/>
       </c>
       <c r="F24" s="68">
-        <f>ROUND(AVERAGE(G24:AV24),1)</f>
-        <v/>
-      </c>
-      <c r="G24" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="H24" s="80" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G24:AX24),1)</f>
+        <v/>
       </c>
       <c r="I24" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J24" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="K24" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L24" s="80" t="n">
-        <v>3</v>
-      </c>
       <c r="M24" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N24" s="80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O24" s="79" t="n">
         <v>3</v>
@@ -14501,23 +14533,23 @@
       <c r="R24" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="S24" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="T24" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U24" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V24" s="80" t="n">
+      <c r="W24" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="X24" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y24" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z24" s="80" t="n">
         <v>3</v>
       </c>
       <c r="AE24" s="79" t="n">
         <v>3</v>
       </c>
       <c r="AF24" s="80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AI24" t="inlineStr">
         <is>
@@ -14539,168 +14571,190 @@
     <row r="25">
       <c r="A25" s="79" t="inlineStr">
         <is>
-          <t>pigiamone99</t>
+          <t>PIPPII</t>
         </is>
       </c>
       <c r="B25" s="79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="79" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E25" s="68">
-        <f>SUM(G25:AV25)</f>
+        <f>SUM(G25:AX25)</f>
         <v/>
       </c>
       <c r="F25" s="68">
-        <f>ROUND(AVERAGE(G25:AV25),1)</f>
-        <v/>
-      </c>
-      <c r="I25" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="J25" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M25" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="N25" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="O25" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P25" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q25" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R25" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W25" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X25" s="80" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G25:AX25),1)</f>
+        <v/>
       </c>
       <c r="Y25" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z25" s="80" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="Z25" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AC25" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD25" s="80" t="n">
+        <v>2</v>
       </c>
       <c r="AE25" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF25" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AI25" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ25" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK25" t="n">
-        <v>3</v>
-      </c>
-      <c r="AL25" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="79" t="inlineStr">
         <is>
-          <t>PIPPII</t>
+          <t>revolver</t>
         </is>
       </c>
       <c r="B26" s="79" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C26" s="68" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26" s="79" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E26" s="68">
-        <f>SUM(G26:AV26)</f>
+        <f>SUM(G26:AX26)</f>
         <v/>
       </c>
       <c r="F26" s="68">
-        <f>ROUND(AVERAGE(G26:AV26),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G26:AX26),1)</f>
+        <v/>
+      </c>
+      <c r="S26" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="T26" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U26" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="V26" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="W26" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="X26" s="80" t="n">
+        <v>3</v>
       </c>
       <c r="Y26" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z26" s="80" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="Z26" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC26" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD26" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE26" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF26" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI26" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="AC26" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD26" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE26" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF26" s="80" t="n">
-        <v>3</v>
+      <c r="AJ26" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL26" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="79" t="inlineStr">
         <is>
-          <t>revolver</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B27" s="79" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C27" s="68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="79" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E27" s="68">
-        <f>SUM(G27:AV27)</f>
+        <f>SUM(G27:AX27)</f>
         <v/>
       </c>
       <c r="F27" s="68">
-        <f>ROUND(AVERAGE(G27:AV27),1)</f>
-        <v/>
-      </c>
-      <c r="S27" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="T27" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U27" s="79" t="inlineStr">
+        <f>ROUND(AVERAGE(G27:AX27),1)</f>
+        <v/>
+      </c>
+      <c r="I27" s="79" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="V27" s="80" t="inlineStr">
+      <c r="J27" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
+      <c r="K27" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L27" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="M27" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="N27" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="Q27" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="R27" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
       <c r="W27" s="79" t="n">
         <v>3</v>
       </c>
@@ -14711,141 +14765,67 @@
         <v>3</v>
       </c>
       <c r="Z27" s="80" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="AA27" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB27" s="80" t="n">
+        <v>1</v>
       </c>
       <c r="AC27" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AD27" s="80" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AE27" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF27" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AI27" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ27" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL27" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="79" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>Roberta</t>
         </is>
       </c>
       <c r="B28" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C28" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="79" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E28" s="68">
-        <f>SUM(G28:AV28)</f>
+        <f>SUM(G28:AX28)</f>
         <v/>
       </c>
       <c r="F28" s="68">
-        <f>ROUND(AVERAGE(G28:AV28),1)</f>
-        <v/>
-      </c>
-      <c r="I28" s="79" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="J28" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="K28" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L28" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M28" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="N28" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="O28" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="Q28" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="R28" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="W28" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X28" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y28" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z28" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA28" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB28" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC28" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD28" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE28" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF28" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM28" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN28" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G28:AX28),1)</f>
+        <v/>
+      </c>
+      <c r="AO28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="79" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>serra008</t>
         </is>
       </c>
       <c r="B29" s="79" t="n">
@@ -14855,27 +14835,123 @@
         <v>0</v>
       </c>
       <c r="D29" s="79" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E29" s="68">
-        <f>SUM(G29:AV29)</f>
+        <f>SUM(G29:AX29)</f>
         <v/>
       </c>
       <c r="F29" s="68">
-        <f>ROUND(AVERAGE(G29:AV29),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G29:AX29),1)</f>
+        <v/>
+      </c>
+      <c r="G29" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="I29" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="J29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="K29" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="M29" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="N29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="O29" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="P29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q29" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="S29" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="T29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="U29" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="W29" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="X29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y29" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z29" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD29" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE29" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF29" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>3</v>
       </c>
       <c r="AO29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP29" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV29" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="79" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B30" s="79" t="n">
@@ -14885,42 +14961,30 @@
         <v>0</v>
       </c>
       <c r="D30" s="79" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E30" s="68">
-        <f>SUM(G30:AV30)</f>
+        <f>SUM(G30:AX30)</f>
         <v/>
       </c>
       <c r="F30" s="68">
-        <f>ROUND(AVERAGE(G30:AV30),1)</f>
+        <f>ROUND(AVERAGE(G30:AX30),1)</f>
         <v/>
       </c>
       <c r="G30" s="79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H30" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I30" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J30" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="K30" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="L30" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M30" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="N30" s="80" t="n">
-        <v>3</v>
-      </c>
       <c r="O30" s="79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P30" s="80" t="n">
         <v>3</v>
@@ -14931,285 +14995,275 @@
       <c r="R30" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="S30" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="T30" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U30" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V30" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W30" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X30" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y30" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z30" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA30" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB30" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC30" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD30" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE30" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF30" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AS30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT30" t="n">
-        <v>3</v>
-      </c>
       <c r="AU30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AV30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="79" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B31" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C31" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="79" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E31" s="68">
-        <f>SUM(G31:AV31)</f>
+        <f>SUM(G31:AX31)</f>
         <v/>
       </c>
       <c r="F31" s="68">
-        <f>ROUND(AVERAGE(G31:AV31),1)</f>
+        <f>ROUND(AVERAGE(G31:AX31),1)</f>
         <v/>
       </c>
       <c r="G31" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H31" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I31" s="79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J31" s="80" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="K31" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L31" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="M31" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" s="80" t="n">
+        <v>2</v>
       </c>
       <c r="O31" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P31" s="80" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q31" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R31" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="AU31" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV31" t="n">
+      <c r="U31" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V31" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y31" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z31" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA31" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB31" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI31" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ31" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK31" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT31" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="79" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B32" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C32" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="79" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E32" s="68">
-        <f>SUM(G32:AV32)</f>
+        <f>SUM(G32:AX32)</f>
         <v/>
       </c>
       <c r="F32" s="68">
-        <f>ROUND(AVERAGE(G32:AV32),1)</f>
-        <v/>
-      </c>
-      <c r="G32" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="H32" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="I32" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J32" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="K32" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L32" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="M32" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="N32" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="O32" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="P32" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="R32" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U32" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V32" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y32" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z32" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA32" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB32" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AI32" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ32" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK32" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL32" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM32" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN32" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G32:AX32),1)</f>
+        <v/>
       </c>
       <c r="AS32" t="n">
         <v>3</v>
       </c>
       <c r="AT32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="79" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B33" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C33" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="79" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E33" s="68">
-        <f>SUM(G33:AV33)</f>
+        <f>SUM(G33:AX33)</f>
         <v/>
       </c>
       <c r="F33" s="68">
-        <f>ROUND(AVERAGE(G33:AV33),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G33:AX33),1)</f>
+        <v/>
+      </c>
+      <c r="O33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P33" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R33" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="W33" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD33" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI33" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ33" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP33" t="n">
+        <v>1</v>
       </c>
       <c r="AS33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="79" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B34" s="79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C34" s="68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="79" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E34" s="68">
-        <f>SUM(G34:AV34)</f>
+        <f>SUM(G34:AX34)</f>
         <v/>
       </c>
       <c r="F34" s="68">
-        <f>ROUND(AVERAGE(G34:AV34),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G34:AX34),1)</f>
+        <v/>
+      </c>
+      <c r="G34" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="H34" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="I34" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="J34" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="K34" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="L34" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
       <c r="O34" s="79" t="n">
         <v>3</v>
@@ -15221,24 +15275,36 @@
         <v>3</v>
       </c>
       <c r="R34" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="S34" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="T34" s="80" t="n">
         <v>2</v>
       </c>
       <c r="W34" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X34" s="80" t="n">
         <v>3</v>
       </c>
+      <c r="Y34" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z34" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA34" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB34" s="80" t="n">
+        <v>2</v>
+      </c>
       <c r="AC34" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD34" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF34" s="80" t="n">
         <v>3</v>
       </c>
       <c r="AI34" t="inlineStr">
@@ -15257,168 +15323,154 @@
       <c r="AL34" t="n">
         <v>3</v>
       </c>
-      <c r="AO34" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP34" t="n">
-        <v>1</v>
+      <c r="AM34" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN34" t="n">
+        <v>3</v>
       </c>
       <c r="AS34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AT34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV34" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="79" t="inlineStr">
         <is>
-          <t>Valh</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B35" s="79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C35" s="68" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="79" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E35" s="68">
-        <f>SUM(G35:AV35)</f>
+        <f>SUM(G35:AX35)</f>
         <v/>
       </c>
       <c r="F35" s="68">
-        <f>ROUND(AVERAGE(G35:AV35),1)</f>
-        <v/>
-      </c>
-      <c r="K35" s="79" t="inlineStr">
+        <f>ROUND(AVERAGE(G35:AX35),1)</f>
+        <v/>
+      </c>
+      <c r="U35" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V35" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="W35" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X35" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="L35" s="80" t="inlineStr">
+      <c r="Y35" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z35" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA35" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB35" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC35" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD35" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE35" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF35" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI35" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="Q35" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="R35" s="80" t="n">
+      <c r="AJ35" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK35" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL35" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AM35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO35" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP35" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="79" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B36" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="79" t="n">
         <v>4</v>
       </c>
-      <c r="C36" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="D36" s="79" t="n">
-        <v>15</v>
-      </c>
       <c r="E36" s="68">
-        <f>SUM(G36:AV36)</f>
+        <f>SUM(G36:AX36)</f>
         <v/>
       </c>
       <c r="F36" s="68">
-        <f>ROUND(AVERAGE(G36:AV36),1)</f>
-        <v/>
-      </c>
-      <c r="G36" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="H36" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="I36" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="J36" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="K36" s="79" t="inlineStr">
+        <f>ROUND(AVERAGE(G36:AX36),1)</f>
+        <v/>
+      </c>
+      <c r="AM36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP36" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="L36" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="O36" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P36" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q36" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R36" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="S36" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="T36" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="W36" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X36" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y36" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z36" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA36" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB36" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC36" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD36" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AI36" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ36" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK36" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL36" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM36" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN36" t="n">
-        <v>3</v>
-      </c>
       <c r="AS36" t="n">
         <v>3</v>
       </c>
@@ -15426,112 +15478,62 @@
         <v>3</v>
       </c>
       <c r="AU36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AV36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="79" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B37" s="79" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C37" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" s="79" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E37" s="68">
-        <f>SUM(G37:AV37)</f>
+        <f>SUM(G37:AX37)</f>
         <v/>
       </c>
       <c r="F37" s="68">
-        <f>ROUND(AVERAGE(G37:AV37),1)</f>
-        <v/>
-      </c>
-      <c r="U37" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V37" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="W37" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X37" s="80" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="Y37" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z37" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA37" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB37" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC37" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD37" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE37" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF37" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI37" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ37" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK37" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL37" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+        <f>ROUND(AVERAGE(G37:AX37),1)</f>
+        <v/>
       </c>
       <c r="AM37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AO37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP37" t="n">
         <v>3</v>
+      </c>
+      <c r="AS37" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT37" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="79" t="inlineStr">
         <is>
-          <t>LucFir3</t>
+          <t>Amazonie</t>
         </is>
       </c>
       <c r="B38" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" s="68" t="n">
         <v>0</v>
@@ -15540,11 +15542,11 @@
         <v>4</v>
       </c>
       <c r="E38" s="68">
-        <f>SUM(G38:AV38)</f>
+        <f>SUM(G38:AX38)</f>
         <v/>
       </c>
       <c r="F38" s="68">
-        <f>ROUND(AVERAGE(G38:AV38),1)</f>
+        <f>ROUND(AVERAGE(G38:AX38),1)</f>
         <v/>
       </c>
       <c r="AM38" t="n">
@@ -15554,12 +15556,10 @@
         <v>3</v>
       </c>
       <c r="AO38" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP38" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="AP38" t="n">
+        <v>2</v>
       </c>
       <c r="AS38" t="n">
         <v>3</v>
@@ -15568,16 +15568,16 @@
         <v>3</v>
       </c>
       <c r="AU38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AV38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="79" t="inlineStr">
         <is>
-          <t>Kle</t>
+          <t>terracrom</t>
         </is>
       </c>
       <c r="B39" s="79" t="n">
@@ -15587,39 +15587,21 @@
         <v>0</v>
       </c>
       <c r="D39" s="79" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E39" s="68">
-        <f>SUM(G39:AV39)</f>
+        <f>SUM(G39:AX39)</f>
         <v/>
       </c>
       <c r="F39" s="68">
-        <f>ROUND(AVERAGE(G39:AV39),1)</f>
-        <v/>
-      </c>
-      <c r="AM39" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN39" t="n">
-        <v>2</v>
-      </c>
-      <c r="AO39" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP39" t="n">
-        <v>3</v>
-      </c>
-      <c r="AS39" t="n">
-        <v>2</v>
-      </c>
-      <c r="AT39" t="n">
-        <v>2</v>
+        <f>ROUND(AVERAGE(G39:AX39),1)</f>
+        <v/>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="79" t="inlineStr">
         <is>
-          <t>Amazonie</t>
+          <t>MIRIAM MIRIAM</t>
         </is>
       </c>
       <c r="B40" s="79" t="n">
@@ -15629,14 +15611,14 @@
         <v>0</v>
       </c>
       <c r="D40" s="79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E40" s="68">
-        <f>SUM(G40:AV40)</f>
+        <f>SUM(G40:AX40)</f>
         <v/>
       </c>
       <c r="F40" s="68">
-        <f>ROUND(AVERAGE(G40:AV40),1)</f>
+        <f>ROUND(AVERAGE(G40:AX40),1)</f>
         <v/>
       </c>
       <c r="AM40" t="n">
@@ -15652,22 +15634,16 @@
         <v>2</v>
       </c>
       <c r="AS40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT40" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU40" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV40" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="79" t="inlineStr">
         <is>
-          <t>terracrom</t>
+          <t>cucco</t>
         </is>
       </c>
       <c r="B41" s="79" t="n">
@@ -15677,21 +15653,45 @@
         <v>0</v>
       </c>
       <c r="D41" s="79" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E41" s="68">
-        <f>SUM(G41:AV41)</f>
+        <f>SUM(G41:AX41)</f>
         <v/>
       </c>
       <c r="F41" s="68">
-        <f>ROUND(AVERAGE(G41:AV41),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G41:AX41),1)</f>
+        <v/>
+      </c>
+      <c r="AM41" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN41" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO41" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP41" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU41" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV41" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="79" t="inlineStr">
         <is>
-          <t>MIRIAM MIRIAM</t>
+          <t>fede61mito</t>
         </is>
       </c>
       <c r="B42" s="79" t="n">
@@ -15701,39 +15701,21 @@
         <v>0</v>
       </c>
       <c r="D42" s="79" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E42" s="68">
-        <f>SUM(G42:AV42)</f>
+        <f>SUM(G42:AX42)</f>
         <v/>
       </c>
       <c r="F42" s="68">
-        <f>ROUND(AVERAGE(G42:AV42),1)</f>
-        <v/>
-      </c>
-      <c r="AM42" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN42" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO42" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP42" t="n">
-        <v>2</v>
-      </c>
-      <c r="AS42" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT42" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G42:AX42),1)</f>
+        <v/>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="79" t="inlineStr">
         <is>
-          <t>cucco</t>
+          <t>Dasters79</t>
         </is>
       </c>
       <c r="B43" s="79" t="n">
@@ -15743,45 +15725,21 @@
         <v>0</v>
       </c>
       <c r="D43" s="79" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E43" s="68">
-        <f>SUM(G43:AV43)</f>
+        <f>SUM(G43:AX43)</f>
         <v/>
       </c>
       <c r="F43" s="68">
-        <f>ROUND(AVERAGE(G43:AV43),1)</f>
-        <v/>
-      </c>
-      <c r="AM43" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN43" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO43" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP43" t="n">
-        <v>3</v>
-      </c>
-      <c r="AS43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU43" t="n">
-        <v>2</v>
-      </c>
-      <c r="AV43" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G43:AX43),1)</f>
+        <v/>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="79" t="inlineStr">
         <is>
-          <t>fede61mito</t>
+          <t>Xx_Herman_xX</t>
         </is>
       </c>
       <c r="B44" s="79" t="n">
@@ -15794,18 +15752,18 @@
         <v>0</v>
       </c>
       <c r="E44" s="68">
-        <f>SUM(G44:AV44)</f>
+        <f>SUM(G44:AX44)</f>
         <v/>
       </c>
       <c r="F44" s="68">
-        <f>ROUND(AVERAGE(G44:AV44),1)</f>
+        <f>ROUND(AVERAGE(G44:AX44),1)</f>
         <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="79" t="inlineStr">
         <is>
-          <t>Dasters79</t>
+          <t>dibba10</t>
         </is>
       </c>
       <c r="B45" s="79" t="n">
@@ -15818,18 +15776,18 @@
         <v>0</v>
       </c>
       <c r="E45" s="68">
-        <f>SUM(G45:AV45)</f>
+        <f>SUM(G45:AX45)</f>
         <v/>
       </c>
       <c r="F45" s="68">
-        <f>ROUND(AVERAGE(G45:AV45),1)</f>
+        <f>ROUND(AVERAGE(G45:AX45),1)</f>
         <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="79" t="inlineStr">
         <is>
-          <t>Artur</t>
+          <t>SanBucaツ</t>
         </is>
       </c>
       <c r="B46" s="79" t="n">
@@ -15842,18 +15800,18 @@
         <v>0</v>
       </c>
       <c r="E46" s="68">
-        <f>SUM(G46:AV46)</f>
+        <f>SUM(G46:AX46)</f>
         <v/>
       </c>
       <c r="F46" s="68">
-        <f>ROUND(AVERAGE(G46:AV46),1)</f>
+        <f>ROUND(AVERAGE(G46:AX46),1)</f>
         <v/>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="79" t="inlineStr">
         <is>
-          <t>Xx_Herman_xX</t>
+          <t>Anto</t>
         </is>
       </c>
       <c r="B47" s="79" t="n">
@@ -15866,42 +15824,52 @@
         <v>0</v>
       </c>
       <c r="E47" s="68">
-        <f>SUM(G47:AV47)</f>
+        <f>SUM(G47:AX47)</f>
         <v/>
       </c>
       <c r="F47" s="68">
-        <f>ROUND(AVERAGE(G47:AV47),1)</f>
+        <f>ROUND(AVERAGE(G47:AX47),1)</f>
         <v/>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="79" t="inlineStr">
         <is>
-          <t>dibba10</t>
+          <t>Michele</t>
         </is>
       </c>
       <c r="B48" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C48" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="68">
-        <f>SUM(G48:AV48)</f>
+        <f>SUM(G48:AX48)</f>
         <v/>
       </c>
       <c r="F48" s="68">
-        <f>ROUND(AVERAGE(G48:AV48),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G48:AX48),1)</f>
+        <v/>
+      </c>
+      <c r="AU48" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AV48" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="79" t="inlineStr">
         <is>
-          <t>SanBucaツ</t>
+          <t>VERRETHERULER</t>
         </is>
       </c>
       <c r="B49" s="79" t="n">
@@ -15914,18 +15882,18 @@
         <v>0</v>
       </c>
       <c r="E49" s="68">
-        <f>SUM(G49:AV49)</f>
+        <f>SUM(G49:AX49)</f>
         <v/>
       </c>
       <c r="F49" s="68">
-        <f>ROUND(AVERAGE(G49:AV49),1)</f>
+        <f>ROUND(AVERAGE(G49:AX49),1)</f>
         <v/>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="79" t="inlineStr">
         <is>
-          <t>Anto</t>
+          <t>GGfresco_08</t>
         </is>
       </c>
       <c r="B50" s="79" t="n">
@@ -15938,46 +15906,36 @@
         <v>0</v>
       </c>
       <c r="E50" s="68">
-        <f>SUM(G50:AV50)</f>
+        <f>SUM(G50:AX50)</f>
         <v/>
       </c>
       <c r="F50" s="68">
-        <f>ROUND(AVERAGE(G50:AV50),1)</f>
+        <f>ROUND(AVERAGE(G50:AX50),1)</f>
         <v/>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="79" t="inlineStr">
         <is>
-          <t>Michele</t>
+          <t>PESCARA MANZIA</t>
         </is>
       </c>
       <c r="B51" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C51" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" s="68">
-        <f>SUM(G51:AV51)</f>
+        <f>SUM(G51:AX51)</f>
         <v/>
       </c>
       <c r="F51" s="68">
-        <f>ROUND(AVERAGE(G51:AV51),1)</f>
-        <v/>
-      </c>
-      <c r="AU51" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AV51" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+        <f>ROUND(AVERAGE(G51:AX51),1)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update WAR data - 2026-02-27
</commit_message>
<xml_diff>
--- a/rewards.xlsx
+++ b/rewards.xlsx
@@ -12486,7 +12486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI51"/>
+  <dimension ref="A1:CI48"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -12803,12 +12803,12 @@
       </c>
       <c r="AY1" s="109" t="inlineStr">
         <is>
-          <t>Colonna51</t>
+          <t>WAR-23 (1)</t>
         </is>
       </c>
       <c r="AZ1" s="109" t="inlineStr">
         <is>
-          <t>Colonna52</t>
+          <t>WAR-23 (2)</t>
         </is>
       </c>
       <c r="BA1" s="109" t="inlineStr">
@@ -13003,11 +13003,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="111">
-        <f>SUM(G2:AX2)</f>
+        <f>SUM(G2:AZ2)</f>
         <v/>
       </c>
       <c r="F2" s="68">
-        <f>ROUND(AVERAGE(G2:AX2),1)</f>
+        <f>ROUND(AVERAGE(G2:AZ2),1)</f>
         <v/>
       </c>
       <c r="G2" s="110" t="n"/>
@@ -13122,11 +13122,11 @@
         <v>0</v>
       </c>
       <c r="E3" s="68">
-        <f>SUM(G3:AX3)</f>
+        <f>SUM(G3:AZ3)</f>
         <v/>
       </c>
       <c r="F3" s="68">
-        <f>ROUND(AVERAGE(G3:AX3),1)</f>
+        <f>ROUND(AVERAGE(G3:AZ3),1)</f>
         <v/>
       </c>
     </row>
@@ -13146,11 +13146,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="68">
-        <f>SUM(G4:AX4)</f>
+        <f>SUM(G4:AZ4)</f>
         <v/>
       </c>
       <c r="F4" s="68">
-        <f>ROUND(AVERAGE(G4:AX4),1)</f>
+        <f>ROUND(AVERAGE(G4:AZ4),1)</f>
         <v/>
       </c>
       <c r="I4" s="79" t="n">
@@ -13198,11 +13198,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="68">
-        <f>SUM(G5:AX5)</f>
+        <f>SUM(G5:AZ5)</f>
         <v/>
       </c>
       <c r="F5" s="68">
-        <f>ROUND(AVERAGE(G5:AX5),1)</f>
+        <f>ROUND(AVERAGE(G5:AZ5),1)</f>
         <v/>
       </c>
       <c r="AO5" t="n">
@@ -13221,20 +13221,20 @@
         </is>
       </c>
       <c r="B6" s="79" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="68" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="79" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" s="68">
-        <f>SUM(G6:AX6)</f>
+        <f>SUM(G6:AZ6)</f>
         <v/>
       </c>
       <c r="F6" s="68">
-        <f>ROUND(AVERAGE(G6:AX6),1)</f>
+        <f>ROUND(AVERAGE(G6:AZ6),1)</f>
         <v/>
       </c>
       <c r="G6" s="79" t="n">
@@ -13347,6 +13347,14 @@
         </is>
       </c>
       <c r="AV6" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AY6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ6" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
@@ -13368,11 +13376,11 @@
         <v>6</v>
       </c>
       <c r="E7" s="68">
-        <f>SUM(G7:AX7)</f>
+        <f>SUM(G7:AZ7)</f>
         <v/>
       </c>
       <c r="F7" s="68">
-        <f>ROUND(AVERAGE(G7:AX7),1)</f>
+        <f>ROUND(AVERAGE(G7:AZ7),1)</f>
         <v/>
       </c>
       <c r="K7" s="79" t="n">
@@ -13428,11 +13436,11 @@
         <v>0</v>
       </c>
       <c r="E8" s="68">
-        <f>SUM(G8:AX8)</f>
+        <f>SUM(G8:AZ8)</f>
         <v/>
       </c>
       <c r="F8" s="68">
-        <f>ROUND(AVERAGE(G8:AX8),1)</f>
+        <f>ROUND(AVERAGE(G8:AZ8),1)</f>
         <v/>
       </c>
     </row>
@@ -13452,11 +13460,11 @@
         <v>13</v>
       </c>
       <c r="E9" s="68">
-        <f>SUM(G9:AX9)</f>
+        <f>SUM(G9:AZ9)</f>
         <v/>
       </c>
       <c r="F9" s="68">
-        <f>ROUND(AVERAGE(G9:AX9),1)</f>
+        <f>ROUND(AVERAGE(G9:AZ9),1)</f>
         <v/>
       </c>
       <c r="G9" s="79" t="n">
@@ -13554,11 +13562,11 @@
         <v>0</v>
       </c>
       <c r="E10" s="68">
-        <f>SUM(G10:AX10)</f>
+        <f>SUM(G10:AZ10)</f>
         <v/>
       </c>
       <c r="F10" s="68">
-        <f>ROUND(AVERAGE(G10:AX10),1)</f>
+        <f>ROUND(AVERAGE(G10:AZ10),1)</f>
         <v/>
       </c>
     </row>
@@ -13578,11 +13586,11 @@
         <v>6</v>
       </c>
       <c r="E11" s="68">
-        <f>SUM(G11:AX11)</f>
+        <f>SUM(G11:AZ11)</f>
         <v/>
       </c>
       <c r="F11" s="68">
-        <f>ROUND(AVERAGE(G11:AX11),1)</f>
+        <f>ROUND(AVERAGE(G11:AZ11),1)</f>
         <v/>
       </c>
       <c r="I11" s="79" t="n">
@@ -13643,20 +13651,20 @@
         </is>
       </c>
       <c r="B12" s="79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="79" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" s="68">
-        <f>SUM(G12:AX12)</f>
+        <f>SUM(G12:AZ12)</f>
         <v/>
       </c>
       <c r="F12" s="68">
-        <f>ROUND(AVERAGE(G12:AX12),1)</f>
+        <f>ROUND(AVERAGE(G12:AZ12),1)</f>
         <v/>
       </c>
       <c r="Q12" s="79" t="n">
@@ -13696,6 +13704,16 @@
       </c>
       <c r="AT12" t="n">
         <v>2</v>
+      </c>
+      <c r="AY12" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AZ12" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -13714,11 +13732,11 @@
         <v>12</v>
       </c>
       <c r="E13" s="68">
-        <f>SUM(G13:AX13)</f>
+        <f>SUM(G13:AZ13)</f>
         <v/>
       </c>
       <c r="F13" s="68">
-        <f>ROUND(AVERAGE(G13:AX13),1)</f>
+        <f>ROUND(AVERAGE(G13:AZ13),1)</f>
         <v/>
       </c>
       <c r="G13" s="79" t="n">
@@ -13810,11 +13828,11 @@
         <v>0</v>
       </c>
       <c r="E14" s="68">
-        <f>SUM(G14:AX14)</f>
+        <f>SUM(G14:AZ14)</f>
         <v/>
       </c>
       <c r="F14" s="68">
-        <f>ROUND(AVERAGE(G14:AX14),1)</f>
+        <f>ROUND(AVERAGE(G14:AZ14),1)</f>
         <v/>
       </c>
     </row>
@@ -13831,14 +13849,14 @@
         <v>1</v>
       </c>
       <c r="D15" s="79" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E15" s="68">
-        <f>SUM(G15:AX15)</f>
+        <f>SUM(G15:AZ15)</f>
         <v/>
       </c>
       <c r="F15" s="68">
-        <f>ROUND(AVERAGE(G15:AX15),1)</f>
+        <f>ROUND(AVERAGE(G15:AZ15),1)</f>
         <v/>
       </c>
       <c r="I15" s="79" t="n">
@@ -13929,6 +13947,12 @@
         <v>3</v>
       </c>
       <c r="AV15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ15" t="n">
         <v>3</v>
       </c>
     </row>
@@ -13948,11 +13972,11 @@
         <v>1</v>
       </c>
       <c r="E16" s="68">
-        <f>SUM(G16:AX16)</f>
+        <f>SUM(G16:AZ16)</f>
         <v/>
       </c>
       <c r="F16" s="68">
-        <f>ROUND(AVERAGE(G16:AX16),1)</f>
+        <f>ROUND(AVERAGE(G16:AZ16),1)</f>
         <v/>
       </c>
       <c r="AE16" s="79" t="n">
@@ -13978,11 +14002,11 @@
         <v>9</v>
       </c>
       <c r="E17" s="68">
-        <f>SUM(G17:AX17)</f>
+        <f>SUM(G17:AZ17)</f>
         <v/>
       </c>
       <c r="F17" s="68">
-        <f>ROUND(AVERAGE(G17:AX17),1)</f>
+        <f>ROUND(AVERAGE(G17:AZ17),1)</f>
         <v/>
       </c>
       <c r="S17" s="79" t="n">
@@ -14057,14 +14081,14 @@
         <v>0</v>
       </c>
       <c r="D18" s="79" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" s="68">
-        <f>SUM(G18:AX18)</f>
+        <f>SUM(G18:AZ18)</f>
         <v/>
       </c>
       <c r="F18" s="68">
-        <f>ROUND(AVERAGE(G18:AX18),1)</f>
+        <f>ROUND(AVERAGE(G18:AZ18),1)</f>
         <v/>
       </c>
       <c r="G18" s="79" t="n">
@@ -14083,6 +14107,12 @@
         <v>3</v>
       </c>
       <c r="Z18" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ18" t="n">
         <v>3</v>
       </c>
     </row>
@@ -14102,11 +14132,11 @@
         <v>1</v>
       </c>
       <c r="E19" s="68">
-        <f>SUM(G19:AX19)</f>
+        <f>SUM(G19:AZ19)</f>
         <v/>
       </c>
       <c r="F19" s="68">
-        <f>ROUND(AVERAGE(G19:AX19),1)</f>
+        <f>ROUND(AVERAGE(G19:AZ19),1)</f>
         <v/>
       </c>
       <c r="AE19" s="79" t="n">
@@ -14129,14 +14159,14 @@
         <v>0</v>
       </c>
       <c r="D20" s="79" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E20" s="68">
-        <f>SUM(G20:AX20)</f>
+        <f>SUM(G20:AZ20)</f>
         <v/>
       </c>
       <c r="F20" s="68">
-        <f>ROUND(AVERAGE(G20:AX20),1)</f>
+        <f>ROUND(AVERAGE(G20:AZ20),1)</f>
         <v/>
       </c>
       <c r="I20" s="79" t="n">
@@ -14196,6 +14226,12 @@
       </c>
       <c r="AV20" t="n">
         <v>1</v>
+      </c>
+      <c r="AY20" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ20" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -14214,11 +14250,11 @@
         <v>10</v>
       </c>
       <c r="E21" s="68">
-        <f>SUM(G21:AX21)</f>
+        <f>SUM(G21:AZ21)</f>
         <v/>
       </c>
       <c r="F21" s="68">
-        <f>ROUND(AVERAGE(G21:AX21),1)</f>
+        <f>ROUND(AVERAGE(G21:AZ21),1)</f>
         <v/>
       </c>
       <c r="G21" s="79" t="inlineStr">
@@ -14304,11 +14340,11 @@
         <v>11</v>
       </c>
       <c r="E22" s="68">
-        <f>SUM(G22:AX22)</f>
+        <f>SUM(G22:AZ22)</f>
         <v/>
       </c>
       <c r="F22" s="68">
-        <f>ROUND(AVERAGE(G22:AX22),1)</f>
+        <f>ROUND(AVERAGE(G22:AZ22),1)</f>
         <v/>
       </c>
       <c r="G22" s="79" t="n">
@@ -14408,11 +14444,11 @@
         <v>11</v>
       </c>
       <c r="E23" s="68">
-        <f>SUM(G23:AX23)</f>
+        <f>SUM(G23:AZ23)</f>
         <v/>
       </c>
       <c r="F23" s="68">
-        <f>ROUND(AVERAGE(G23:AX23),1)</f>
+        <f>ROUND(AVERAGE(G23:AZ23),1)</f>
         <v/>
       </c>
       <c r="G23" s="79" t="n">
@@ -14502,11 +14538,11 @@
         <v>8</v>
       </c>
       <c r="E24" s="68">
-        <f>SUM(G24:AX24)</f>
+        <f>SUM(G24:AZ24)</f>
         <v/>
       </c>
       <c r="F24" s="68">
-        <f>ROUND(AVERAGE(G24:AX24),1)</f>
+        <f>ROUND(AVERAGE(G24:AZ24),1)</f>
         <v/>
       </c>
       <c r="I24" s="79" t="n">
@@ -14584,11 +14620,11 @@
         <v>3</v>
       </c>
       <c r="E25" s="68">
-        <f>SUM(G25:AX25)</f>
+        <f>SUM(G25:AZ25)</f>
         <v/>
       </c>
       <c r="F25" s="68">
-        <f>ROUND(AVERAGE(G25:AX25),1)</f>
+        <f>ROUND(AVERAGE(G25:AZ25),1)</f>
         <v/>
       </c>
       <c r="Y25" s="79" t="n">
@@ -14628,11 +14664,11 @@
         <v>8</v>
       </c>
       <c r="E26" s="68">
-        <f>SUM(G26:AX26)</f>
+        <f>SUM(G26:AZ26)</f>
         <v/>
       </c>
       <c r="F26" s="68">
-        <f>ROUND(AVERAGE(G26:AX26),1)</f>
+        <f>ROUND(AVERAGE(G26:AZ26),1)</f>
         <v/>
       </c>
       <c r="S26" s="79" t="n">
@@ -14710,11 +14746,11 @@
         <v>10</v>
       </c>
       <c r="E27" s="68">
-        <f>SUM(G27:AX27)</f>
+        <f>SUM(G27:AZ27)</f>
         <v/>
       </c>
       <c r="F27" s="68">
-        <f>ROUND(AVERAGE(G27:AX27),1)</f>
+        <f>ROUND(AVERAGE(G27:AZ27),1)</f>
         <v/>
       </c>
       <c r="I27" s="79" t="inlineStr">
@@ -14808,11 +14844,11 @@
         <v>1</v>
       </c>
       <c r="E28" s="68">
-        <f>SUM(G28:AX28)</f>
+        <f>SUM(G28:AZ28)</f>
         <v/>
       </c>
       <c r="F28" s="68">
-        <f>ROUND(AVERAGE(G28:AX28),1)</f>
+        <f>ROUND(AVERAGE(G28:AZ28),1)</f>
         <v/>
       </c>
       <c r="AO28" t="n">
@@ -14825,7 +14861,7 @@
     <row r="29">
       <c r="A29" s="79" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B29" s="79" t="n">
@@ -14835,42 +14871,30 @@
         <v>0</v>
       </c>
       <c r="D29" s="79" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E29" s="68">
-        <f>SUM(G29:AX29)</f>
+        <f>SUM(G29:AZ29)</f>
         <v/>
       </c>
       <c r="F29" s="68">
-        <f>ROUND(AVERAGE(G29:AX29),1)</f>
+        <f>ROUND(AVERAGE(G29:AZ29),1)</f>
         <v/>
       </c>
       <c r="G29" s="79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H29" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I29" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J29" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="K29" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="L29" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="M29" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="N29" s="80" t="n">
-        <v>3</v>
-      </c>
       <c r="O29" s="79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P29" s="80" t="n">
         <v>3</v>
@@ -14881,285 +14905,275 @@
       <c r="R29" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="S29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="T29" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V29" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="W29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X29" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z29" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA29" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB29" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD29" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE29" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF29" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AS29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT29" t="n">
-        <v>3</v>
-      </c>
       <c r="AU29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AV29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="79" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B30" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="79" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E30" s="68">
-        <f>SUM(G30:AX30)</f>
+        <f>SUM(G30:AZ30)</f>
         <v/>
       </c>
       <c r="F30" s="68">
-        <f>ROUND(AVERAGE(G30:AX30),1)</f>
+        <f>ROUND(AVERAGE(G30:AZ30),1)</f>
         <v/>
       </c>
       <c r="G30" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H30" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I30" s="79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J30" s="80" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="K30" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="L30" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="M30" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" s="80" t="n">
+        <v>2</v>
       </c>
       <c r="O30" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P30" s="80" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q30" s="79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R30" s="80" t="n">
         <v>3</v>
       </c>
-      <c r="AU30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV30" t="n">
+      <c r="U30" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V30" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y30" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z30" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA30" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB30" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI30" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ30" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT30" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="79" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>SubOhm</t>
         </is>
       </c>
       <c r="B31" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C31" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="79" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E31" s="68">
-        <f>SUM(G31:AX31)</f>
+        <f>SUM(G31:AZ31)</f>
         <v/>
       </c>
       <c r="F31" s="68">
-        <f>ROUND(AVERAGE(G31:AX31),1)</f>
-        <v/>
-      </c>
-      <c r="G31" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="H31" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="I31" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J31" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="K31" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="L31" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="M31" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="N31" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="O31" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="P31" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="R31" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="U31" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V31" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y31" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z31" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA31" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB31" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AI31" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ31" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK31" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL31" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM31" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN31" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G31:AZ31),1)</f>
+        <v/>
       </c>
       <c r="AS31" t="n">
         <v>3</v>
       </c>
       <c r="AT31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="79" t="inlineStr">
         <is>
-          <t>SubOhm</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B32" s="79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C32" s="68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="79" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E32" s="68">
-        <f>SUM(G32:AX32)</f>
+        <f>SUM(G32:AZ32)</f>
         <v/>
       </c>
       <c r="F32" s="68">
-        <f>ROUND(AVERAGE(G32:AX32),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G32:AZ32),1)</f>
+        <v/>
+      </c>
+      <c r="O32" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="P32" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="R32" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="W32" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X32" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC32" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD32" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE32" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF32" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI32" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AJ32" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="AK32" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>1</v>
       </c>
       <c r="AS32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="79" t="inlineStr">
         <is>
-          <t>th4nos</t>
+          <t>xbladze</t>
         </is>
       </c>
       <c r="B33" s="79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C33" s="68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="79" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E33" s="68">
-        <f>SUM(G33:AX33)</f>
+        <f>SUM(G33:AZ33)</f>
         <v/>
       </c>
       <c r="F33" s="68">
-        <f>ROUND(AVERAGE(G33:AX33),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G33:AZ33),1)</f>
+        <v/>
+      </c>
+      <c r="G33" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="H33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="I33" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="J33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="K33" s="79" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
+      </c>
+      <c r="L33" s="80" t="inlineStr">
+        <is>
+          <t>SKIP</t>
+        </is>
       </c>
       <c r="O33" s="79" t="n">
         <v>3</v>
@@ -15171,24 +15185,36 @@
         <v>3</v>
       </c>
       <c r="R33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="S33" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="T33" s="80" t="n">
         <v>2</v>
       </c>
       <c r="W33" s="79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X33" s="80" t="n">
         <v>3</v>
       </c>
+      <c r="Y33" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z33" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA33" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB33" s="80" t="n">
+        <v>2</v>
+      </c>
       <c r="AC33" s="79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD33" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE33" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF33" s="80" t="n">
         <v>3</v>
       </c>
       <c r="AI33" t="inlineStr">
@@ -15207,241 +15233,181 @@
       <c r="AL33" t="n">
         <v>3</v>
       </c>
-      <c r="AO33" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP33" t="n">
-        <v>1</v>
+      <c r="AM33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN33" t="n">
+        <v>3</v>
       </c>
       <c r="AS33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AT33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV33" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="79" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>zordan</t>
         </is>
       </c>
       <c r="B34" s="79" t="n">
         <v>4</v>
       </c>
       <c r="C34" s="68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="79" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E34" s="68">
-        <f>SUM(G34:AX34)</f>
+        <f>SUM(G34:AZ34)</f>
         <v/>
       </c>
       <c r="F34" s="68">
-        <f>ROUND(AVERAGE(G34:AX34),1)</f>
-        <v/>
-      </c>
-      <c r="G34" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="H34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="I34" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="J34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="K34" s="79" t="inlineStr">
+        <f>ROUND(AVERAGE(G34:AZ34),1)</f>
+        <v/>
+      </c>
+      <c r="U34" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="V34" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="W34" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="X34" s="80" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="L34" s="80" t="inlineStr">
+      <c r="Y34" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z34" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA34" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB34" s="80" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC34" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD34" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE34" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF34" s="80" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI34" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="O34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="P34" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="R34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="S34" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="T34" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="W34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="X34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y34" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA34" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB34" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC34" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD34" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AI34" t="inlineStr">
+      <c r="AJ34" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="AJ34" t="inlineStr">
+      <c r="AK34" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL34" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="AK34" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL34" t="n">
-        <v>3</v>
-      </c>
       <c r="AM34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AN34" t="n">
         <v>3</v>
       </c>
-      <c r="AS34" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT34" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU34" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV34" t="n">
-        <v>3</v>
+      <c r="AO34" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY34" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ34" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="79" t="inlineStr">
         <is>
-          <t>zordan</t>
+          <t>LucFir3</t>
         </is>
       </c>
       <c r="B35" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="79" t="n">
         <v>4</v>
       </c>
-      <c r="C35" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="79" t="n">
-        <v>10</v>
-      </c>
       <c r="E35" s="68">
-        <f>SUM(G35:AX35)</f>
+        <f>SUM(G35:AZ35)</f>
         <v/>
       </c>
       <c r="F35" s="68">
-        <f>ROUND(AVERAGE(G35:AX35),1)</f>
-        <v/>
-      </c>
-      <c r="U35" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="V35" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="W35" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="X35" s="80" t="inlineStr">
+        <f>ROUND(AVERAGE(G35:AZ35),1)</f>
+        <v/>
+      </c>
+      <c r="AM35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP35" t="inlineStr">
         <is>
           <t>SKIP</t>
         </is>
       </c>
-      <c r="Y35" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z35" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA35" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB35" s="80" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC35" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD35" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE35" s="79" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF35" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI35" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AJ35" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AK35" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL35" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AM35" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN35" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO35" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP35" t="n">
-        <v>3</v>
+      <c r="AS35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="79" t="inlineStr">
         <is>
-          <t>LucFir3</t>
+          <t>Kle</t>
         </is>
       </c>
       <c r="B36" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="68" t="n">
         <v>0</v>
@@ -15450,44 +15416,42 @@
         <v>4</v>
       </c>
       <c r="E36" s="68">
-        <f>SUM(G36:AX36)</f>
+        <f>SUM(G36:AZ36)</f>
         <v/>
       </c>
       <c r="F36" s="68">
-        <f>ROUND(AVERAGE(G36:AX36),1)</f>
+        <f>ROUND(AVERAGE(G36:AZ36),1)</f>
         <v/>
       </c>
       <c r="AM36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AO36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP36" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="AP36" t="n">
+        <v>3</v>
       </c>
       <c r="AS36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT36" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV36" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="AY36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ36" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="79" t="inlineStr">
         <is>
-          <t>Kle</t>
+          <t>Amazonie</t>
         </is>
       </c>
       <c r="B37" s="79" t="n">
@@ -15497,39 +15461,51 @@
         <v>0</v>
       </c>
       <c r="D37" s="79" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E37" s="68">
-        <f>SUM(G37:AX37)</f>
+        <f>SUM(G37:AZ37)</f>
         <v/>
       </c>
       <c r="F37" s="68">
-        <f>ROUND(AVERAGE(G37:AX37),1)</f>
+        <f>ROUND(AVERAGE(G37:AZ37),1)</f>
         <v/>
       </c>
       <c r="AM37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AN37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AO37" t="n">
         <v>3</v>
       </c>
       <c r="AP37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AS37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AT37" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="AU37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ37" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="79" t="inlineStr">
         <is>
-          <t>Amazonie</t>
+          <t>terracrom</t>
         </is>
       </c>
       <c r="B38" s="79" t="n">
@@ -15539,45 +15515,21 @@
         <v>0</v>
       </c>
       <c r="D38" s="79" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E38" s="68">
-        <f>SUM(G38:AX38)</f>
+        <f>SUM(G38:AZ38)</f>
         <v/>
       </c>
       <c r="F38" s="68">
-        <f>ROUND(AVERAGE(G38:AX38),1)</f>
-        <v/>
-      </c>
-      <c r="AM38" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN38" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO38" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP38" t="n">
-        <v>2</v>
-      </c>
-      <c r="AS38" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT38" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU38" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV38" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G38:AZ38),1)</f>
+        <v/>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="79" t="inlineStr">
         <is>
-          <t>terracrom</t>
+          <t>MIRIAM MIRIAM</t>
         </is>
       </c>
       <c r="B39" s="79" t="n">
@@ -15587,21 +15539,39 @@
         <v>0</v>
       </c>
       <c r="D39" s="79" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E39" s="68">
-        <f>SUM(G39:AX39)</f>
+        <f>SUM(G39:AZ39)</f>
         <v/>
       </c>
       <c r="F39" s="68">
-        <f>ROUND(AVERAGE(G39:AX39),1)</f>
-        <v/>
+        <f>ROUND(AVERAGE(G39:AZ39),1)</f>
+        <v/>
+      </c>
+      <c r="AM39" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN39" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO39" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP39" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT39" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="79" t="inlineStr">
         <is>
-          <t>MIRIAM MIRIAM</t>
+          <t>cucco</t>
         </is>
       </c>
       <c r="B40" s="79" t="n">
@@ -15611,18 +15581,18 @@
         <v>0</v>
       </c>
       <c r="D40" s="79" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E40" s="68">
-        <f>SUM(G40:AX40)</f>
+        <f>SUM(G40:AZ40)</f>
         <v/>
       </c>
       <c r="F40" s="68">
-        <f>ROUND(AVERAGE(G40:AX40),1)</f>
+        <f>ROUND(AVERAGE(G40:AZ40),1)</f>
         <v/>
       </c>
       <c r="AM40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AN40" t="n">
         <v>3</v>
@@ -15631,19 +15601,31 @@
         <v>3</v>
       </c>
       <c r="AP40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AS40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT40" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="AU40" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV40" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY40" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ40" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="79" t="inlineStr">
         <is>
-          <t>cucco</t>
+          <t>fede61mito</t>
         </is>
       </c>
       <c r="B41" s="79" t="n">
@@ -15653,45 +15635,21 @@
         <v>0</v>
       </c>
       <c r="D41" s="79" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E41" s="68">
-        <f>SUM(G41:AX41)</f>
+        <f>SUM(G41:AZ41)</f>
         <v/>
       </c>
       <c r="F41" s="68">
-        <f>ROUND(AVERAGE(G41:AX41),1)</f>
-        <v/>
-      </c>
-      <c r="AM41" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN41" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO41" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP41" t="n">
-        <v>3</v>
-      </c>
-      <c r="AS41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU41" t="n">
-        <v>2</v>
-      </c>
-      <c r="AV41" t="n">
-        <v>3</v>
+        <f>ROUND(AVERAGE(G41:AZ41),1)</f>
+        <v/>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="79" t="inlineStr">
         <is>
-          <t>fede61mito</t>
+          <t>Dasters79</t>
         </is>
       </c>
       <c r="B42" s="79" t="n">
@@ -15704,18 +15662,18 @@
         <v>0</v>
       </c>
       <c r="E42" s="68">
-        <f>SUM(G42:AX42)</f>
+        <f>SUM(G42:AZ42)</f>
         <v/>
       </c>
       <c r="F42" s="68">
-        <f>ROUND(AVERAGE(G42:AX42),1)</f>
+        <f>ROUND(AVERAGE(G42:AZ42),1)</f>
         <v/>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="79" t="inlineStr">
         <is>
-          <t>Dasters79</t>
+          <t>Xx_Herman_xX</t>
         </is>
       </c>
       <c r="B43" s="79" t="n">
@@ -15728,18 +15686,18 @@
         <v>0</v>
       </c>
       <c r="E43" s="68">
-        <f>SUM(G43:AX43)</f>
+        <f>SUM(G43:AZ43)</f>
         <v/>
       </c>
       <c r="F43" s="68">
-        <f>ROUND(AVERAGE(G43:AX43),1)</f>
+        <f>ROUND(AVERAGE(G43:AZ43),1)</f>
         <v/>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="79" t="inlineStr">
         <is>
-          <t>Xx_Herman_xX</t>
+          <t>dibba10</t>
         </is>
       </c>
       <c r="B44" s="79" t="n">
@@ -15752,18 +15710,18 @@
         <v>0</v>
       </c>
       <c r="E44" s="68">
-        <f>SUM(G44:AX44)</f>
+        <f>SUM(G44:AZ44)</f>
         <v/>
       </c>
       <c r="F44" s="68">
-        <f>ROUND(AVERAGE(G44:AX44),1)</f>
+        <f>ROUND(AVERAGE(G44:AZ44),1)</f>
         <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="79" t="inlineStr">
         <is>
-          <t>dibba10</t>
+          <t>VERRETHERULER</t>
         </is>
       </c>
       <c r="B45" s="79" t="n">
@@ -15776,18 +15734,18 @@
         <v>0</v>
       </c>
       <c r="E45" s="68">
-        <f>SUM(G45:AX45)</f>
+        <f>SUM(G45:AZ45)</f>
         <v/>
       </c>
       <c r="F45" s="68">
-        <f>ROUND(AVERAGE(G45:AX45),1)</f>
+        <f>ROUND(AVERAGE(G45:AZ45),1)</f>
         <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="79" t="inlineStr">
         <is>
-          <t>SanBucaツ</t>
+          <t>GGfresco_08</t>
         </is>
       </c>
       <c r="B46" s="79" t="n">
@@ -15800,18 +15758,18 @@
         <v>0</v>
       </c>
       <c r="E46" s="68">
-        <f>SUM(G46:AX46)</f>
+        <f>SUM(G46:AZ46)</f>
         <v/>
       </c>
       <c r="F46" s="68">
-        <f>ROUND(AVERAGE(G46:AX46),1)</f>
+        <f>ROUND(AVERAGE(G46:AZ46),1)</f>
         <v/>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="79" t="inlineStr">
         <is>
-          <t>Anto</t>
+          <t>PESCARA MANZIA</t>
         </is>
       </c>
       <c r="B47" s="79" t="n">
@@ -15824,117 +15782,35 @@
         <v>0</v>
       </c>
       <c r="E47" s="68">
-        <f>SUM(G47:AX47)</f>
+        <f>SUM(G47:AZ47)</f>
         <v/>
       </c>
       <c r="F47" s="68">
-        <f>ROUND(AVERAGE(G47:AX47),1)</f>
+        <f>ROUND(AVERAGE(G47:AZ47),1)</f>
         <v/>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="79" t="inlineStr">
         <is>
-          <t>Michele</t>
+          <t>eltishqipe</t>
         </is>
       </c>
       <c r="B48" s="79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C48" s="68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" s="68">
-        <f>SUM(G48:AX48)</f>
+        <f>SUM(G48:AZ48)</f>
         <v/>
       </c>
       <c r="F48" s="68">
-        <f>ROUND(AVERAGE(G48:AX48),1)</f>
-        <v/>
-      </c>
-      <c r="AU48" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-      <c r="AV48" t="inlineStr">
-        <is>
-          <t>SKIP</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="79" t="inlineStr">
-        <is>
-          <t>VERRETHERULER</t>
-        </is>
-      </c>
-      <c r="B49" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="68">
-        <f>SUM(G49:AX49)</f>
-        <v/>
-      </c>
-      <c r="F49" s="68">
-        <f>ROUND(AVERAGE(G49:AX49),1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="79" t="inlineStr">
-        <is>
-          <t>GGfresco_08</t>
-        </is>
-      </c>
-      <c r="B50" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="C50" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="68">
-        <f>SUM(G50:AX50)</f>
-        <v/>
-      </c>
-      <c r="F50" s="68">
-        <f>ROUND(AVERAGE(G50:AX50),1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="79" t="inlineStr">
-        <is>
-          <t>PESCARA MANZIA</t>
-        </is>
-      </c>
-      <c r="B51" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="C51" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="68">
-        <f>SUM(G51:AX51)</f>
-        <v/>
-      </c>
-      <c r="F51" s="68">
-        <f>ROUND(AVERAGE(G51:AX51),1)</f>
+        <f>ROUND(AVERAGE(G48:AZ48),1)</f>
         <v/>
       </c>
     </row>

</xml_diff>